<commit_message>
Update non-verbs data in non_verbs.xlsx
</commit_message>
<xml_diff>
--- a/non_verbs.xlsx
+++ b/non_verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698A7F2D-7DFA-449C-977E-FFBDC29BDBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E6A5C5-1855-4BE6-A48C-E43F0E710347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="544">
   <si>
     <t>Kanji</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1512,6 +1512,171 @@
   </si>
   <si>
     <t>冷氣／空調</t>
+  </si>
+  <si>
+    <t>船</t>
+  </si>
+  <si>
+    <t>ふね</t>
+  </si>
+  <si>
+    <t>港</t>
+  </si>
+  <si>
+    <t>みなと</t>
+  </si>
+  <si>
+    <t>港口、碼頭</t>
+  </si>
+  <si>
+    <t>線路</t>
+  </si>
+  <si>
+    <t>せんろ</t>
+  </si>
+  <si>
+    <t>鐵軌、鐵路</t>
+  </si>
+  <si>
+    <t>汽車</t>
+  </si>
+  <si>
+    <t>きしゃ</t>
+  </si>
+  <si>
+    <t>蒸汽火車</t>
+  </si>
+  <si>
+    <t>列車</t>
+  </si>
+  <si>
+    <t>れっしゃ</t>
+  </si>
+  <si>
+    <t>特急</t>
+  </si>
+  <si>
+    <t>とっきゅう</t>
+  </si>
+  <si>
+    <t>特快車</t>
+  </si>
+  <si>
+    <t>乗り物</t>
+  </si>
+  <si>
+    <t>のりもの</t>
+  </si>
+  <si>
+    <t>交通工具</t>
+  </si>
+  <si>
+    <t>新幹線</t>
+  </si>
+  <si>
+    <t>しんかんせん</t>
+  </si>
+  <si>
+    <t>エスカレーター</t>
+  </si>
+  <si>
+    <t>電扶梯</t>
+  </si>
+  <si>
+    <t>オートバイ</t>
+  </si>
+  <si>
+    <t>摩托車</t>
+  </si>
+  <si>
+    <t>機械</t>
+  </si>
+  <si>
+    <t>きかい</t>
+  </si>
+  <si>
+    <t>電灯</t>
+  </si>
+  <si>
+    <t>でんとう</t>
+  </si>
+  <si>
+    <t>電燈</t>
+  </si>
+  <si>
+    <t>電球</t>
+  </si>
+  <si>
+    <t>でんきゅう</t>
+  </si>
+  <si>
+    <t>電燈泡</t>
+  </si>
+  <si>
+    <t>除湿機</t>
+  </si>
+  <si>
+    <t>じょしつき</t>
+  </si>
+  <si>
+    <t>除濕機</t>
+  </si>
+  <si>
+    <t>電子辞書</t>
+  </si>
+  <si>
+    <t>でんしじしょ</t>
+  </si>
+  <si>
+    <t>電子辭典</t>
+  </si>
+  <si>
+    <t>ベル</t>
+  </si>
+  <si>
+    <t>電鈴</t>
+  </si>
+  <si>
+    <t>ソフト</t>
+  </si>
+  <si>
+    <t>軟體</t>
+  </si>
+  <si>
+    <t>ハード</t>
+  </si>
+  <si>
+    <t>硬體</t>
+  </si>
+  <si>
+    <t>ステレオ</t>
+  </si>
+  <si>
+    <t>立體音響</t>
+  </si>
+  <si>
+    <t>プリンター</t>
+  </si>
+  <si>
+    <t>印表機</t>
+  </si>
+  <si>
+    <t>キーボード</t>
+  </si>
+  <si>
+    <t>鍵盤</t>
+  </si>
+  <si>
+    <t>コンピューター</t>
+  </si>
+  <si>
+    <t>デジタルカメラ</t>
+  </si>
+  <si>
+    <t>[5]</t>
+  </si>
+  <si>
+    <t>數位相機</t>
   </si>
 </sst>
 </file>
@@ -1920,10 +2085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F257"/>
+  <dimension ref="A1:F280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="C255" sqref="C255"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="D270" sqref="D270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4388,6 +4553,328 @@
         <v>488</v>
       </c>
     </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>489</v>
+      </c>
+      <c r="B258" t="s">
+        <v>490</v>
+      </c>
+      <c r="C258" t="s">
+        <v>419</v>
+      </c>
+      <c r="D258" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>491</v>
+      </c>
+      <c r="B259" t="s">
+        <v>492</v>
+      </c>
+      <c r="C259" t="s">
+        <v>401</v>
+      </c>
+      <c r="D259" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>494</v>
+      </c>
+      <c r="B260" t="s">
+        <v>495</v>
+      </c>
+      <c r="C260" t="s">
+        <v>419</v>
+      </c>
+      <c r="D260" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>497</v>
+      </c>
+      <c r="B261" t="s">
+        <v>498</v>
+      </c>
+      <c r="C261" t="s">
+        <v>450</v>
+      </c>
+      <c r="D261" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>500</v>
+      </c>
+      <c r="B262" t="s">
+        <v>501</v>
+      </c>
+      <c r="C262" t="s">
+        <v>433</v>
+      </c>
+      <c r="D262" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>502</v>
+      </c>
+      <c r="B263" t="s">
+        <v>503</v>
+      </c>
+      <c r="C263" t="s">
+        <v>401</v>
+      </c>
+      <c r="D263" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>505</v>
+      </c>
+      <c r="B264" t="s">
+        <v>506</v>
+      </c>
+      <c r="C264" t="s">
+        <v>401</v>
+      </c>
+      <c r="D264" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>508</v>
+      </c>
+      <c r="B265" t="s">
+        <v>509</v>
+      </c>
+      <c r="C265" t="s">
+        <v>439</v>
+      </c>
+      <c r="D265" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>510</v>
+      </c>
+      <c r="B266" t="s">
+        <v>510</v>
+      </c>
+      <c r="C266" t="s">
+        <v>454</v>
+      </c>
+      <c r="D266" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>512</v>
+      </c>
+      <c r="B267" t="s">
+        <v>512</v>
+      </c>
+      <c r="C267" t="s">
+        <v>439</v>
+      </c>
+      <c r="D267" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>514</v>
+      </c>
+      <c r="B268" t="s">
+        <v>515</v>
+      </c>
+      <c r="C268" t="s">
+        <v>430</v>
+      </c>
+      <c r="D268" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>516</v>
+      </c>
+      <c r="B269" t="s">
+        <v>517</v>
+      </c>
+      <c r="C269" t="s">
+        <v>401</v>
+      </c>
+      <c r="D269" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>519</v>
+      </c>
+      <c r="B270" t="s">
+        <v>520</v>
+      </c>
+      <c r="C270" t="s">
+        <v>401</v>
+      </c>
+      <c r="D270" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>522</v>
+      </c>
+      <c r="B271" t="s">
+        <v>523</v>
+      </c>
+      <c r="C271" t="s">
+        <v>439</v>
+      </c>
+      <c r="D271" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>525</v>
+      </c>
+      <c r="B272" t="s">
+        <v>526</v>
+      </c>
+      <c r="C272" t="s">
+        <v>454</v>
+      </c>
+      <c r="D272" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>528</v>
+      </c>
+      <c r="B273" t="s">
+        <v>528</v>
+      </c>
+      <c r="C273" t="s">
+        <v>419</v>
+      </c>
+      <c r="D273" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>530</v>
+      </c>
+      <c r="B274" t="s">
+        <v>530</v>
+      </c>
+      <c r="C274" t="s">
+        <v>419</v>
+      </c>
+      <c r="D274" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>532</v>
+      </c>
+      <c r="B275" t="s">
+        <v>532</v>
+      </c>
+      <c r="C275" t="s">
+        <v>419</v>
+      </c>
+      <c r="D275" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>534</v>
+      </c>
+      <c r="B276" t="s">
+        <v>534</v>
+      </c>
+      <c r="C276" t="s">
+        <v>401</v>
+      </c>
+      <c r="D276" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>536</v>
+      </c>
+      <c r="B277" t="s">
+        <v>536</v>
+      </c>
+      <c r="C277" t="s">
+        <v>401</v>
+      </c>
+      <c r="D277" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>538</v>
+      </c>
+      <c r="B278" t="s">
+        <v>538</v>
+      </c>
+      <c r="C278" t="s">
+        <v>439</v>
+      </c>
+      <c r="D278" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>540</v>
+      </c>
+      <c r="B279" t="s">
+        <v>540</v>
+      </c>
+      <c r="C279" t="s">
+        <v>439</v>
+      </c>
+      <c r="D279" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>541</v>
+      </c>
+      <c r="B280" t="s">
+        <v>541</v>
+      </c>
+      <c r="C280" t="s">
+        <v>542</v>
+      </c>
+      <c r="D280" t="s">
+        <v>543</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
``` No code changes made. ```
</commit_message>
<xml_diff>
--- a/non_verbs.xlsx
+++ b/non_verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E6A5C5-1855-4BE6-A48C-E43F0E710347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D5DCB3-BB0B-4D90-B754-374613D2F1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="720">
   <si>
     <t>Kanji</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -851,9 +851,6 @@
     <t>いがく</t>
   </si>
   <si>
-    <t>科学</t>
-  </si>
-  <si>
     <t>かがく</t>
   </si>
   <si>
@@ -1073,24 +1070,6 @@
     <t>ごはん</t>
   </si>
   <si>
-    <t>朝ご飯</t>
-  </si>
-  <si>
-    <t>あさごはん</t>
-  </si>
-  <si>
-    <t>昼ご飯</t>
-  </si>
-  <si>
-    <t>ひるごはん</t>
-  </si>
-  <si>
-    <t>晩ご飯</t>
-  </si>
-  <si>
-    <t>ばんごはん</t>
-  </si>
-  <si>
     <t>夕飯</t>
   </si>
   <si>
@@ -1677,6 +1656,566 @@
   </si>
   <si>
     <t>數位相機</t>
+  </si>
+  <si>
+    <t>デザート</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>搭乗券</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>とうじょうけん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>しゅくじつ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>休日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>きゅうじつ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>準備</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>じゅんび</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>席</t>
+  </si>
+  <si>
+    <t>せき</t>
+  </si>
+  <si>
+    <t>座位</t>
+  </si>
+  <si>
+    <t>壁</t>
+  </si>
+  <si>
+    <t>かべ</t>
+  </si>
+  <si>
+    <t>牆壁</t>
+  </si>
+  <si>
+    <t>屋根</t>
+  </si>
+  <si>
+    <t>やね</t>
+  </si>
+  <si>
+    <t>屋頂</t>
+  </si>
+  <si>
+    <t>屋上</t>
+  </si>
+  <si>
+    <t>おくじょう</t>
+  </si>
+  <si>
+    <t>樓頂</t>
+  </si>
+  <si>
+    <t>寺</t>
+  </si>
+  <si>
+    <t>てら</t>
+  </si>
+  <si>
+    <t>寺廟</t>
+  </si>
+  <si>
+    <t>神社</t>
+  </si>
+  <si>
+    <t>じんじゃ</t>
+  </si>
+  <si>
+    <t>教会</t>
+  </si>
+  <si>
+    <t>きょうかい</t>
+  </si>
+  <si>
+    <t>教會</t>
+  </si>
+  <si>
+    <t>講堂</t>
+  </si>
+  <si>
+    <t>こうどう</t>
+  </si>
+  <si>
+    <t>禮堂</t>
+  </si>
+  <si>
+    <t>表</t>
+  </si>
+  <si>
+    <t>おもて</t>
+  </si>
+  <si>
+    <t>表面／正面</t>
+  </si>
+  <si>
+    <t>裏</t>
+  </si>
+  <si>
+    <t>うら</t>
+  </si>
+  <si>
+    <t>裡面／反面</t>
+  </si>
+  <si>
+    <t>真ん中</t>
+  </si>
+  <si>
+    <t>まんなか</t>
+  </si>
+  <si>
+    <t>正中間</t>
+  </si>
+  <si>
+    <t>隅</t>
+  </si>
+  <si>
+    <t>すみ</t>
+  </si>
+  <si>
+    <t>角落</t>
+  </si>
+  <si>
+    <t>間</t>
+  </si>
+  <si>
+    <t>あいだ</t>
+  </si>
+  <si>
+    <t>中間／之間</t>
+  </si>
+  <si>
+    <t>途中</t>
+  </si>
+  <si>
+    <t>とちゅう</t>
+  </si>
+  <si>
+    <t>途中／中途</t>
+  </si>
+  <si>
+    <t>以上</t>
+  </si>
+  <si>
+    <t>いじょう</t>
+  </si>
+  <si>
+    <t>以下</t>
+  </si>
+  <si>
+    <t>いか</t>
+  </si>
+  <si>
+    <t>以内</t>
+  </si>
+  <si>
+    <t>いない</t>
+  </si>
+  <si>
+    <t>以內</t>
+  </si>
+  <si>
+    <t>以外</t>
+  </si>
+  <si>
+    <t>いがい</t>
+  </si>
+  <si>
+    <t>住所</t>
+  </si>
+  <si>
+    <t>じゅうしょ</t>
+  </si>
+  <si>
+    <t>住址／住處</t>
+  </si>
+  <si>
+    <t>遠く</t>
+  </si>
+  <si>
+    <t>とおく</t>
+  </si>
+  <si>
+    <t>遠處</t>
+  </si>
+  <si>
+    <t>近所</t>
+  </si>
+  <si>
+    <t>きんじょ</t>
+  </si>
+  <si>
+    <t>近處／附近</t>
+  </si>
+  <si>
+    <t>通り</t>
+  </si>
+  <si>
+    <t>とおり</t>
+  </si>
+  <si>
+    <t>大街道</t>
+  </si>
+  <si>
+    <t>坂</t>
+  </si>
+  <si>
+    <t>さか</t>
+  </si>
+  <si>
+    <t>坡道</t>
+  </si>
+  <si>
+    <t>市</t>
+  </si>
+  <si>
+    <t>し</t>
+  </si>
+  <si>
+    <t>田舎</t>
+  </si>
+  <si>
+    <t>いなか</t>
+  </si>
+  <si>
+    <t>鄉下</t>
+  </si>
+  <si>
+    <t>郊外</t>
+  </si>
+  <si>
+    <t>こうがい</t>
+  </si>
+  <si>
+    <t>郊區</t>
+  </si>
+  <si>
+    <t>国際</t>
+  </si>
+  <si>
+    <t>こくさい</t>
+  </si>
+  <si>
+    <t>國際</t>
+  </si>
+  <si>
+    <t>西洋</t>
+  </si>
+  <si>
+    <t>せいよう</t>
+  </si>
+  <si>
+    <t>世界</t>
+  </si>
+  <si>
+    <t>せかい</t>
+  </si>
+  <si>
+    <t>島</t>
+  </si>
+  <si>
+    <t>しま</t>
+  </si>
+  <si>
+    <t>島嶼</t>
+  </si>
+  <si>
+    <t>湖</t>
+  </si>
+  <si>
+    <t>みずうみ</t>
+  </si>
+  <si>
+    <t>[3][2]</t>
+  </si>
+  <si>
+    <t>海岸</t>
+  </si>
+  <si>
+    <t>かいがん</t>
+  </si>
+  <si>
+    <t>旅館</t>
+  </si>
+  <si>
+    <t>りょかん</t>
+  </si>
+  <si>
+    <t>受付</t>
+  </si>
+  <si>
+    <t>うけつけ</t>
+  </si>
+  <si>
+    <t>櫃檯</t>
+  </si>
+  <si>
+    <t>床屋</t>
+  </si>
+  <si>
+    <t>とこや</t>
+  </si>
+  <si>
+    <t>理髮店</t>
+  </si>
+  <si>
+    <t>美容院</t>
+  </si>
+  <si>
+    <t>びよういん</t>
+  </si>
+  <si>
+    <t>会場</t>
+  </si>
+  <si>
+    <t>かいじょう</t>
+  </si>
+  <si>
+    <t>會場</t>
+  </si>
+  <si>
+    <t>工場</t>
+  </si>
+  <si>
+    <t>こうじょう</t>
+  </si>
+  <si>
+    <t>工廠</t>
+  </si>
+  <si>
+    <t>売り場</t>
+  </si>
+  <si>
+    <t>うりば</t>
+  </si>
+  <si>
+    <t>賣場</t>
+  </si>
+  <si>
+    <t>事務所</t>
+  </si>
+  <si>
+    <t>じむしょ</t>
+  </si>
+  <si>
+    <t>会議室</t>
+  </si>
+  <si>
+    <t>かいぎしつ</t>
+  </si>
+  <si>
+    <t>會議室</t>
+  </si>
+  <si>
+    <t>展覧会</t>
+  </si>
+  <si>
+    <t>てんらんかい</t>
+  </si>
+  <si>
+    <t>展覽會</t>
+  </si>
+  <si>
+    <t>動物園</t>
+  </si>
+  <si>
+    <t>どうぶつえん</t>
+  </si>
+  <si>
+    <t>美術館</t>
+  </si>
+  <si>
+    <t>びじゅつかん</t>
+  </si>
+  <si>
+    <t>新聞社</t>
+  </si>
+  <si>
+    <t>しんぶんしゃ</t>
+  </si>
+  <si>
+    <t>報社</t>
+  </si>
+  <si>
+    <t>研究室</t>
+  </si>
+  <si>
+    <t>けんきゅうしつ</t>
+  </si>
+  <si>
+    <t>駐車場</t>
+  </si>
+  <si>
+    <t>ちゅうしゃじょう</t>
+  </si>
+  <si>
+    <t>停車場</t>
+  </si>
+  <si>
+    <t>ビル</t>
+  </si>
+  <si>
+    <t>大樓</t>
+  </si>
+  <si>
+    <t>アジア</t>
+  </si>
+  <si>
+    <t>亞洲</t>
+  </si>
+  <si>
+    <t>アフリカ</t>
+  </si>
+  <si>
+    <t>非洲</t>
+  </si>
+  <si>
+    <t>アメリカ</t>
+  </si>
+  <si>
+    <t>美國</t>
+  </si>
+  <si>
+    <t>テニスコート</t>
+  </si>
+  <si>
+    <t>網球場</t>
+  </si>
+  <si>
+    <t>ガソリンスタンド</t>
+  </si>
+  <si>
+    <t>[6]</t>
+  </si>
+  <si>
+    <t>加油站</t>
+  </si>
+  <si>
+    <t>スーパーマーケット</t>
+  </si>
+  <si>
+    <t>超市</t>
+  </si>
+  <si>
+    <t>米</t>
+  </si>
+  <si>
+    <t>こめ</t>
+  </si>
+  <si>
+    <t>豚カツ</t>
+  </si>
+  <si>
+    <t>とんかつ</t>
+  </si>
+  <si>
+    <t>炸豬排</t>
+  </si>
+  <si>
+    <t>カツ丼</t>
+  </si>
+  <si>
+    <t>かつどん</t>
+  </si>
+  <si>
+    <t>豬排蓋飯</t>
+  </si>
+  <si>
+    <t>食料品</t>
+  </si>
+  <si>
+    <t>しょくりょうひん</t>
+  </si>
+  <si>
+    <t>食品</t>
+  </si>
+  <si>
+    <t>味噌</t>
+  </si>
+  <si>
+    <t>みそ</t>
+  </si>
+  <si>
+    <t>味噌、豆醬</t>
+  </si>
+  <si>
+    <t>葡萄</t>
+  </si>
+  <si>
+    <t>ケーキ</t>
+  </si>
+  <si>
+    <t>蛋糕</t>
+  </si>
+  <si>
+    <t>サラダ</t>
+  </si>
+  <si>
+    <t>沙拉</t>
+  </si>
+  <si>
+    <t>ジャム</t>
+  </si>
+  <si>
+    <t>果醬</t>
+  </si>
+  <si>
+    <t>ビーフ</t>
+  </si>
+  <si>
+    <t>ステーキ</t>
+  </si>
+  <si>
+    <t>牛排</t>
+  </si>
+  <si>
+    <t>ハンバーグ</t>
+  </si>
+  <si>
+    <t>漢堡肉</t>
+  </si>
+  <si>
+    <t>ハンバーガー</t>
+  </si>
+  <si>
+    <t>漢堡</t>
+  </si>
+  <si>
+    <t>ポークステーキ</t>
+  </si>
+  <si>
+    <t>豬排</t>
+  </si>
+  <si>
+    <t>ミルク</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>科学／化学</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2085,10 +2624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F280"/>
+  <dimension ref="A1:F351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
-      <selection activeCell="D270" sqref="D270"/>
+    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="B340" sqref="B340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3533,178 +4072,178 @@
     </row>
     <row r="155" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
+        <v>719</v>
+      </c>
+      <c r="B155" t="s">
         <v>270</v>
-      </c>
-      <c r="B155" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B156" t="s">
         <v>272</v>
-      </c>
-      <c r="B156" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B157" t="s">
         <v>274</v>
-      </c>
-      <c r="B157" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B158" t="s">
         <v>276</v>
-      </c>
-      <c r="B158" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B159" t="s">
         <v>278</v>
-      </c>
-      <c r="B159" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B160" t="s">
         <v>280</v>
-      </c>
-      <c r="B160" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B161" t="s">
         <v>282</v>
-      </c>
-      <c r="B161" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B162" t="s">
         <v>284</v>
-      </c>
-      <c r="B162" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B163" t="s">
         <v>286</v>
-      </c>
-      <c r="B163" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B164" t="s">
         <v>288</v>
-      </c>
-      <c r="B164" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A165" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B165" t="s">
         <v>290</v>
-      </c>
-      <c r="B165" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A166" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B166" t="s">
         <v>292</v>
-      </c>
-      <c r="B166" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A167" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B167" t="s">
         <v>294</v>
-      </c>
-      <c r="B167" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A168" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B168" t="s">
         <v>296</v>
-      </c>
-      <c r="B168" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A169" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B169" t="s">
         <v>298</v>
-      </c>
-      <c r="B169" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>299</v>
+      </c>
+      <c r="B170" t="s">
         <v>300</v>
-      </c>
-      <c r="B170" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>301</v>
+      </c>
+      <c r="B171" t="s">
         <v>302</v>
-      </c>
-      <c r="B171" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>303</v>
+      </c>
+      <c r="B172" t="s">
         <v>304</v>
-      </c>
-      <c r="B172" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>305</v>
+      </c>
+      <c r="B173" t="s">
         <v>306</v>
-      </c>
-      <c r="B173" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>307</v>
+      </c>
+      <c r="B174" t="s">
         <v>308</v>
-      </c>
-      <c r="B174" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>309</v>
+      </c>
+      <c r="B175" t="s">
         <v>310</v>
-      </c>
-      <c r="B175" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>311</v>
+      </c>
+      <c r="B176" t="s">
         <v>312</v>
-      </c>
-      <c r="B176" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3712,464 +4251,482 @@
         <v>219</v>
       </c>
       <c r="B177" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>314</v>
+      </c>
+      <c r="B178" t="s">
         <v>315</v>
-      </c>
-      <c r="B178" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>316</v>
+      </c>
+      <c r="B179" t="s">
         <v>317</v>
-      </c>
-      <c r="B179" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>318</v>
+      </c>
+      <c r="B180" t="s">
         <v>319</v>
-      </c>
-      <c r="B180" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>320</v>
+      </c>
+      <c r="B181" t="s">
         <v>321</v>
-      </c>
-      <c r="B181" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>322</v>
+      </c>
+      <c r="B182" t="s">
         <v>323</v>
-      </c>
-      <c r="B182" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>324</v>
+      </c>
+      <c r="B183" t="s">
         <v>325</v>
-      </c>
-      <c r="B183" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B184" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B185" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B186" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B187" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B188" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A189" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B189" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A190" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B190" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A191" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B191" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>337</v>
+      </c>
+      <c r="B192" t="s">
         <v>338</v>
-      </c>
-      <c r="B192" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>339</v>
+      </c>
+      <c r="B193" t="s">
         <v>340</v>
-      </c>
-      <c r="B193" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>341</v>
+      </c>
+      <c r="B194" t="s">
         <v>342</v>
-      </c>
-      <c r="B194" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>343</v>
+      </c>
+      <c r="B195" t="s">
         <v>344</v>
-      </c>
-      <c r="B195" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>345</v>
+      </c>
+      <c r="B196" t="s">
         <v>346</v>
-      </c>
-      <c r="B196" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>347</v>
+      </c>
+      <c r="B197" t="s">
         <v>348</v>
-      </c>
-      <c r="B197" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>349</v>
+      </c>
+      <c r="B198" t="s">
         <v>350</v>
-      </c>
-      <c r="B198" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B199" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B200" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B201" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B202" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>358</v>
+      </c>
+      <c r="B203" t="s">
         <v>359</v>
-      </c>
-      <c r="B203" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
+        <v>360</v>
+      </c>
+      <c r="B204" t="s">
         <v>361</v>
-      </c>
-      <c r="B204" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>362</v>
+      </c>
+      <c r="B205" t="s">
         <v>363</v>
-      </c>
-      <c r="B205" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>364</v>
+      </c>
+      <c r="B206" t="s">
         <v>365</v>
-      </c>
-      <c r="B206" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
+        <v>366</v>
+      </c>
+      <c r="B207" t="s">
         <v>367</v>
-      </c>
-      <c r="B207" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>368</v>
+      </c>
+      <c r="B208" t="s">
         <v>369</v>
       </c>
-      <c r="B208" t="s">
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+      <c r="B209" t="s">
         <v>371</v>
       </c>
-      <c r="B209" t="s">
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+      <c r="B210" t="s">
         <v>373</v>
       </c>
-      <c r="B210" t="s">
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+      <c r="B211" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>375</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B212" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>377</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B213" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
         <v>379</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B214" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>381</v>
       </c>
-      <c r="B214" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+      <c r="B215" t="s">
         <v>382</v>
       </c>
-      <c r="B215" t="s">
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="B216" t="s">
         <v>384</v>
       </c>
-      <c r="B216" t="s">
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="B217" t="s">
         <v>386</v>
       </c>
-      <c r="B217" t="s">
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+      <c r="B218" t="s">
         <v>388</v>
       </c>
-      <c r="B218" t="s">
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+      <c r="B219" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>390</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B220" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+      <c r="B221" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>392</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B222" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+      <c r="C222" t="s">
         <v>394</v>
       </c>
-      <c r="B221" t="s">
+      <c r="D222" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>396</v>
-      </c>
-      <c r="B222" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>397</v>
       </c>
       <c r="B223" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C223" t="s">
+        <v>398</v>
+      </c>
+      <c r="D223" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B224" t="s">
-        <v>398</v>
+        <v>401</v>
+      </c>
+      <c r="C224" t="s">
+        <v>394</v>
+      </c>
+      <c r="D224" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B225" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C225" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="D225" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B226" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C226" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="D226" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B227" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C227" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="D227" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B228" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C228" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="D228" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
+        <v>414</v>
+      </c>
+      <c r="B229" t="s">
+        <v>414</v>
+      </c>
+      <c r="C229" t="s">
         <v>412</v>
       </c>
-      <c r="B229" t="s">
-        <v>413</v>
-      </c>
-      <c r="C229" t="s">
-        <v>401</v>
-      </c>
       <c r="D229" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B230" t="s">
         <v>416</v>
       </c>
       <c r="C230" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="D230" t="s">
         <v>417</v>
@@ -4183,35 +4740,35 @@
         <v>418</v>
       </c>
       <c r="C231" t="s">
+        <v>394</v>
+      </c>
+      <c r="D231" t="s">
         <v>419</v>
-      </c>
-      <c r="D231" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
+        <v>420</v>
+      </c>
+      <c r="B232" t="s">
+        <v>420</v>
+      </c>
+      <c r="C232" t="s">
+        <v>412</v>
+      </c>
+      <c r="D232" t="s">
         <v>421</v>
-      </c>
-      <c r="B232" t="s">
-        <v>421</v>
-      </c>
-      <c r="C232" t="s">
-        <v>419</v>
-      </c>
-      <c r="D232" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
+        <v>422</v>
+      </c>
+      <c r="B233" t="s">
+        <v>422</v>
+      </c>
+      <c r="C233" t="s">
         <v>423</v>
-      </c>
-      <c r="B233" t="s">
-        <v>423</v>
-      </c>
-      <c r="C233" t="s">
-        <v>401</v>
       </c>
       <c r="D233" t="s">
         <v>424</v>
@@ -4225,231 +4782,231 @@
         <v>425</v>
       </c>
       <c r="C234" t="s">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="D234" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B235" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C235" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D235" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B236" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C236" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D236" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B237" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C237" t="s">
-        <v>433</v>
+        <v>398</v>
       </c>
       <c r="D237" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B238" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C238" t="s">
-        <v>430</v>
+        <v>398</v>
       </c>
       <c r="D238" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B239" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C239" t="s">
-        <v>439</v>
+        <v>398</v>
       </c>
       <c r="D239" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B240" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C240" t="s">
-        <v>405</v>
+        <v>443</v>
       </c>
       <c r="D240" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B241" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C241" t="s">
-        <v>405</v>
+        <v>447</v>
       </c>
       <c r="D241" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B242" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="C242" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="D242" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="B243" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="C243" t="s">
-        <v>450</v>
+        <v>394</v>
       </c>
       <c r="D243" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B244" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C244" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="D244" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B245" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C245" t="s">
-        <v>419</v>
+        <v>432</v>
       </c>
       <c r="D245" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B246" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C246" t="s">
-        <v>401</v>
+        <v>462</v>
       </c>
       <c r="D246" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B247" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C247" t="s">
-        <v>439</v>
+        <v>394</v>
       </c>
       <c r="D247" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="B248" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="C248" t="s">
-        <v>439</v>
+        <v>394</v>
       </c>
       <c r="D248" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B249" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C249" t="s">
-        <v>469</v>
+        <v>412</v>
       </c>
       <c r="D249" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B250" t="s">
         <v>472</v>
       </c>
       <c r="C250" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="D250" t="s">
         <v>473</v>
@@ -4460,80 +5017,80 @@
         <v>474</v>
       </c>
       <c r="B251" t="s">
+        <v>474</v>
+      </c>
+      <c r="C251" t="s">
+        <v>412</v>
+      </c>
+      <c r="D251" t="s">
         <v>475</v>
-      </c>
-      <c r="C251" t="s">
-        <v>401</v>
-      </c>
-      <c r="D251" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
+        <v>476</v>
+      </c>
+      <c r="B252" t="s">
+        <v>476</v>
+      </c>
+      <c r="C252" t="s">
+        <v>412</v>
+      </c>
+      <c r="D252" t="s">
         <v>477</v>
-      </c>
-      <c r="B252" t="s">
-        <v>477</v>
-      </c>
-      <c r="C252" t="s">
-        <v>419</v>
-      </c>
-      <c r="D252" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>478</v>
+      </c>
+      <c r="B253" t="s">
+        <v>478</v>
+      </c>
+      <c r="C253" t="s">
+        <v>394</v>
+      </c>
+      <c r="D253" t="s">
         <v>479</v>
-      </c>
-      <c r="B253" t="s">
-        <v>479</v>
-      </c>
-      <c r="C253" t="s">
-        <v>419</v>
-      </c>
-      <c r="D253" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
+        <v>480</v>
+      </c>
+      <c r="B254" t="s">
+        <v>480</v>
+      </c>
+      <c r="C254" t="s">
+        <v>394</v>
+      </c>
+      <c r="D254" t="s">
         <v>481</v>
-      </c>
-      <c r="B254" t="s">
-        <v>481</v>
-      </c>
-      <c r="C254" t="s">
-        <v>419</v>
-      </c>
-      <c r="D254" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B255" t="s">
         <v>483</v>
       </c>
       <c r="C255" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D255" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B256" t="s">
         <v>485</v>
       </c>
       <c r="C256" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="D256" t="s">
         <v>486</v>
@@ -4544,38 +5101,38 @@
         <v>487</v>
       </c>
       <c r="B257" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C257" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="D257" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B258" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C258" t="s">
-        <v>419</v>
+        <v>443</v>
       </c>
       <c r="D258" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B259" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C259" t="s">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="D259" t="s">
         <v>493</v>
@@ -4583,55 +5140,55 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B260" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C260" t="s">
-        <v>419</v>
+        <v>394</v>
       </c>
       <c r="D260" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B261" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C261" t="s">
-        <v>450</v>
+        <v>394</v>
       </c>
       <c r="D261" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B262" t="s">
+        <v>502</v>
+      </c>
+      <c r="C262" t="s">
+        <v>432</v>
+      </c>
+      <c r="D262" t="s">
         <v>501</v>
-      </c>
-      <c r="C262" t="s">
-        <v>433</v>
-      </c>
-      <c r="D262" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B263" t="s">
         <v>503</v>
       </c>
       <c r="C263" t="s">
-        <v>401</v>
+        <v>447</v>
       </c>
       <c r="D263" t="s">
         <v>504</v>
@@ -4642,38 +5199,38 @@
         <v>505</v>
       </c>
       <c r="B264" t="s">
+        <v>505</v>
+      </c>
+      <c r="C264" t="s">
+        <v>432</v>
+      </c>
+      <c r="D264" t="s">
         <v>506</v>
-      </c>
-      <c r="C264" t="s">
-        <v>401</v>
-      </c>
-      <c r="D264" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
+        <v>507</v>
+      </c>
+      <c r="B265" t="s">
         <v>508</v>
       </c>
-      <c r="B265" t="s">
-        <v>509</v>
-      </c>
       <c r="C265" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="D265" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B266" t="s">
         <v>510</v>
       </c>
       <c r="C266" t="s">
-        <v>454</v>
+        <v>394</v>
       </c>
       <c r="D266" t="s">
         <v>511</v>
@@ -4684,66 +5241,66 @@
         <v>512</v>
       </c>
       <c r="B267" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C267" t="s">
-        <v>439</v>
+        <v>394</v>
       </c>
       <c r="D267" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B268" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C268" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D268" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B269" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C269" t="s">
-        <v>401</v>
+        <v>447</v>
       </c>
       <c r="D269" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B270" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C270" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="D270" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B271" t="s">
         <v>523</v>
       </c>
       <c r="C271" t="s">
-        <v>439</v>
+        <v>412</v>
       </c>
       <c r="D271" t="s">
         <v>524</v>
@@ -4754,125 +5311,1083 @@
         <v>525</v>
       </c>
       <c r="B272" t="s">
+        <v>525</v>
+      </c>
+      <c r="C272" t="s">
+        <v>412</v>
+      </c>
+      <c r="D272" t="s">
         <v>526</v>
-      </c>
-      <c r="C272" t="s">
-        <v>454</v>
-      </c>
-      <c r="D272" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>527</v>
+      </c>
+      <c r="B273" t="s">
+        <v>527</v>
+      </c>
+      <c r="C273" t="s">
+        <v>394</v>
+      </c>
+      <c r="D273" t="s">
         <v>528</v>
-      </c>
-      <c r="B273" t="s">
-        <v>528</v>
-      </c>
-      <c r="C273" t="s">
-        <v>419</v>
-      </c>
-      <c r="D273" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
+        <v>529</v>
+      </c>
+      <c r="B274" t="s">
+        <v>529</v>
+      </c>
+      <c r="C274" t="s">
+        <v>394</v>
+      </c>
+      <c r="D274" t="s">
         <v>530</v>
-      </c>
-      <c r="B274" t="s">
-        <v>530</v>
-      </c>
-      <c r="C274" t="s">
-        <v>419</v>
-      </c>
-      <c r="D274" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
+        <v>531</v>
+      </c>
+      <c r="B275" t="s">
+        <v>531</v>
+      </c>
+      <c r="C275" t="s">
+        <v>432</v>
+      </c>
+      <c r="D275" t="s">
         <v>532</v>
-      </c>
-      <c r="B275" t="s">
-        <v>532</v>
-      </c>
-      <c r="C275" t="s">
-        <v>419</v>
-      </c>
-      <c r="D275" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B276" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C276" t="s">
-        <v>401</v>
+        <v>432</v>
       </c>
       <c r="D276" t="s">
-        <v>535</v>
+        <v>479</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
+        <v>534</v>
+      </c>
+      <c r="B277" t="s">
+        <v>534</v>
+      </c>
+      <c r="C277" t="s">
+        <v>535</v>
+      </c>
+      <c r="D277" t="s">
         <v>536</v>
-      </c>
-      <c r="B277" t="s">
-        <v>536</v>
-      </c>
-      <c r="C277" t="s">
-        <v>401</v>
-      </c>
-      <c r="D277" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
+        <v>537</v>
+      </c>
+      <c r="B278" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A279" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="B278" t="s">
-        <v>538</v>
-      </c>
-      <c r="C278" t="s">
-        <v>439</v>
-      </c>
-      <c r="D278" t="s">
+      <c r="B279" s="3" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
+    <row r="280" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A280" t="s">
         <v>540</v>
       </c>
-      <c r="B279" t="s">
-        <v>540</v>
-      </c>
-      <c r="C279" t="s">
-        <v>439</v>
-      </c>
-      <c r="D279" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
+      <c r="B280" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="B280" t="s">
-        <v>541</v>
-      </c>
-      <c r="C280" t="s">
+    </row>
+    <row r="281" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A281" t="s">
         <v>542</v>
       </c>
-      <c r="D280" t="s">
+      <c r="B281" s="3" t="s">
         <v>543</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A282" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>546</v>
+      </c>
+      <c r="B283" t="s">
+        <v>547</v>
+      </c>
+      <c r="C283" t="s">
+        <v>412</v>
+      </c>
+      <c r="D283" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>549</v>
+      </c>
+      <c r="B284" t="s">
+        <v>550</v>
+      </c>
+      <c r="C284" t="s">
+        <v>394</v>
+      </c>
+      <c r="D284" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>552</v>
+      </c>
+      <c r="B285" t="s">
+        <v>553</v>
+      </c>
+      <c r="C285" t="s">
+        <v>412</v>
+      </c>
+      <c r="D285" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>555</v>
+      </c>
+      <c r="B286" t="s">
+        <v>556</v>
+      </c>
+      <c r="C286" t="s">
+        <v>394</v>
+      </c>
+      <c r="D286" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>558</v>
+      </c>
+      <c r="B287" t="s">
+        <v>559</v>
+      </c>
+      <c r="C287" t="s">
+        <v>398</v>
+      </c>
+      <c r="D287" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>561</v>
+      </c>
+      <c r="B288" t="s">
+        <v>562</v>
+      </c>
+      <c r="C288" t="s">
+        <v>412</v>
+      </c>
+      <c r="D288" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>563</v>
+      </c>
+      <c r="B289" t="s">
+        <v>564</v>
+      </c>
+      <c r="C289" t="s">
+        <v>394</v>
+      </c>
+      <c r="D289" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>566</v>
+      </c>
+      <c r="B290" t="s">
+        <v>567</v>
+      </c>
+      <c r="C290" t="s">
+        <v>394</v>
+      </c>
+      <c r="D290" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>569</v>
+      </c>
+      <c r="B291" t="s">
+        <v>570</v>
+      </c>
+      <c r="C291" t="s">
+        <v>432</v>
+      </c>
+      <c r="D291" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>572</v>
+      </c>
+      <c r="B292" t="s">
+        <v>573</v>
+      </c>
+      <c r="C292" t="s">
+        <v>398</v>
+      </c>
+      <c r="D292" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>575</v>
+      </c>
+      <c r="B293" t="s">
+        <v>576</v>
+      </c>
+      <c r="C293" t="s">
+        <v>394</v>
+      </c>
+      <c r="D293" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>578</v>
+      </c>
+      <c r="B294" t="s">
+        <v>579</v>
+      </c>
+      <c r="C294" t="s">
+        <v>412</v>
+      </c>
+      <c r="D294" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>581</v>
+      </c>
+      <c r="B295" t="s">
+        <v>582</v>
+      </c>
+      <c r="C295" t="s">
+        <v>394</v>
+      </c>
+      <c r="D295" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>584</v>
+      </c>
+      <c r="B296" t="s">
+        <v>585</v>
+      </c>
+      <c r="C296" t="s">
+        <v>394</v>
+      </c>
+      <c r="D296" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>587</v>
+      </c>
+      <c r="B297" t="s">
+        <v>588</v>
+      </c>
+      <c r="C297" t="s">
+        <v>412</v>
+      </c>
+      <c r="D297" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>589</v>
+      </c>
+      <c r="B298" t="s">
+        <v>590</v>
+      </c>
+      <c r="C298" t="s">
+        <v>412</v>
+      </c>
+      <c r="D298" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>591</v>
+      </c>
+      <c r="B299" t="s">
+        <v>592</v>
+      </c>
+      <c r="C299" t="s">
+        <v>412</v>
+      </c>
+      <c r="D299" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>594</v>
+      </c>
+      <c r="B300" t="s">
+        <v>595</v>
+      </c>
+      <c r="C300" t="s">
+        <v>412</v>
+      </c>
+      <c r="D300" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>596</v>
+      </c>
+      <c r="B301" t="s">
+        <v>597</v>
+      </c>
+      <c r="C301" t="s">
+        <v>412</v>
+      </c>
+      <c r="D301" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>599</v>
+      </c>
+      <c r="B302" t="s">
+        <v>600</v>
+      </c>
+      <c r="C302" t="s">
+        <v>432</v>
+      </c>
+      <c r="D302" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>602</v>
+      </c>
+      <c r="B303" t="s">
+        <v>603</v>
+      </c>
+      <c r="C303" t="s">
+        <v>412</v>
+      </c>
+      <c r="D303" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>605</v>
+      </c>
+      <c r="B304" t="s">
+        <v>606</v>
+      </c>
+      <c r="C304" t="s">
+        <v>432</v>
+      </c>
+      <c r="D304" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>608</v>
+      </c>
+      <c r="B305" t="s">
+        <v>609</v>
+      </c>
+      <c r="C305" t="s">
+        <v>398</v>
+      </c>
+      <c r="D305" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>611</v>
+      </c>
+      <c r="B306" t="s">
+        <v>612</v>
+      </c>
+      <c r="C306" t="s">
+        <v>412</v>
+      </c>
+      <c r="D306" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>613</v>
+      </c>
+      <c r="B307" t="s">
+        <v>614</v>
+      </c>
+      <c r="C307" t="s">
+        <v>394</v>
+      </c>
+      <c r="D307" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>616</v>
+      </c>
+      <c r="B308" t="s">
+        <v>617</v>
+      </c>
+      <c r="C308" t="s">
+        <v>412</v>
+      </c>
+      <c r="D308" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>619</v>
+      </c>
+      <c r="B309" t="s">
+        <v>620</v>
+      </c>
+      <c r="C309" t="s">
+        <v>394</v>
+      </c>
+      <c r="D309" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>622</v>
+      </c>
+      <c r="B310" t="s">
+        <v>623</v>
+      </c>
+      <c r="C310" t="s">
+        <v>412</v>
+      </c>
+      <c r="D310" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>624</v>
+      </c>
+      <c r="B311" t="s">
+        <v>625</v>
+      </c>
+      <c r="C311" t="s">
+        <v>412</v>
+      </c>
+      <c r="D311" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>626</v>
+      </c>
+      <c r="B312" t="s">
+        <v>627</v>
+      </c>
+      <c r="C312" t="s">
+        <v>398</v>
+      </c>
+      <c r="D312" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>629</v>
+      </c>
+      <c r="B313" t="s">
+        <v>630</v>
+      </c>
+      <c r="C313" t="s">
+        <v>631</v>
+      </c>
+      <c r="D313" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>632</v>
+      </c>
+      <c r="B314" t="s">
+        <v>633</v>
+      </c>
+      <c r="C314" t="s">
+        <v>394</v>
+      </c>
+      <c r="D314" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>634</v>
+      </c>
+      <c r="B315" t="s">
+        <v>635</v>
+      </c>
+      <c r="C315" t="s">
+        <v>394</v>
+      </c>
+      <c r="D315" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>636</v>
+      </c>
+      <c r="B316" t="s">
+        <v>637</v>
+      </c>
+      <c r="C316" t="s">
+        <v>394</v>
+      </c>
+      <c r="D316" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>639</v>
+      </c>
+      <c r="B317" t="s">
+        <v>640</v>
+      </c>
+      <c r="C317" t="s">
+        <v>394</v>
+      </c>
+      <c r="D317" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>642</v>
+      </c>
+      <c r="B318" t="s">
+        <v>643</v>
+      </c>
+      <c r="C318" t="s">
+        <v>398</v>
+      </c>
+      <c r="D318" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>644</v>
+      </c>
+      <c r="B319" t="s">
+        <v>645</v>
+      </c>
+      <c r="C319" t="s">
+        <v>394</v>
+      </c>
+      <c r="D319" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>647</v>
+      </c>
+      <c r="B320" t="s">
+        <v>648</v>
+      </c>
+      <c r="C320" t="s">
+        <v>432</v>
+      </c>
+      <c r="D320" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>650</v>
+      </c>
+      <c r="B321" t="s">
+        <v>651</v>
+      </c>
+      <c r="C321" t="s">
+        <v>394</v>
+      </c>
+      <c r="D321" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>653</v>
+      </c>
+      <c r="B322" t="s">
+        <v>654</v>
+      </c>
+      <c r="C322" t="s">
+        <v>398</v>
+      </c>
+      <c r="D322" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>655</v>
+      </c>
+      <c r="B323" t="s">
+        <v>656</v>
+      </c>
+      <c r="C323" t="s">
+        <v>432</v>
+      </c>
+      <c r="D323" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>658</v>
+      </c>
+      <c r="B324" t="s">
+        <v>659</v>
+      </c>
+      <c r="C324" t="s">
+        <v>432</v>
+      </c>
+      <c r="D324" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>661</v>
+      </c>
+      <c r="B325" t="s">
+        <v>662</v>
+      </c>
+      <c r="C325" t="s">
+        <v>447</v>
+      </c>
+      <c r="D325" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>663</v>
+      </c>
+      <c r="B326" t="s">
+        <v>664</v>
+      </c>
+      <c r="C326" t="s">
+        <v>631</v>
+      </c>
+      <c r="D326" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>665</v>
+      </c>
+      <c r="B327" t="s">
+        <v>666</v>
+      </c>
+      <c r="C327" t="s">
+        <v>432</v>
+      </c>
+      <c r="D327" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>668</v>
+      </c>
+      <c r="B328" t="s">
+        <v>669</v>
+      </c>
+      <c r="C328" t="s">
+        <v>432</v>
+      </c>
+      <c r="D328" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>670</v>
+      </c>
+      <c r="B329" t="s">
+        <v>671</v>
+      </c>
+      <c r="C329" t="s">
+        <v>394</v>
+      </c>
+      <c r="D329" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>673</v>
+      </c>
+      <c r="B330" t="s">
+        <v>673</v>
+      </c>
+      <c r="C330" t="s">
+        <v>412</v>
+      </c>
+      <c r="D330" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>675</v>
+      </c>
+      <c r="B331" t="s">
+        <v>675</v>
+      </c>
+      <c r="C331" t="s">
+        <v>412</v>
+      </c>
+      <c r="D331" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>677</v>
+      </c>
+      <c r="B332" t="s">
+        <v>677</v>
+      </c>
+      <c r="C332" t="s">
+        <v>394</v>
+      </c>
+      <c r="D332" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>679</v>
+      </c>
+      <c r="B333" t="s">
+        <v>679</v>
+      </c>
+      <c r="C333" t="s">
+        <v>394</v>
+      </c>
+      <c r="D333" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>681</v>
+      </c>
+      <c r="B334" t="s">
+        <v>681</v>
+      </c>
+      <c r="C334" t="s">
+        <v>447</v>
+      </c>
+      <c r="D334" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>683</v>
+      </c>
+      <c r="B335" t="s">
+        <v>683</v>
+      </c>
+      <c r="C335" t="s">
+        <v>684</v>
+      </c>
+      <c r="D335" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>686</v>
+      </c>
+      <c r="B336" t="s">
+        <v>686</v>
+      </c>
+      <c r="C336" t="s">
+        <v>535</v>
+      </c>
+      <c r="D336" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>688</v>
+      </c>
+      <c r="B337" t="s">
+        <v>689</v>
+      </c>
+      <c r="C337" t="s">
+        <v>398</v>
+      </c>
+      <c r="D337" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>690</v>
+      </c>
+      <c r="B338" t="s">
+        <v>691</v>
+      </c>
+      <c r="C338" t="s">
+        <v>394</v>
+      </c>
+      <c r="D338" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>693</v>
+      </c>
+      <c r="B339" t="s">
+        <v>694</v>
+      </c>
+      <c r="C339" t="s">
+        <v>394</v>
+      </c>
+      <c r="D339" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>696</v>
+      </c>
+      <c r="B340" t="s">
+        <v>697</v>
+      </c>
+      <c r="C340" t="s">
+        <v>394</v>
+      </c>
+      <c r="D340" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>699</v>
+      </c>
+      <c r="B341" t="s">
+        <v>700</v>
+      </c>
+      <c r="C341" t="s">
+        <v>412</v>
+      </c>
+      <c r="D341" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>702</v>
+      </c>
+      <c r="B342" t="s">
+        <v>319</v>
+      </c>
+      <c r="C342" t="s">
+        <v>394</v>
+      </c>
+      <c r="D342" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>703</v>
+      </c>
+      <c r="B343" t="s">
+        <v>703</v>
+      </c>
+      <c r="C343" t="s">
+        <v>412</v>
+      </c>
+      <c r="D343" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>705</v>
+      </c>
+      <c r="B344" t="s">
+        <v>705</v>
+      </c>
+      <c r="C344" t="s">
+        <v>412</v>
+      </c>
+      <c r="D344" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>707</v>
+      </c>
+      <c r="B345" t="s">
+        <v>707</v>
+      </c>
+      <c r="C345" t="s">
+        <v>412</v>
+      </c>
+      <c r="D345" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>709</v>
+      </c>
+      <c r="B346" t="s">
+        <v>709</v>
+      </c>
+      <c r="C346" t="s">
+        <v>412</v>
+      </c>
+      <c r="D346" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>710</v>
+      </c>
+      <c r="B347" t="s">
+        <v>710</v>
+      </c>
+      <c r="C347" t="s">
+        <v>398</v>
+      </c>
+      <c r="D347" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>712</v>
+      </c>
+      <c r="B348" t="s">
+        <v>712</v>
+      </c>
+      <c r="C348" t="s">
+        <v>432</v>
+      </c>
+      <c r="D348" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>714</v>
+      </c>
+      <c r="B349" t="s">
+        <v>714</v>
+      </c>
+      <c r="C349" t="s">
+        <v>432</v>
+      </c>
+      <c r="D349" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>716</v>
+      </c>
+      <c r="B350" t="s">
+        <v>716</v>
+      </c>
+      <c r="C350" t="s">
+        <v>535</v>
+      </c>
+      <c r="D350" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A351" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="B351" s="3" t="s">
+        <v>718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add ba form support
</commit_message>
<xml_diff>
--- a/non_verbs.xlsx
+++ b/non_verbs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mptang\Desktop\local testing\online-web-app-deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B491F6ED-AAB2-4C59-9ADF-881C1E3855C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA46A4B-0FF7-412B-B1BA-63E75FB5D17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
+    <workbookView xWindow="32565" yWindow="4020" windowWidth="21600" windowHeight="11295" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2576,11 +2576,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2589,14 +2589,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2666,7 +2666,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2682,9 +2682,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2722,7 +2722,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2828,7 +2828,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2970,7 +2970,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2980,11 +2980,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
   <dimension ref="A1:F395"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
-      <selection activeCell="D403" sqref="D403"/>
+    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
+      <selection activeCell="D335" sqref="D335"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
@@ -2994,7 +2994,7 @@
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3006,7 +3006,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3018,7 +3018,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="18.75">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -3030,7 +3030,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18.75">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -3042,7 +3042,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="18.75">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -3054,7 +3054,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="18.75">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="18.75">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="18.75">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -3090,7 +3090,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="18.75">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -3102,7 +3102,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="18.75">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="18.75">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="18.75">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="18.75">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="18.75">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="18.75">
       <c r="A15" s="5" t="s">
         <v>40</v>
       </c>
@@ -3156,7 +3156,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="18.75">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="18.75">
       <c r="A17" s="5" t="s">
         <v>44</v>
       </c>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="18.75">
       <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="18.75">
       <c r="A19" s="5" t="s">
         <v>48</v>
       </c>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18.75">
       <c r="A20" s="5" t="s">
         <v>50</v>
       </c>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="18.75">
       <c r="A21" s="5" t="s">
         <v>52</v>
       </c>
@@ -3210,7 +3210,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="18.75">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="18.75">
       <c r="A23" s="5" t="s">
         <v>56</v>
       </c>
@@ -3228,7 +3228,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="18.75">
       <c r="A24" s="5" t="s">
         <v>58</v>
       </c>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="18.75">
       <c r="A25" s="5" t="s">
         <v>60</v>
       </c>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="18.75">
       <c r="A26" s="5" t="s">
         <v>62</v>
       </c>
@@ -3255,7 +3255,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="18.75">
       <c r="A27" s="5" t="s">
         <v>63</v>
       </c>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="18.75">
       <c r="A28" s="5" t="s">
         <v>64</v>
       </c>
@@ -3273,7 +3273,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="18.75">
       <c r="A29" s="5" t="s">
         <v>66</v>
       </c>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="18.75">
       <c r="A30" s="5" t="s">
         <v>68</v>
       </c>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="18.75">
       <c r="A31" s="5" t="s">
         <v>70</v>
       </c>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="18.75">
       <c r="A32" s="5" t="s">
         <v>72</v>
       </c>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="18.75">
       <c r="A33" s="5" t="s">
         <v>74</v>
       </c>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="18.75">
       <c r="A34" s="5" t="s">
         <v>76</v>
       </c>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18.75">
       <c r="A35" s="5" t="s">
         <v>78</v>
       </c>
@@ -3336,7 +3336,7 @@
       </c>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="18.75">
       <c r="A36" s="5" t="s">
         <v>15</v>
       </c>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="18.75">
       <c r="A37" s="5" t="s">
         <v>80</v>
       </c>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18.75">
       <c r="A38" s="5" t="s">
         <v>81</v>
       </c>
@@ -3363,7 +3363,7 @@
       </c>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="18.75">
       <c r="A39" s="5" t="s">
         <v>18</v>
       </c>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="18.75">
       <c r="A40" s="5" t="s">
         <v>20</v>
       </c>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="18.75">
       <c r="A41" s="5" t="s">
         <v>20</v>
       </c>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="18.75">
       <c r="A42" s="5" t="s">
         <v>83</v>
       </c>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="18.75">
       <c r="A43" s="5" t="s">
         <v>85</v>
       </c>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="18.75">
       <c r="A44" s="5" t="s">
         <v>86</v>
       </c>
@@ -3417,7 +3417,7 @@
       </c>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="18.75">
       <c r="A45" s="5" t="s">
         <v>22</v>
       </c>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="18.75">
       <c r="A46" s="5" t="s">
         <v>23</v>
       </c>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="18.75">
       <c r="A47" s="5" t="s">
         <v>24</v>
       </c>
@@ -3444,7 +3444,7 @@
       </c>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:6" ht="18.75">
       <c r="A48" s="5" t="s">
         <v>25</v>
       </c>
@@ -3456,7 +3456,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6" ht="18.75">
       <c r="A49" s="5" t="s">
         <v>89</v>
       </c>
@@ -3468,7 +3468,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6" ht="18.75">
       <c r="A50" s="5" t="s">
         <v>91</v>
       </c>
@@ -3480,7 +3480,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6" ht="18.75">
       <c r="A51" s="5" t="s">
         <v>92</v>
       </c>
@@ -3492,7 +3492,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6" ht="18.75">
       <c r="A52" s="5" t="s">
         <v>93</v>
       </c>
@@ -3504,7 +3504,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6" ht="18.75">
       <c r="A53" s="5" t="s">
         <v>95</v>
       </c>
@@ -3516,7 +3516,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6" ht="18.75">
       <c r="A54" s="5" t="s">
         <v>97</v>
       </c>
@@ -3528,7 +3528,7 @@
       <c r="E54" s="3"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:6" ht="18.75">
       <c r="A55" s="5" t="s">
         <v>98</v>
       </c>
@@ -3540,7 +3540,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:6" ht="18.75">
       <c r="A56" s="5" t="s">
         <v>100</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="E56" s="3"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:6" ht="18.75">
       <c r="A57" s="5" t="s">
         <v>102</v>
       </c>
@@ -3564,7 +3564,7 @@
       <c r="E57" s="3"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:6" ht="18.75">
       <c r="A58" s="5" t="s">
         <v>104</v>
       </c>
@@ -3576,7 +3576,7 @@
       <c r="E58" s="3"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:6" ht="18.75">
       <c r="A59" s="5" t="s">
         <v>106</v>
       </c>
@@ -3588,7 +3588,7 @@
       <c r="E59" s="3"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" ht="18.75">
       <c r="A60" s="5" t="s">
         <v>108</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:6" ht="18.75">
       <c r="A61" s="5" t="s">
         <v>16</v>
       </c>
@@ -3612,7 +3612,7 @@
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:6" ht="18.75">
       <c r="A62" s="5" t="s">
         <v>110</v>
       </c>
@@ -3624,7 +3624,7 @@
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:6" ht="18.75">
       <c r="A63" s="5" t="s">
         <v>112</v>
       </c>
@@ -3636,7 +3636,7 @@
       <c r="E63" s="3"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:6" ht="18.75">
       <c r="A64" s="5" t="s">
         <v>113</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="E64" s="3"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:6" ht="18.75">
       <c r="A65" s="5" t="s">
         <v>114</v>
       </c>
@@ -3660,7 +3660,7 @@
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:6" ht="18.75">
       <c r="A66" s="5" t="s">
         <v>116</v>
       </c>
@@ -3672,7 +3672,7 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:6" ht="18.75">
       <c r="A67" s="5" t="s">
         <v>118</v>
       </c>
@@ -3684,7 +3684,7 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:6" ht="18.75">
       <c r="A68" s="5" t="s">
         <v>119</v>
       </c>
@@ -3696,7 +3696,7 @@
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:6" ht="18.75">
       <c r="A69" s="5" t="s">
         <v>120</v>
       </c>
@@ -3708,7 +3708,7 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:6" ht="18.75">
       <c r="A70" s="5" t="s">
         <v>122</v>
       </c>
@@ -3720,7 +3720,7 @@
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:6" ht="18.75">
       <c r="A71" s="5" t="s">
         <v>124</v>
       </c>
@@ -3732,7 +3732,7 @@
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:6" ht="18.75">
       <c r="A72" s="5" t="s">
         <v>125</v>
       </c>
@@ -3744,7 +3744,7 @@
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:6" ht="18.75">
       <c r="A73" s="5" t="s">
         <v>127</v>
       </c>
@@ -3756,7 +3756,7 @@
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:6" ht="18.75">
       <c r="A74" s="5" t="s">
         <v>129</v>
       </c>
@@ -3768,7 +3768,7 @@
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:6" ht="18.75">
       <c r="A75" s="5" t="s">
         <v>131</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:6" ht="18.75">
       <c r="A76" s="5" t="s">
         <v>133</v>
       </c>
@@ -3792,7 +3792,7 @@
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:6" ht="18.75">
       <c r="A77" s="5" t="s">
         <v>135</v>
       </c>
@@ -3804,7 +3804,7 @@
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:6" ht="18.75">
       <c r="A78" s="5" t="s">
         <v>137</v>
       </c>
@@ -3816,7 +3816,7 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="18.75">
       <c r="A79" s="5" t="s">
         <v>139</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="18.75">
       <c r="A80" s="5" t="s">
         <v>141</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="18.75">
       <c r="A81" s="5" t="s">
         <v>143</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="18.75">
       <c r="A82" s="5" t="s">
         <v>145</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="18.75">
       <c r="A83" s="5" t="s">
         <v>147</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="18.75">
       <c r="A84" s="5" t="s">
         <v>149</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="18.75">
       <c r="A85" s="5" t="s">
         <v>150</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="18.75">
       <c r="A86" s="5" t="s">
         <v>152</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="18.75">
       <c r="A87" s="5" t="s">
         <v>154</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="18.75">
       <c r="A88" s="5" t="s">
         <v>156</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="18.75">
       <c r="A89" s="5" t="s">
         <v>158</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="18.75">
       <c r="A90" s="5" t="s">
         <v>160</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="18.75">
       <c r="A91" s="5" t="s">
         <v>162</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="18.75">
       <c r="A92" s="5" t="s">
         <v>164</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="18.75">
       <c r="A93" s="5" t="s">
         <v>166</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="18.75">
       <c r="A94" s="5" t="s">
         <v>168</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="18.75">
       <c r="A95" s="5" t="s">
         <v>170</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="18.75">
       <c r="A96" s="5" t="s">
         <v>172</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="18.75">
       <c r="A97" s="5" t="s">
         <v>174</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="18.75">
       <c r="A98" s="5" t="s">
         <v>176</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="18.75">
       <c r="A99" s="5" t="s">
         <v>178</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="18.75">
       <c r="A100" s="5" t="s">
         <v>180</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="18.75">
       <c r="A101" s="5" t="s">
         <v>182</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="18.75">
       <c r="A102" s="5" t="s">
         <v>184</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="18.75">
       <c r="A103" s="5" t="s">
         <v>186</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="18.75">
       <c r="A104" s="5" t="s">
         <v>187</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="18.75">
       <c r="A105" s="5" t="s">
         <v>188</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="18.75">
       <c r="A106" s="5" t="s">
         <v>189</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="18.75">
       <c r="A107" s="5" t="s">
         <v>190</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="18.75">
       <c r="A108" s="5" t="s">
         <v>192</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="18.75">
       <c r="A109" s="5" t="s">
         <v>194</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="18.75">
       <c r="A110" s="5" t="s">
         <v>196</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="18.75">
       <c r="A111" s="5" t="s">
         <v>198</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="18.75">
       <c r="A112" s="5" t="s">
         <v>200</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="18.75">
       <c r="A113" s="5" t="s">
         <v>202</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="18.75">
       <c r="A114" s="5" t="s">
         <v>204</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="18.75">
       <c r="A115" s="5" t="s">
         <v>206</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="18.75">
       <c r="A116" s="5" t="s">
         <v>208</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="18.75">
       <c r="A117" s="5" t="s">
         <v>210</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="18.75">
       <c r="A118" s="5" t="s">
         <v>212</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="18.75">
       <c r="A119" s="5" t="s">
         <v>214</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="18.75">
       <c r="A120" s="5" t="s">
         <v>215</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="18.75">
       <c r="A121" s="5" t="s">
         <v>216</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="18.75">
       <c r="A122" s="5" t="s">
         <v>217</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="18.75">
       <c r="A123" s="5" t="s">
         <v>218</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="18.75">
       <c r="A124" s="5" t="s">
         <v>220</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="18.75">
       <c r="A125" s="5" t="s">
         <v>221</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="18.75">
       <c r="A126" s="5" t="s">
         <v>222</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="18.75">
       <c r="A127" s="5" t="s">
         <v>223</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" ht="18.75">
       <c r="A128" s="5" t="s">
         <v>224</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" ht="18.75">
       <c r="A129" s="5" t="s">
         <v>226</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" ht="18.75">
       <c r="A130" s="5" t="s">
         <v>228</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" ht="18.75">
       <c r="A131" s="5" t="s">
         <v>230</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" ht="18.75">
       <c r="A132" s="5" t="s">
         <v>232</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" ht="18.75">
       <c r="A133" s="5" t="s">
         <v>234</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" ht="18.75">
       <c r="A134" s="5" t="s">
         <v>236</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" ht="18.75">
       <c r="A135" s="5" t="s">
         <v>238</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" ht="18.75">
       <c r="A136" s="5" t="s">
         <v>240</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" ht="18.75">
       <c r="A137" s="5" t="s">
         <v>242</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" ht="18.75">
       <c r="A138" s="5" t="s">
         <v>244</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" ht="18.75">
       <c r="A139" s="5" t="s">
         <v>246</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" ht="18.75">
       <c r="A140" s="5" t="s">
         <v>248</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" ht="18.75">
       <c r="A141" s="5" t="s">
         <v>250</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" ht="18.75">
       <c r="A142" s="5" t="s">
         <v>252</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" ht="18.75">
       <c r="A143" s="5" t="s">
         <v>254</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" ht="18.75">
       <c r="A144" s="5" t="s">
         <v>256</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" ht="18.75">
       <c r="A145" s="5" t="s">
         <v>258</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" ht="18.75">
       <c r="A146" s="5" t="s">
         <v>259</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" ht="18.75">
       <c r="A147" s="5" t="s">
         <v>260</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" ht="18.75">
       <c r="A148" s="5" t="s">
         <v>261</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" ht="18.75">
       <c r="A149" s="5" t="s">
         <v>262</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" ht="18.75">
       <c r="A150" s="5" t="s">
         <v>263</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" ht="18.75">
       <c r="A151" s="5" t="s">
         <v>264</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" ht="18.75">
       <c r="A152" s="5" t="s">
         <v>265</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" ht="18.75">
       <c r="A153" s="5" t="s">
         <v>266</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" ht="18.75">
       <c r="A154" s="5" t="s">
         <v>268</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" ht="18.75">
       <c r="A155" s="5" t="s">
         <v>719</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" ht="18.75">
       <c r="A156" s="5" t="s">
         <v>271</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" ht="18.75">
       <c r="A157" s="5" t="s">
         <v>273</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" ht="18.75">
       <c r="A158" s="5" t="s">
         <v>275</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" ht="18.75">
       <c r="A159" s="5" t="s">
         <v>277</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" ht="18.75">
       <c r="A160" s="5" t="s">
         <v>279</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" ht="18.75">
       <c r="A161" s="5" t="s">
         <v>281</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" ht="18.75">
       <c r="A162" s="5" t="s">
         <v>283</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" ht="18.75">
       <c r="A163" s="5" t="s">
         <v>285</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" ht="18.75">
       <c r="A164" s="5" t="s">
         <v>287</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:2" ht="18.75">
       <c r="A165" s="3" t="s">
         <v>289</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:2" ht="18.75">
       <c r="A166" s="7" t="s">
         <v>291</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:2" ht="18.75">
       <c r="A167" s="7" t="s">
         <v>293</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:2" ht="18.75">
       <c r="A168" s="7" t="s">
         <v>295</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:2" ht="18.75">
       <c r="A169" s="7" t="s">
         <v>297</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2">
       <c r="A170" t="s">
         <v>299</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2">
       <c r="A171" t="s">
         <v>301</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2">
       <c r="A172" t="s">
         <v>303</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2">
       <c r="A173" t="s">
         <v>305</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2">
       <c r="A174" t="s">
         <v>307</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2">
       <c r="A175" t="s">
         <v>309</v>
       </c>
@@ -4592,7 +4592,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2">
       <c r="A176" t="s">
         <v>311</v>
       </c>
@@ -4600,7 +4600,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2">
       <c r="A177" t="s">
         <v>219</v>
       </c>
@@ -4608,7 +4608,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2">
       <c r="A178" t="s">
         <v>314</v>
       </c>
@@ -4616,7 +4616,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2">
       <c r="A179" t="s">
         <v>316</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2">
       <c r="A180" t="s">
         <v>318</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2">
       <c r="A181" t="s">
         <v>320</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2">
       <c r="A182" t="s">
         <v>322</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2">
       <c r="A183" t="s">
         <v>324</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2">
       <c r="A184" t="s">
         <v>326</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2">
       <c r="A185" t="s">
         <v>327</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2">
       <c r="A186" t="s">
         <v>328</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2">
       <c r="A187" t="s">
         <v>329</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2">
       <c r="A188" t="s">
         <v>330</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:2" ht="18.75">
       <c r="A189" s="3" t="s">
         <v>331</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:2" ht="18.75">
       <c r="A190" s="3" t="s">
         <v>333</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:2" ht="18.75">
       <c r="A191" s="3" t="s">
         <v>335</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2">
       <c r="A192" t="s">
         <v>337</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2">
       <c r="A193" t="s">
         <v>339</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2">
       <c r="A194" t="s">
         <v>341</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2">
       <c r="A195" t="s">
         <v>343</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2">
       <c r="A196" t="s">
         <v>345</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2">
       <c r="A197" t="s">
         <v>347</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2">
       <c r="A198" t="s">
         <v>349</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2">
       <c r="A199" t="s">
         <v>351</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2">
       <c r="A200" t="s">
         <v>352</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2">
       <c r="A201" t="s">
         <v>354</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2">
       <c r="A202" t="s">
         <v>356</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2">
       <c r="A203" t="s">
         <v>358</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2">
       <c r="A204" t="s">
         <v>360</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2">
       <c r="A205" t="s">
         <v>362</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2">
       <c r="A206" t="s">
         <v>364</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2">
       <c r="A207" t="s">
         <v>366</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2">
       <c r="A208" t="s">
         <v>368</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4">
       <c r="A209" t="s">
         <v>370</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4">
       <c r="A210" t="s">
         <v>372</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4">
       <c r="A211" t="s">
         <v>374</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4">
       <c r="A212" t="s">
         <v>375</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4">
       <c r="A213" t="s">
         <v>377</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4">
       <c r="A214" t="s">
         <v>379</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4">
       <c r="A215" t="s">
         <v>381</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4">
       <c r="A216" t="s">
         <v>383</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4">
       <c r="A217" t="s">
         <v>385</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4">
       <c r="A218" t="s">
         <v>387</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4">
       <c r="A219" t="s">
         <v>389</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4">
       <c r="A220" t="s">
         <v>390</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4">
       <c r="A221" t="s">
         <v>391</v>
       </c>
@@ -4960,7 +4960,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4">
       <c r="A222" t="s">
         <v>392</v>
       </c>
@@ -4974,7 +4974,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4">
       <c r="A223" t="s">
         <v>396</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4">
       <c r="A224" t="s">
         <v>400</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4">
       <c r="A225" t="s">
         <v>402</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4">
       <c r="A226" t="s">
         <v>405</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4">
       <c r="A227" t="s">
         <v>408</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4">
       <c r="A228" t="s">
         <v>411</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4">
       <c r="A229" t="s">
         <v>414</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4">
       <c r="A230" t="s">
         <v>416</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4">
       <c r="A231" t="s">
         <v>418</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4">
       <c r="A232" t="s">
         <v>420</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4">
       <c r="A233" t="s">
         <v>422</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4">
       <c r="A234" t="s">
         <v>425</v>
       </c>
@@ -5142,7 +5142,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4">
       <c r="A235" t="s">
         <v>428</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4">
       <c r="A236" t="s">
         <v>430</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4">
       <c r="A237" t="s">
         <v>434</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4">
       <c r="A238" t="s">
         <v>436</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4">
       <c r="A239" t="s">
         <v>439</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4">
       <c r="A240" t="s">
         <v>442</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4">
       <c r="A241" t="s">
         <v>445</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4">
       <c r="A242" t="s">
         <v>449</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4">
       <c r="A243" t="s">
         <v>452</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4">
       <c r="A244" t="s">
         <v>454</v>
       </c>
@@ -5282,7 +5282,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4">
       <c r="A245" t="s">
         <v>457</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4">
       <c r="A246" t="s">
         <v>460</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4">
       <c r="A247" t="s">
         <v>464</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4">
       <c r="A248" t="s">
         <v>467</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4">
       <c r="A249" t="s">
         <v>470</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4">
       <c r="A250" t="s">
         <v>472</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4">
       <c r="A251" t="s">
         <v>474</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4">
       <c r="A252" t="s">
         <v>476</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4">
       <c r="A253" t="s">
         <v>478</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4">
       <c r="A254" t="s">
         <v>480</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4">
       <c r="A255" t="s">
         <v>482</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4">
       <c r="A256" t="s">
         <v>484</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4">
       <c r="A257" t="s">
         <v>487</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4">
       <c r="A258" t="s">
         <v>490</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4">
       <c r="A259" t="s">
         <v>493</v>
       </c>
@@ -5492,7 +5492,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4">
       <c r="A260" t="s">
         <v>495</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4">
       <c r="A261" t="s">
         <v>498</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4">
       <c r="A262" t="s">
         <v>501</v>
       </c>
@@ -5534,7 +5534,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4">
       <c r="A263" t="s">
         <v>503</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4">
       <c r="A264" t="s">
         <v>505</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4">
       <c r="A265" t="s">
         <v>507</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4">
       <c r="A266" t="s">
         <v>509</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4">
       <c r="A267" t="s">
         <v>512</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4">
       <c r="A268" t="s">
         <v>515</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4">
       <c r="A269" t="s">
         <v>518</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4">
       <c r="A270" t="s">
         <v>521</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4">
       <c r="A271" t="s">
         <v>523</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4">
       <c r="A272" t="s">
         <v>525</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4">
       <c r="A273" t="s">
         <v>527</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4">
       <c r="A274" t="s">
         <v>529</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4">
       <c r="A275" t="s">
         <v>531</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4">
       <c r="A276" t="s">
         <v>533</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4">
       <c r="A277" t="s">
         <v>534</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4">
       <c r="A278" t="s">
         <v>537</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:4" ht="18.75">
       <c r="A279" s="3" t="s">
         <v>538</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:4" ht="18.75">
       <c r="A280" t="s">
         <v>540</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:4" ht="18.75">
       <c r="A281" t="s">
         <v>542</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:4" ht="18.75">
       <c r="A282" s="3" t="s">
         <v>544</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4">
       <c r="A283" t="s">
         <v>546</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:4">
       <c r="A284" t="s">
         <v>549</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4">
       <c r="A285" t="s">
         <v>552</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4">
       <c r="A286" t="s">
         <v>555</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4">
       <c r="A287" t="s">
         <v>558</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4">
       <c r="A288" t="s">
         <v>561</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:4">
       <c r="A289" t="s">
         <v>563</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4">
       <c r="A290" t="s">
         <v>566</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4">
       <c r="A291" t="s">
         <v>569</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4">
       <c r="A292" t="s">
         <v>572</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4">
       <c r="A293" t="s">
         <v>575</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4">
       <c r="A294" t="s">
         <v>578</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4">
       <c r="A295" t="s">
         <v>581</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4">
       <c r="A296" t="s">
         <v>584</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4">
       <c r="A297" t="s">
         <v>587</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4">
       <c r="A298" t="s">
         <v>589</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4">
       <c r="A299" t="s">
         <v>591</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4">
       <c r="A300" t="s">
         <v>594</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4">
       <c r="A301" t="s">
         <v>596</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4">
       <c r="A302" t="s">
         <v>599</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4">
       <c r="A303" t="s">
         <v>602</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4">
       <c r="A304" t="s">
         <v>605</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4">
       <c r="A305" t="s">
         <v>608</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:4">
       <c r="A306" t="s">
         <v>611</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:4">
       <c r="A307" t="s">
         <v>613</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4">
       <c r="A308" t="s">
         <v>616</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:4">
       <c r="A309" t="s">
         <v>619</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4">
       <c r="A310" t="s">
         <v>622</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4">
       <c r="A311" t="s">
         <v>624</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4">
       <c r="A312" t="s">
         <v>626</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4">
       <c r="A313" t="s">
         <v>629</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4">
       <c r="A314" t="s">
         <v>632</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:4">
       <c r="A315" t="s">
         <v>634</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4">
       <c r="A316" t="s">
         <v>636</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4">
       <c r="A317" t="s">
         <v>639</v>
       </c>
@@ -6274,7 +6274,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:4">
       <c r="A318" t="s">
         <v>642</v>
       </c>
@@ -6288,7 +6288,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:4">
       <c r="A319" t="s">
         <v>644</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:4">
       <c r="A320" t="s">
         <v>647</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4">
       <c r="A321" t="s">
         <v>650</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4">
       <c r="A322" t="s">
         <v>653</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4">
       <c r="A323" t="s">
         <v>655</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4">
       <c r="A324" t="s">
         <v>658</v>
       </c>
@@ -6372,7 +6372,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4">
       <c r="A325" t="s">
         <v>661</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:4">
       <c r="A326" t="s">
         <v>663</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4">
       <c r="A327" t="s">
         <v>665</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4">
       <c r="A328" t="s">
         <v>668</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:4">
       <c r="A329" t="s">
         <v>670</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4">
       <c r="A330" t="s">
         <v>673</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:4">
       <c r="A331" t="s">
         <v>675</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:4">
       <c r="A332" t="s">
         <v>677</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4">
       <c r="A333" t="s">
         <v>679</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:4">
       <c r="A334" t="s">
         <v>681</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:4">
       <c r="A335" t="s">
         <v>683</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:4">
       <c r="A336" t="s">
         <v>686</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:4">
       <c r="A337" t="s">
         <v>688</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:4">
       <c r="A338" t="s">
         <v>690</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:4">
       <c r="A339" t="s">
         <v>693</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:4">
       <c r="A340" t="s">
         <v>696</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:4">
       <c r="A341" t="s">
         <v>699</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:4">
       <c r="A342" t="s">
         <v>702</v>
       </c>
@@ -6624,7 +6624,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:4">
       <c r="A343" t="s">
         <v>703</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:4">
       <c r="A344" t="s">
         <v>705</v>
       </c>
@@ -6652,7 +6652,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:4">
       <c r="A345" t="s">
         <v>707</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:4">
       <c r="A346" t="s">
         <v>709</v>
       </c>
@@ -6680,7 +6680,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:4">
       <c r="A347" t="s">
         <v>710</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:4">
       <c r="A348" t="s">
         <v>712</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:4">
       <c r="A349" t="s">
         <v>714</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:4">
       <c r="A350" t="s">
         <v>716</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="351" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="351" spans="1:4" ht="18.75">
       <c r="A351" s="3" t="s">
         <v>718</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:4">
       <c r="A352" t="s">
         <v>720</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:4">
       <c r="A353" t="s">
         <v>723</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:4">
       <c r="A354" t="s">
         <v>726</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:4">
       <c r="A355" t="s">
         <v>729</v>
       </c>
@@ -6800,7 +6800,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:4">
       <c r="A356" t="s">
         <v>732</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:4">
       <c r="A357" t="s">
         <v>735</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:4">
       <c r="A358" t="s">
         <v>738</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:4">
       <c r="A359" t="s">
         <v>741</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:4">
       <c r="A360" t="s">
         <v>744</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:4">
       <c r="A361" t="s">
         <v>747</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:4">
       <c r="A362" t="s">
         <v>749</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:4">
       <c r="A363" t="s">
         <v>751</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:4">
       <c r="A364" t="s">
         <v>753</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:4">
       <c r="A365" t="s">
         <v>756</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:4">
       <c r="A366" t="s">
         <v>759</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:4">
       <c r="A367" t="s">
         <v>762</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:4">
       <c r="A368" t="s">
         <v>765</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:4">
       <c r="A369" t="s">
         <v>768</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:4">
       <c r="A370" t="s">
         <v>771</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:4">
       <c r="A371" t="s">
         <v>774</v>
       </c>
@@ -7024,7 +7024,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:4">
       <c r="A372" t="s">
         <v>776</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:4">
       <c r="A373" t="s">
         <v>778</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:4">
       <c r="A374" t="s">
         <v>780</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:4">
       <c r="A375" t="s">
         <v>782</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:4">
       <c r="A376" t="s">
         <v>784</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:4">
       <c r="A377" t="s">
         <v>786</v>
       </c>
@@ -7108,7 +7108,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:4">
       <c r="A378" t="s">
         <v>788</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:4">
       <c r="A379" t="s">
         <v>790</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:4">
       <c r="A380" t="s">
         <v>793</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:4">
       <c r="A381" t="s">
         <v>796</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:4">
       <c r="A382" t="s">
         <v>799</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:4">
       <c r="A383" t="s">
         <v>802</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:4">
       <c r="A384" t="s">
         <v>805</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:4">
       <c r="A385" t="s">
         <v>807</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:4">
       <c r="A386" t="s">
         <v>810</v>
       </c>
@@ -7234,7 +7234,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:4">
       <c r="A387" t="s">
         <v>813</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:4">
       <c r="A388" t="s">
         <v>816</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:4">
       <c r="A389" t="s">
         <v>819</v>
       </c>
@@ -7276,7 +7276,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:4">
       <c r="A390" t="s">
         <v>822</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:4">
       <c r="A391" t="s">
         <v>825</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:4">
       <c r="A392" t="s">
         <v>828</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:4">
       <c r="A393" t="s">
         <v>830</v>
       </c>
@@ -7332,7 +7332,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:4">
       <c r="A394" t="s">
         <v>833</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:4">
       <c r="A395" t="s">
         <v>836</v>
       </c>

</xml_diff>

<commit_message>
add verbs and non verbs
</commit_message>
<xml_diff>
--- a/non_verbs.xlsx
+++ b/non_verbs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mptang\Desktop\local testing\online-web-app-deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB442C06-34DE-4804-8B70-566AF29E50BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B164DF-57C3-4D43-B6B6-805A92E9B339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="3570" windowWidth="21600" windowHeight="11295" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
+    <workbookView xWindow="35700" yWindow="3345" windowWidth="21600" windowHeight="11295" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="921">
   <si>
     <t>Kanji</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2811,6 +2811,27 @@
   </si>
   <si>
     <t>廣播員</t>
+  </si>
+  <si>
+    <t>活動</t>
+  </si>
+  <si>
+    <t>かつどう</t>
+  </si>
+  <si>
+    <t>確認</t>
+  </si>
+  <si>
+    <t>かくにん</t>
+  </si>
+  <si>
+    <t>通勤</t>
+  </si>
+  <si>
+    <t>つうきん</t>
+  </si>
+  <si>
+    <t>ソーダ</t>
   </si>
 </sst>
 </file>
@@ -3219,10 +3240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F425"/>
+  <dimension ref="A1:F429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="D415" sqref="D415"/>
+    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
+      <selection activeCell="A430" sqref="A430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7979,6 +8000,38 @@
         <v>913</v>
       </c>
     </row>
+    <row r="426" spans="1:4">
+      <c r="A426" t="s">
+        <v>914</v>
+      </c>
+      <c r="B426" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4">
+      <c r="A427" t="s">
+        <v>916</v>
+      </c>
+      <c r="B427" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4">
+      <c r="A428" t="s">
+        <v>918</v>
+      </c>
+      <c r="B428" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4">
+      <c r="A429" t="s">
+        <v>920</v>
+      </c>
+      <c r="B429" t="s">
+        <v>920</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update non_verbs.xlsx with new data
</commit_message>
<xml_diff>
--- a/non_verbs.xlsx
+++ b/non_verbs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mptang\Desktop\local testing\online-web-app-deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B164DF-57C3-4D43-B6B6-805A92E9B339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45DE2F5-A9CF-4566-A43C-B095AF8BA269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35700" yWindow="3345" windowWidth="21600" windowHeight="11295" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="926">
   <si>
     <t>Kanji</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2832,17 +2832,37 @@
   </si>
   <si>
     <t>ソーダ</t>
+  </si>
+  <si>
+    <t>テープ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>全部</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ぜんぶ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>無理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>むり</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2851,14 +2871,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2928,7 +2948,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2944,9 +2964,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2984,7 +3004,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3090,7 +3110,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3232,7 +3252,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3240,13 +3260,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F429"/>
+  <dimension ref="A1:F432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="A430" sqref="A430"/>
+    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
+      <selection activeCell="B432" sqref="B432"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
@@ -3256,7 +3276,7 @@
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3268,7 +3288,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3280,7 +3300,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -3292,7 +3312,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -3304,7 +3324,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -3316,7 +3336,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -3328,7 +3348,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -3340,7 +3360,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75">
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -3352,7 +3372,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -3364,7 +3384,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75">
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -3373,7 +3393,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75">
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -3382,7 +3402,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75">
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -3391,7 +3411,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75">
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -3400,7 +3420,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75">
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
@@ -3409,7 +3429,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75">
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>40</v>
       </c>
@@ -3418,7 +3438,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="18.75">
+    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -3427,7 +3447,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75">
+    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>44</v>
       </c>
@@ -3436,7 +3456,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75">
+    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>46</v>
       </c>
@@ -3445,7 +3465,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75">
+    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>48</v>
       </c>
@@ -3454,7 +3474,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75">
+    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>50</v>
       </c>
@@ -3463,7 +3483,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75">
+    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>52</v>
       </c>
@@ -3472,7 +3492,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75">
+    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
@@ -3481,7 +3501,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75">
+    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>56</v>
       </c>
@@ -3490,7 +3510,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75">
+    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>58</v>
       </c>
@@ -3499,7 +3519,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75">
+    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>60</v>
       </c>
@@ -3508,7 +3528,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="18.75">
+    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>62</v>
       </c>
@@ -3517,7 +3537,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75">
+    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>63</v>
       </c>
@@ -3526,7 +3546,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75">
+    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>64</v>
       </c>
@@ -3535,7 +3555,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="18.75">
+    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>66</v>
       </c>
@@ -3544,7 +3564,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="18.75">
+    <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>68</v>
       </c>
@@ -3553,7 +3573,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75">
+    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>70</v>
       </c>
@@ -3562,7 +3582,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75">
+    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>72</v>
       </c>
@@ -3571,7 +3591,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75">
+    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>74</v>
       </c>
@@ -3580,7 +3600,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75">
+    <row r="34" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>76</v>
       </c>
@@ -3589,7 +3609,7 @@
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="18.75">
+    <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>78</v>
       </c>
@@ -3598,7 +3618,7 @@
       </c>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75">
+    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>15</v>
       </c>
@@ -3607,7 +3627,7 @@
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="18.75">
+    <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>80</v>
       </c>
@@ -3616,7 +3636,7 @@
       </c>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="18.75">
+    <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>81</v>
       </c>
@@ -3625,7 +3645,7 @@
       </c>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="18.75">
+    <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>18</v>
       </c>
@@ -3634,7 +3654,7 @@
       </c>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="18.75">
+    <row r="40" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>20</v>
       </c>
@@ -3643,7 +3663,7 @@
       </c>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="18.75">
+    <row r="41" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>20</v>
       </c>
@@ -3652,7 +3672,7 @@
       </c>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" ht="18.75">
+    <row r="42" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>83</v>
       </c>
@@ -3661,7 +3681,7 @@
       </c>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="18.75">
+    <row r="43" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>85</v>
       </c>
@@ -3670,7 +3690,7 @@
       </c>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="18.75">
+    <row r="44" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>86</v>
       </c>
@@ -3679,7 +3699,7 @@
       </c>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="18.75">
+    <row r="45" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>22</v>
       </c>
@@ -3688,7 +3708,7 @@
       </c>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" ht="18.75">
+    <row r="46" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>23</v>
       </c>
@@ -3697,7 +3717,7 @@
       </c>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" ht="18.75">
+    <row r="47" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>24</v>
       </c>
@@ -3706,7 +3726,7 @@
       </c>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" ht="18.75">
+    <row r="48" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A48" s="5" t="s">
         <v>25</v>
       </c>
@@ -3718,7 +3738,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" ht="18.75">
+    <row r="49" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A49" s="5" t="s">
         <v>89</v>
       </c>
@@ -3730,7 +3750,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" ht="18.75">
+    <row r="50" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A50" s="5" t="s">
         <v>91</v>
       </c>
@@ -3742,7 +3762,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:6" ht="18.75">
+    <row r="51" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>92</v>
       </c>
@@ -3754,7 +3774,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" ht="18.75">
+    <row r="52" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>93</v>
       </c>
@@ -3766,7 +3786,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" ht="18.75">
+    <row r="53" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
         <v>95</v>
       </c>
@@ -3778,7 +3798,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" ht="18.75">
+    <row r="54" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
         <v>97</v>
       </c>
@@ -3790,7 +3810,7 @@
       <c r="E54" s="3"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" ht="18.75">
+    <row r="55" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>98</v>
       </c>
@@ -3802,7 +3822,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" ht="18.75">
+    <row r="56" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A56" s="5" t="s">
         <v>100</v>
       </c>
@@ -3814,7 +3834,7 @@
       <c r="E56" s="3"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" ht="18.75">
+    <row r="57" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A57" s="5" t="s">
         <v>102</v>
       </c>
@@ -3826,7 +3846,7 @@
       <c r="E57" s="3"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" ht="18.75">
+    <row r="58" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A58" s="5" t="s">
         <v>104</v>
       </c>
@@ -3838,7 +3858,7 @@
       <c r="E58" s="3"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" ht="18.75">
+    <row r="59" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>106</v>
       </c>
@@ -3850,7 +3870,7 @@
       <c r="E59" s="3"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" ht="18.75">
+    <row r="60" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>108</v>
       </c>
@@ -3862,7 +3882,7 @@
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6" ht="18.75">
+    <row r="61" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>16</v>
       </c>
@@ -3874,7 +3894,7 @@
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" ht="18.75">
+    <row r="62" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
         <v>110</v>
       </c>
@@ -3886,7 +3906,7 @@
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:6" ht="18.75">
+    <row r="63" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>112</v>
       </c>
@@ -3898,7 +3918,7 @@
       <c r="E63" s="3"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" ht="18.75">
+    <row r="64" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>113</v>
       </c>
@@ -3910,7 +3930,7 @@
       <c r="E64" s="3"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" ht="18.75">
+    <row r="65" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
         <v>114</v>
       </c>
@@ -3922,7 +3942,7 @@
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" ht="18.75">
+    <row r="66" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A66" s="5" t="s">
         <v>116</v>
       </c>
@@ -3934,7 +3954,7 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" ht="18.75">
+    <row r="67" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A67" s="5" t="s">
         <v>118</v>
       </c>
@@ -3946,7 +3966,7 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6" ht="18.75">
+    <row r="68" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A68" s="5" t="s">
         <v>119</v>
       </c>
@@ -3958,7 +3978,7 @@
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6" ht="18.75">
+    <row r="69" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A69" s="5" t="s">
         <v>120</v>
       </c>
@@ -3970,7 +3990,7 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6" ht="18.75">
+    <row r="70" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A70" s="5" t="s">
         <v>122</v>
       </c>
@@ -3982,7 +4002,7 @@
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="1:6" ht="18.75">
+    <row r="71" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A71" s="5" t="s">
         <v>124</v>
       </c>
@@ -3994,7 +4014,7 @@
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:6" ht="18.75">
+    <row r="72" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A72" s="5" t="s">
         <v>125</v>
       </c>
@@ -4006,7 +4026,7 @@
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6" ht="18.75">
+    <row r="73" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A73" s="5" t="s">
         <v>127</v>
       </c>
@@ -4018,7 +4038,7 @@
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:6" ht="18.75">
+    <row r="74" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A74" s="5" t="s">
         <v>129</v>
       </c>
@@ -4030,7 +4050,7 @@
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="1:6" ht="18.75">
+    <row r="75" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A75" s="5" t="s">
         <v>131</v>
       </c>
@@ -4042,7 +4062,7 @@
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="1:6" ht="18.75">
+    <row r="76" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A76" s="5" t="s">
         <v>133</v>
       </c>
@@ -4054,7 +4074,7 @@
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="1:6" ht="18.75">
+    <row r="77" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A77" s="5" t="s">
         <v>135</v>
       </c>
@@ -4066,7 +4086,7 @@
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6" ht="18.75">
+    <row r="78" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A78" s="5" t="s">
         <v>137</v>
       </c>
@@ -4078,7 +4098,7 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:6" ht="18.75">
+    <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>139</v>
       </c>
@@ -4086,7 +4106,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="18.75">
+    <row r="80" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>141</v>
       </c>
@@ -4094,7 +4114,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="18.75">
+    <row r="81" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>143</v>
       </c>
@@ -4102,7 +4122,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="18.75">
+    <row r="82" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>145</v>
       </c>
@@ -4110,7 +4130,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="18.75">
+    <row r="83" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>147</v>
       </c>
@@ -4118,7 +4138,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="18.75">
+    <row r="84" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>149</v>
       </c>
@@ -4126,7 +4146,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="18.75">
+    <row r="85" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>150</v>
       </c>
@@ -4134,7 +4154,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="18.75">
+    <row r="86" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>152</v>
       </c>
@@ -4142,7 +4162,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="18.75">
+    <row r="87" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>154</v>
       </c>
@@ -4150,7 +4170,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="18.75">
+    <row r="88" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>156</v>
       </c>
@@ -4158,7 +4178,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="18.75">
+    <row r="89" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>158</v>
       </c>
@@ -4166,7 +4186,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="18.75">
+    <row r="90" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>160</v>
       </c>
@@ -4174,7 +4194,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="18.75">
+    <row r="91" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>162</v>
       </c>
@@ -4182,7 +4202,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="18.75">
+    <row r="92" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>164</v>
       </c>
@@ -4190,7 +4210,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="18.75">
+    <row r="93" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>166</v>
       </c>
@@ -4198,7 +4218,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="18.75">
+    <row r="94" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>168</v>
       </c>
@@ -4206,7 +4226,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="18.75">
+    <row r="95" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>170</v>
       </c>
@@ -4214,7 +4234,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="18.75">
+    <row r="96" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>172</v>
       </c>
@@ -4222,7 +4242,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="18.75">
+    <row r="97" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>174</v>
       </c>
@@ -4230,7 +4250,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="18.75">
+    <row r="98" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>176</v>
       </c>
@@ -4238,7 +4258,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="18.75">
+    <row r="99" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>178</v>
       </c>
@@ -4246,7 +4266,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="18.75">
+    <row r="100" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>180</v>
       </c>
@@ -4254,7 +4274,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="18.75">
+    <row r="101" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>182</v>
       </c>
@@ -4262,7 +4282,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="18.75">
+    <row r="102" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>184</v>
       </c>
@@ -4270,7 +4290,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="18.75">
+    <row r="103" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>186</v>
       </c>
@@ -4278,7 +4298,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="18.75">
+    <row r="104" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>187</v>
       </c>
@@ -4286,7 +4306,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="18.75">
+    <row r="105" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>188</v>
       </c>
@@ -4294,7 +4314,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="18.75">
+    <row r="106" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>189</v>
       </c>
@@ -4302,7 +4322,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="18.75">
+    <row r="107" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>190</v>
       </c>
@@ -4310,7 +4330,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="18.75">
+    <row r="108" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>192</v>
       </c>
@@ -4318,7 +4338,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="18.75">
+    <row r="109" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>194</v>
       </c>
@@ -4326,7 +4346,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="18.75">
+    <row r="110" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>196</v>
       </c>
@@ -4334,7 +4354,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="18.75">
+    <row r="111" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>198</v>
       </c>
@@ -4342,7 +4362,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="18.75">
+    <row r="112" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>200</v>
       </c>
@@ -4350,7 +4370,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="18.75">
+    <row r="113" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>202</v>
       </c>
@@ -4358,7 +4378,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="18.75">
+    <row r="114" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>204</v>
       </c>
@@ -4366,7 +4386,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="18.75">
+    <row r="115" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>206</v>
       </c>
@@ -4374,7 +4394,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="18.75">
+    <row r="116" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>208</v>
       </c>
@@ -4382,7 +4402,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="18.75">
+    <row r="117" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>210</v>
       </c>
@@ -4390,7 +4410,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="18.75">
+    <row r="118" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>212</v>
       </c>
@@ -4398,7 +4418,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="18.75">
+    <row r="119" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>214</v>
       </c>
@@ -4406,7 +4426,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="18.75">
+    <row r="120" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>215</v>
       </c>
@@ -4414,7 +4434,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="18.75">
+    <row r="121" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>216</v>
       </c>
@@ -4422,7 +4442,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="18.75">
+    <row r="122" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>217</v>
       </c>
@@ -4430,7 +4450,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="18.75">
+    <row r="123" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>218</v>
       </c>
@@ -4438,7 +4458,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="18.75">
+    <row r="124" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>220</v>
       </c>
@@ -4446,7 +4466,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="18.75">
+    <row r="125" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>221</v>
       </c>
@@ -4454,7 +4474,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="18.75">
+    <row r="126" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>222</v>
       </c>
@@ -4462,7 +4482,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="18.75">
+    <row r="127" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>223</v>
       </c>
@@ -4470,7 +4490,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="18.75">
+    <row r="128" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>224</v>
       </c>
@@ -4478,7 +4498,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="18.75">
+    <row r="129" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>226</v>
       </c>
@@ -4486,7 +4506,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="18.75">
+    <row r="130" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>228</v>
       </c>
@@ -4494,7 +4514,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="18.75">
+    <row r="131" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>230</v>
       </c>
@@ -4502,7 +4522,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="18.75">
+    <row r="132" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>232</v>
       </c>
@@ -4510,7 +4530,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="18.75">
+    <row r="133" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>234</v>
       </c>
@@ -4518,7 +4538,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="18.75">
+    <row r="134" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>236</v>
       </c>
@@ -4526,7 +4546,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="18.75">
+    <row r="135" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>238</v>
       </c>
@@ -4534,7 +4554,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="18.75">
+    <row r="136" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>240</v>
       </c>
@@ -4542,7 +4562,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="18.75">
+    <row r="137" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>242</v>
       </c>
@@ -4550,7 +4570,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="18.75">
+    <row r="138" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>244</v>
       </c>
@@ -4558,7 +4578,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="18.75">
+    <row r="139" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>246</v>
       </c>
@@ -4566,7 +4586,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="18.75">
+    <row r="140" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>248</v>
       </c>
@@ -4574,7 +4594,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="18.75">
+    <row r="141" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>250</v>
       </c>
@@ -4582,7 +4602,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="18.75">
+    <row r="142" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>252</v>
       </c>
@@ -4590,7 +4610,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="18.75">
+    <row r="143" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>254</v>
       </c>
@@ -4598,7 +4618,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="18.75">
+    <row r="144" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>256</v>
       </c>
@@ -4606,7 +4626,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="18.75">
+    <row r="145" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>258</v>
       </c>
@@ -4614,7 +4634,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="18.75">
+    <row r="146" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>259</v>
       </c>
@@ -4622,7 +4642,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="18.75">
+    <row r="147" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>260</v>
       </c>
@@ -4630,7 +4650,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="18.75">
+    <row r="148" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>261</v>
       </c>
@@ -4638,7 +4658,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="18.75">
+    <row r="149" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>262</v>
       </c>
@@ -4646,7 +4666,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="18.75">
+    <row r="150" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>263</v>
       </c>
@@ -4654,7 +4674,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="18.75">
+    <row r="151" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>264</v>
       </c>
@@ -4662,7 +4682,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="18.75">
+    <row r="152" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>265</v>
       </c>
@@ -4670,7 +4690,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="18.75">
+    <row r="153" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>266</v>
       </c>
@@ -4678,7 +4698,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="18.75">
+    <row r="154" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>268</v>
       </c>
@@ -4686,7 +4706,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="18.75">
+    <row r="155" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>719</v>
       </c>
@@ -4694,7 +4714,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="18.75">
+    <row r="156" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>271</v>
       </c>
@@ -4702,7 +4722,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="18.75">
+    <row r="157" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>273</v>
       </c>
@@ -4710,7 +4730,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="18.75">
+    <row r="158" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>275</v>
       </c>
@@ -4718,7 +4738,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="18.75">
+    <row r="159" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>277</v>
       </c>
@@ -4726,7 +4746,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="18.75">
+    <row r="160" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>279</v>
       </c>
@@ -4734,7 +4754,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="18.75">
+    <row r="161" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>281</v>
       </c>
@@ -4742,7 +4762,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="18.75">
+    <row r="162" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>283</v>
       </c>
@@ -4750,7 +4770,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="18.75">
+    <row r="163" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>285</v>
       </c>
@@ -4758,7 +4778,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="18.75">
+    <row r="164" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>287</v>
       </c>
@@ -4766,7 +4786,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="18.75">
+    <row r="165" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A165" s="3" t="s">
         <v>289</v>
       </c>
@@ -4774,7 +4794,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="18.75">
+    <row r="166" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A166" s="7" t="s">
         <v>291</v>
       </c>
@@ -4782,7 +4802,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="18.75">
+    <row r="167" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A167" s="7" t="s">
         <v>293</v>
       </c>
@@ -4790,7 +4810,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="18.75">
+    <row r="168" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A168" s="7" t="s">
         <v>295</v>
       </c>
@@ -4798,7 +4818,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="18.75">
+    <row r="169" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A169" s="7" t="s">
         <v>297</v>
       </c>
@@ -4806,7 +4826,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>299</v>
       </c>
@@ -4814,7 +4834,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>301</v>
       </c>
@@ -4822,7 +4842,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>303</v>
       </c>
@@ -4830,7 +4850,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>305</v>
       </c>
@@ -4838,7 +4858,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>307</v>
       </c>
@@ -4846,7 +4866,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>309</v>
       </c>
@@ -4854,7 +4874,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>311</v>
       </c>
@@ -4862,7 +4882,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>219</v>
       </c>
@@ -4870,7 +4890,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>314</v>
       </c>
@@ -4878,7 +4898,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>316</v>
       </c>
@@ -4886,7 +4906,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>318</v>
       </c>
@@ -4894,7 +4914,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>320</v>
       </c>
@@ -4902,7 +4922,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>322</v>
       </c>
@@ -4910,7 +4930,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>324</v>
       </c>
@@ -4918,7 +4938,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>326</v>
       </c>
@@ -4926,7 +4946,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>327</v>
       </c>
@@ -4934,7 +4954,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>328</v>
       </c>
@@ -4942,7 +4962,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>329</v>
       </c>
@@ -4950,7 +4970,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>330</v>
       </c>
@@ -4958,7 +4978,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="18.75">
+    <row r="189" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A189" s="3" t="s">
         <v>331</v>
       </c>
@@ -4966,7 +4986,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="18.75">
+    <row r="190" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A190" s="3" t="s">
         <v>333</v>
       </c>
@@ -4974,7 +4994,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="18.75">
+    <row r="191" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A191" s="3" t="s">
         <v>335</v>
       </c>
@@ -4982,7 +5002,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>337</v>
       </c>
@@ -4990,7 +5010,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>339</v>
       </c>
@@ -4998,7 +5018,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>341</v>
       </c>
@@ -5006,7 +5026,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>343</v>
       </c>
@@ -5014,7 +5034,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>345</v>
       </c>
@@ -5022,7 +5042,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>347</v>
       </c>
@@ -5030,7 +5050,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>349</v>
       </c>
@@ -5038,7 +5058,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>351</v>
       </c>
@@ -5046,7 +5066,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>352</v>
       </c>
@@ -5054,7 +5074,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>354</v>
       </c>
@@ -5062,7 +5082,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>356</v>
       </c>
@@ -5070,7 +5090,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>358</v>
       </c>
@@ -5078,7 +5098,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>360</v>
       </c>
@@ -5086,7 +5106,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>362</v>
       </c>
@@ -5094,7 +5114,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>364</v>
       </c>
@@ -5102,7 +5122,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>366</v>
       </c>
@@ -5110,7 +5130,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>368</v>
       </c>
@@ -5118,7 +5138,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>370</v>
       </c>
@@ -5126,7 +5146,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>372</v>
       </c>
@@ -5134,7 +5154,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>374</v>
       </c>
@@ -5142,7 +5162,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>375</v>
       </c>
@@ -5150,7 +5170,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>377</v>
       </c>
@@ -5158,7 +5178,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>379</v>
       </c>
@@ -5166,7 +5186,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>381</v>
       </c>
@@ -5174,7 +5194,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="216" spans="1:4">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>383</v>
       </c>
@@ -5182,7 +5202,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="217" spans="1:4">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>385</v>
       </c>
@@ -5190,7 +5210,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="218" spans="1:4">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>387</v>
       </c>
@@ -5198,7 +5218,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="219" spans="1:4">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>389</v>
       </c>
@@ -5206,7 +5226,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="220" spans="1:4">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>390</v>
       </c>
@@ -5214,7 +5234,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="221" spans="1:4">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>391</v>
       </c>
@@ -5222,7 +5242,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="222" spans="1:4">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>392</v>
       </c>
@@ -5236,7 +5256,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="223" spans="1:4">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>396</v>
       </c>
@@ -5250,7 +5270,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="224" spans="1:4">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>400</v>
       </c>
@@ -5264,7 +5284,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="225" spans="1:4">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>402</v>
       </c>
@@ -5278,7 +5298,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="226" spans="1:4">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>405</v>
       </c>
@@ -5292,7 +5312,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="227" spans="1:4">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>408</v>
       </c>
@@ -5306,7 +5326,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="228" spans="1:4">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>411</v>
       </c>
@@ -5320,7 +5340,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="229" spans="1:4">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>414</v>
       </c>
@@ -5334,7 +5354,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="230" spans="1:4">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>416</v>
       </c>
@@ -5348,7 +5368,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="231" spans="1:4">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>418</v>
       </c>
@@ -5362,7 +5382,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="232" spans="1:4">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>420</v>
       </c>
@@ -5376,7 +5396,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="233" spans="1:4">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>422</v>
       </c>
@@ -5390,7 +5410,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="234" spans="1:4">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>425</v>
       </c>
@@ -5404,7 +5424,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="235" spans="1:4">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>428</v>
       </c>
@@ -5418,7 +5438,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="236" spans="1:4">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>430</v>
       </c>
@@ -5432,7 +5452,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="237" spans="1:4">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>434</v>
       </c>
@@ -5446,7 +5466,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="238" spans="1:4">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>436</v>
       </c>
@@ -5460,7 +5480,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="239" spans="1:4">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>439</v>
       </c>
@@ -5474,7 +5494,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="240" spans="1:4">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>442</v>
       </c>
@@ -5488,7 +5508,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="241" spans="1:4">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>445</v>
       </c>
@@ -5502,7 +5522,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="242" spans="1:4">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>449</v>
       </c>
@@ -5516,7 +5536,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="243" spans="1:4">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>452</v>
       </c>
@@ -5530,7 +5550,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="244" spans="1:4">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>454</v>
       </c>
@@ -5544,7 +5564,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="245" spans="1:4">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>457</v>
       </c>
@@ -5558,7 +5578,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="246" spans="1:4">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>460</v>
       </c>
@@ -5572,7 +5592,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="247" spans="1:4">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>464</v>
       </c>
@@ -5586,7 +5606,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="248" spans="1:4">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>467</v>
       </c>
@@ -5600,7 +5620,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="249" spans="1:4">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>470</v>
       </c>
@@ -5614,7 +5634,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="250" spans="1:4">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>472</v>
       </c>
@@ -5628,7 +5648,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="251" spans="1:4">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>474</v>
       </c>
@@ -5642,7 +5662,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="252" spans="1:4">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>476</v>
       </c>
@@ -5656,7 +5676,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="253" spans="1:4">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>478</v>
       </c>
@@ -5670,7 +5690,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="254" spans="1:4">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>480</v>
       </c>
@@ -5684,7 +5704,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="255" spans="1:4">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>482</v>
       </c>
@@ -5698,7 +5718,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="256" spans="1:4">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>484</v>
       </c>
@@ -5712,7 +5732,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="257" spans="1:4">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>487</v>
       </c>
@@ -5726,7 +5746,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="258" spans="1:4">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>490</v>
       </c>
@@ -5740,7 +5760,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="259" spans="1:4">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>493</v>
       </c>
@@ -5754,7 +5774,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="260" spans="1:4">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>495</v>
       </c>
@@ -5768,7 +5788,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="261" spans="1:4">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>498</v>
       </c>
@@ -5782,7 +5802,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="262" spans="1:4">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>501</v>
       </c>
@@ -5796,7 +5816,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="263" spans="1:4">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>503</v>
       </c>
@@ -5810,7 +5830,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="264" spans="1:4">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>505</v>
       </c>
@@ -5824,7 +5844,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="265" spans="1:4">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>507</v>
       </c>
@@ -5838,7 +5858,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="266" spans="1:4">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>509</v>
       </c>
@@ -5852,7 +5872,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="267" spans="1:4">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>512</v>
       </c>
@@ -5866,7 +5886,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="268" spans="1:4">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>515</v>
       </c>
@@ -5880,7 +5900,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="269" spans="1:4">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>518</v>
       </c>
@@ -5894,7 +5914,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="270" spans="1:4">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>521</v>
       </c>
@@ -5908,7 +5928,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="271" spans="1:4">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>523</v>
       </c>
@@ -5922,7 +5942,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="272" spans="1:4">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>525</v>
       </c>
@@ -5936,7 +5956,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="273" spans="1:4">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>527</v>
       </c>
@@ -5950,7 +5970,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="274" spans="1:4">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>529</v>
       </c>
@@ -5964,7 +5984,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="275" spans="1:4">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>531</v>
       </c>
@@ -5978,7 +5998,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="276" spans="1:4">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>533</v>
       </c>
@@ -5992,7 +6012,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="277" spans="1:4">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>534</v>
       </c>
@@ -6006,7 +6026,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="278" spans="1:4">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>537</v>
       </c>
@@ -6014,7 +6034,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="18.75">
+    <row r="279" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A279" s="3" t="s">
         <v>838</v>
       </c>
@@ -6022,7 +6042,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="18.75">
+    <row r="280" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A280" s="3" t="s">
         <v>538</v>
       </c>
@@ -6030,7 +6050,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="18.75">
+    <row r="281" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A281" t="s">
         <v>540</v>
       </c>
@@ -6038,7 +6058,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="18.75">
+    <row r="282" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A282" t="s">
         <v>542</v>
       </c>
@@ -6046,7 +6066,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="18.75">
+    <row r="283" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A283" s="3" t="s">
         <v>544</v>
       </c>
@@ -6054,7 +6074,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="284" spans="1:4">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>546</v>
       </c>
@@ -6068,7 +6088,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="285" spans="1:4">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>549</v>
       </c>
@@ -6082,7 +6102,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="286" spans="1:4">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>552</v>
       </c>
@@ -6096,7 +6116,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="287" spans="1:4">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>555</v>
       </c>
@@ -6110,7 +6130,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="288" spans="1:4">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>558</v>
       </c>
@@ -6124,7 +6144,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="289" spans="1:4">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>561</v>
       </c>
@@ -6138,7 +6158,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="290" spans="1:4">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>563</v>
       </c>
@@ -6152,7 +6172,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="291" spans="1:4">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>566</v>
       </c>
@@ -6166,7 +6186,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="292" spans="1:4">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>569</v>
       </c>
@@ -6180,7 +6200,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="293" spans="1:4">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>572</v>
       </c>
@@ -6194,7 +6214,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="294" spans="1:4">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>575</v>
       </c>
@@ -6208,7 +6228,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="295" spans="1:4">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>578</v>
       </c>
@@ -6222,7 +6242,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="296" spans="1:4">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>581</v>
       </c>
@@ -6236,7 +6256,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="297" spans="1:4">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>584</v>
       </c>
@@ -6250,7 +6270,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="298" spans="1:4">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>587</v>
       </c>
@@ -6264,7 +6284,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="299" spans="1:4">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>589</v>
       </c>
@@ -6278,7 +6298,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="300" spans="1:4">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>591</v>
       </c>
@@ -6292,7 +6312,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="301" spans="1:4">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>594</v>
       </c>
@@ -6306,7 +6326,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="302" spans="1:4">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>596</v>
       </c>
@@ -6320,7 +6340,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="303" spans="1:4">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>599</v>
       </c>
@@ -6334,7 +6354,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="304" spans="1:4">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>602</v>
       </c>
@@ -6348,7 +6368,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="305" spans="1:4">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>605</v>
       </c>
@@ -6362,7 +6382,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="306" spans="1:4">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>608</v>
       </c>
@@ -6376,7 +6396,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="307" spans="1:4">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>611</v>
       </c>
@@ -6390,7 +6410,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="308" spans="1:4">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>613</v>
       </c>
@@ -6404,7 +6424,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="309" spans="1:4">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>616</v>
       </c>
@@ -6418,7 +6438,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="310" spans="1:4">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>619</v>
       </c>
@@ -6432,7 +6452,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="311" spans="1:4">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>622</v>
       </c>
@@ -6446,7 +6466,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="312" spans="1:4">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>624</v>
       </c>
@@ -6460,7 +6480,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="313" spans="1:4">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>626</v>
       </c>
@@ -6474,7 +6494,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="314" spans="1:4">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>629</v>
       </c>
@@ -6488,7 +6508,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="315" spans="1:4">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>632</v>
       </c>
@@ -6502,7 +6522,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="316" spans="1:4">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>634</v>
       </c>
@@ -6516,7 +6536,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="317" spans="1:4">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>636</v>
       </c>
@@ -6530,7 +6550,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="318" spans="1:4">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>639</v>
       </c>
@@ -6544,7 +6564,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="319" spans="1:4">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>642</v>
       </c>
@@ -6558,7 +6578,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="320" spans="1:4">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>644</v>
       </c>
@@ -6572,7 +6592,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="321" spans="1:4">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>647</v>
       </c>
@@ -6586,7 +6606,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="322" spans="1:4">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>650</v>
       </c>
@@ -6600,7 +6620,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="323" spans="1:4">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>653</v>
       </c>
@@ -6614,7 +6634,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="324" spans="1:4">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>655</v>
       </c>
@@ -6628,7 +6648,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="325" spans="1:4">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>658</v>
       </c>
@@ -6642,7 +6662,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="326" spans="1:4">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>661</v>
       </c>
@@ -6656,7 +6676,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="327" spans="1:4">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>663</v>
       </c>
@@ -6670,7 +6690,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="328" spans="1:4">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>665</v>
       </c>
@@ -6684,7 +6704,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="329" spans="1:4">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>668</v>
       </c>
@@ -6698,7 +6718,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="330" spans="1:4">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>670</v>
       </c>
@@ -6712,7 +6732,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="331" spans="1:4">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>673</v>
       </c>
@@ -6726,7 +6746,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="332" spans="1:4">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>675</v>
       </c>
@@ -6740,7 +6760,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="333" spans="1:4">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>677</v>
       </c>
@@ -6754,7 +6774,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="334" spans="1:4">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>679</v>
       </c>
@@ -6768,7 +6788,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="335" spans="1:4">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>681</v>
       </c>
@@ -6782,7 +6802,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="336" spans="1:4">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>683</v>
       </c>
@@ -6796,7 +6816,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="337" spans="1:4">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>686</v>
       </c>
@@ -6810,7 +6830,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="338" spans="1:4">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>688</v>
       </c>
@@ -6824,7 +6844,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="339" spans="1:4">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>690</v>
       </c>
@@ -6838,7 +6858,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="340" spans="1:4">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>693</v>
       </c>
@@ -6852,7 +6872,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="341" spans="1:4">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>696</v>
       </c>
@@ -6866,7 +6886,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="342" spans="1:4">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>699</v>
       </c>
@@ -6880,7 +6900,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="343" spans="1:4">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>702</v>
       </c>
@@ -6894,7 +6914,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="344" spans="1:4">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>703</v>
       </c>
@@ -6908,7 +6928,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="345" spans="1:4">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>705</v>
       </c>
@@ -6922,7 +6942,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="346" spans="1:4">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>707</v>
       </c>
@@ -6936,7 +6956,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="347" spans="1:4">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>709</v>
       </c>
@@ -6950,7 +6970,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="348" spans="1:4">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>710</v>
       </c>
@@ -6964,7 +6984,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="349" spans="1:4">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>712</v>
       </c>
@@ -6978,7 +6998,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="350" spans="1:4">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>714</v>
       </c>
@@ -6992,7 +7012,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="351" spans="1:4">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>716</v>
       </c>
@@ -7006,7 +7026,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="352" spans="1:4" ht="18.75">
+    <row r="352" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A352" s="3" t="s">
         <v>718</v>
       </c>
@@ -7014,7 +7034,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="353" spans="1:4">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>720</v>
       </c>
@@ -7028,7 +7048,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="354" spans="1:4">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>723</v>
       </c>
@@ -7042,7 +7062,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="355" spans="1:4">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>726</v>
       </c>
@@ -7056,7 +7076,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="356" spans="1:4">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>729</v>
       </c>
@@ -7070,7 +7090,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="357" spans="1:4">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>732</v>
       </c>
@@ -7084,7 +7104,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="358" spans="1:4">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>735</v>
       </c>
@@ -7098,7 +7118,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="359" spans="1:4">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>738</v>
       </c>
@@ -7112,7 +7132,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="360" spans="1:4">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>741</v>
       </c>
@@ -7126,7 +7146,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="361" spans="1:4">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>744</v>
       </c>
@@ -7140,7 +7160,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="362" spans="1:4">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>747</v>
       </c>
@@ -7154,7 +7174,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="363" spans="1:4">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>749</v>
       </c>
@@ -7168,7 +7188,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="364" spans="1:4">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>751</v>
       </c>
@@ -7182,7 +7202,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="365" spans="1:4">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>753</v>
       </c>
@@ -7196,7 +7216,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="366" spans="1:4">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>756</v>
       </c>
@@ -7210,7 +7230,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="367" spans="1:4">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>759</v>
       </c>
@@ -7224,7 +7244,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="368" spans="1:4">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>762</v>
       </c>
@@ -7238,7 +7258,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="369" spans="1:4">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>765</v>
       </c>
@@ -7252,7 +7272,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="370" spans="1:4">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>768</v>
       </c>
@@ -7266,7 +7286,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="371" spans="1:4">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>771</v>
       </c>
@@ -7280,7 +7300,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="372" spans="1:4">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>774</v>
       </c>
@@ -7294,7 +7314,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="373" spans="1:4">
+    <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>776</v>
       </c>
@@ -7308,7 +7328,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="374" spans="1:4">
+    <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>778</v>
       </c>
@@ -7322,7 +7342,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="375" spans="1:4">
+    <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>780</v>
       </c>
@@ -7336,7 +7356,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="376" spans="1:4">
+    <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>782</v>
       </c>
@@ -7350,7 +7370,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="377" spans="1:4">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>784</v>
       </c>
@@ -7364,7 +7384,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="378" spans="1:4">
+    <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>786</v>
       </c>
@@ -7378,7 +7398,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="379" spans="1:4">
+    <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>788</v>
       </c>
@@ -7392,7 +7412,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="380" spans="1:4">
+    <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>790</v>
       </c>
@@ -7406,7 +7426,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="381" spans="1:4">
+    <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>793</v>
       </c>
@@ -7420,7 +7440,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="382" spans="1:4">
+    <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>796</v>
       </c>
@@ -7434,7 +7454,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="383" spans="1:4">
+    <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>799</v>
       </c>
@@ -7448,7 +7468,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="384" spans="1:4">
+    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>802</v>
       </c>
@@ -7462,7 +7482,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="385" spans="1:4">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>805</v>
       </c>
@@ -7476,7 +7496,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="386" spans="1:4">
+    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>807</v>
       </c>
@@ -7490,7 +7510,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="387" spans="1:4">
+    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>810</v>
       </c>
@@ -7504,7 +7524,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="388" spans="1:4">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>813</v>
       </c>
@@ -7518,7 +7538,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="389" spans="1:4">
+    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>816</v>
       </c>
@@ -7532,7 +7552,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="390" spans="1:4">
+    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>819</v>
       </c>
@@ -7546,7 +7566,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="391" spans="1:4">
+    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>822</v>
       </c>
@@ -7560,7 +7580,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="392" spans="1:4">
+    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>825</v>
       </c>
@@ -7574,7 +7594,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="393" spans="1:4">
+    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>828</v>
       </c>
@@ -7588,7 +7608,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="394" spans="1:4">
+    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>830</v>
       </c>
@@ -7602,7 +7622,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="395" spans="1:4">
+    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>833</v>
       </c>
@@ -7616,7 +7636,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="396" spans="1:4">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>836</v>
       </c>
@@ -7630,7 +7650,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="397" spans="1:4" ht="18.75">
+    <row r="397" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A397" s="3" t="s">
         <v>839</v>
       </c>
@@ -7638,7 +7658,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="398" spans="1:4" ht="18.75">
+    <row r="398" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A398" s="3" t="s">
         <v>841</v>
       </c>
@@ -7646,7 +7666,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="399" spans="1:4" ht="18.75">
+    <row r="399" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A399" s="3" t="s">
         <v>843</v>
       </c>
@@ -7654,7 +7674,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="400" spans="1:4" ht="18.75">
+    <row r="400" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A400" s="3" t="s">
         <v>845</v>
       </c>
@@ -7662,7 +7682,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="401" spans="1:4" ht="18.75">
+    <row r="401" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A401" s="3" t="s">
         <v>847</v>
       </c>
@@ -7670,7 +7690,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="402" spans="1:4" ht="18.75">
+    <row r="402" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A402" s="3" t="s">
         <v>849</v>
       </c>
@@ -7678,7 +7698,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="403" spans="1:4">
+    <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>851</v>
       </c>
@@ -7692,7 +7712,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="404" spans="1:4">
+    <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>853</v>
       </c>
@@ -7706,7 +7726,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="405" spans="1:4">
+    <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>855</v>
       </c>
@@ -7720,7 +7740,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="406" spans="1:4">
+    <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>858</v>
       </c>
@@ -7734,7 +7754,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="407" spans="1:4">
+    <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>861</v>
       </c>
@@ -7748,7 +7768,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="408" spans="1:4">
+    <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>863</v>
       </c>
@@ -7762,7 +7782,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="409" spans="1:4">
+    <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>866</v>
       </c>
@@ -7776,7 +7796,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="410" spans="1:4">
+    <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>869</v>
       </c>
@@ -7790,7 +7810,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="411" spans="1:4">
+    <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>872</v>
       </c>
@@ -7804,7 +7824,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="412" spans="1:4">
+    <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>875</v>
       </c>
@@ -7818,7 +7838,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="413" spans="1:4">
+    <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>878</v>
       </c>
@@ -7832,7 +7852,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="414" spans="1:4">
+    <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>880</v>
       </c>
@@ -7846,7 +7866,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="415" spans="1:4">
+    <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>882</v>
       </c>
@@ -7860,7 +7880,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="416" spans="1:4">
+    <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>885</v>
       </c>
@@ -7874,7 +7894,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="417" spans="1:4">
+    <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>888</v>
       </c>
@@ -7888,7 +7908,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="418" spans="1:4">
+    <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>892</v>
       </c>
@@ -7902,7 +7922,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="419" spans="1:4">
+    <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>895</v>
       </c>
@@ -7916,7 +7936,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="420" spans="1:4">
+    <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>898</v>
       </c>
@@ -7930,7 +7950,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="421" spans="1:4">
+    <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>901</v>
       </c>
@@ -7944,7 +7964,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="422" spans="1:4">
+    <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>904</v>
       </c>
@@ -7958,7 +7978,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="423" spans="1:4">
+    <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>906</v>
       </c>
@@ -7972,7 +7992,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="424" spans="1:4">
+    <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>909</v>
       </c>
@@ -7986,7 +8006,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="425" spans="1:4">
+    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>912</v>
       </c>
@@ -8000,7 +8020,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="426" spans="1:4">
+    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>914</v>
       </c>
@@ -8008,7 +8028,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="427" spans="1:4">
+    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>916</v>
       </c>
@@ -8016,7 +8036,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="428" spans="1:4">
+    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>918</v>
       </c>
@@ -8024,12 +8044,36 @@
         <v>919</v>
       </c>
     </row>
-    <row r="429" spans="1:4">
+    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>920</v>
       </c>
       <c r="B429" t="s">
         <v>920</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A430" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="B430" s="3" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A431" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="B431" s="3" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A432" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="B432" s="3" t="s">
+        <v>925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update non_verbs.xlsx with modified content
</commit_message>
<xml_diff>
--- a/non_verbs.xlsx
+++ b/non_verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45DE2F5-A9CF-4566-A43C-B095AF8BA269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE5F637-3AF8-4D31-95D8-1AFB8B47FD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="925">
   <si>
     <t>Kanji</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1104,9 +1104,6 @@
   </si>
   <si>
     <t>パン</t>
-  </si>
-  <si>
-    <t>pão〔葡〕</t>
   </si>
   <si>
     <t>料理</t>
@@ -3262,8 +3259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
   <dimension ref="A1:F432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
-      <selection activeCell="B432" sqref="B432"/>
+    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4708,7 +4705,7 @@
     </row>
     <row r="155" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B155" t="s">
         <v>270</v>
@@ -5071,3009 +5068,3009 @@
         <v>352</v>
       </c>
       <c r="B200" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
+        <v>353</v>
+      </c>
+      <c r="B201" t="s">
         <v>354</v>
-      </c>
-      <c r="B201" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
+        <v>355</v>
+      </c>
+      <c r="B202" t="s">
         <v>356</v>
-      </c>
-      <c r="B202" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>357</v>
+      </c>
+      <c r="B203" t="s">
         <v>358</v>
-      </c>
-      <c r="B203" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
+        <v>359</v>
+      </c>
+      <c r="B204" t="s">
         <v>360</v>
-      </c>
-      <c r="B204" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>361</v>
+      </c>
+      <c r="B205" t="s">
         <v>362</v>
-      </c>
-      <c r="B205" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>363</v>
+      </c>
+      <c r="B206" t="s">
         <v>364</v>
-      </c>
-      <c r="B206" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
+        <v>365</v>
+      </c>
+      <c r="B207" t="s">
         <v>366</v>
-      </c>
-      <c r="B207" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>367</v>
+      </c>
+      <c r="B208" t="s">
         <v>368</v>
-      </c>
-      <c r="B208" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
+        <v>369</v>
+      </c>
+      <c r="B209" t="s">
         <v>370</v>
-      </c>
-      <c r="B209" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
+        <v>371</v>
+      </c>
+      <c r="B210" t="s">
         <v>372</v>
-      </c>
-      <c r="B210" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B211" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
+        <v>374</v>
+      </c>
+      <c r="B212" t="s">
         <v>375</v>
-      </c>
-      <c r="B212" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
+        <v>376</v>
+      </c>
+      <c r="B213" t="s">
         <v>377</v>
-      </c>
-      <c r="B213" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
+        <v>378</v>
+      </c>
+      <c r="B214" t="s">
         <v>379</v>
-      </c>
-      <c r="B214" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>380</v>
+      </c>
+      <c r="B215" t="s">
         <v>381</v>
-      </c>
-      <c r="B215" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
+        <v>382</v>
+      </c>
+      <c r="B216" t="s">
         <v>383</v>
-      </c>
-      <c r="B216" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
+        <v>384</v>
+      </c>
+      <c r="B217" t="s">
         <v>385</v>
-      </c>
-      <c r="B217" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>386</v>
+      </c>
+      <c r="B218" t="s">
         <v>387</v>
-      </c>
-      <c r="B218" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B219" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B220" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B221" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
+        <v>391</v>
+      </c>
+      <c r="B222" t="s">
         <v>392</v>
       </c>
-      <c r="B222" t="s">
+      <c r="C222" t="s">
         <v>393</v>
       </c>
-      <c r="C222" t="s">
+      <c r="D222" t="s">
         <v>394</v>
-      </c>
-      <c r="D222" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
+        <v>395</v>
+      </c>
+      <c r="B223" t="s">
         <v>396</v>
       </c>
-      <c r="B223" t="s">
+      <c r="C223" t="s">
         <v>397</v>
       </c>
-      <c r="C223" t="s">
+      <c r="D223" t="s">
         <v>398</v>
-      </c>
-      <c r="D223" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>399</v>
+      </c>
+      <c r="B224" t="s">
         <v>400</v>
       </c>
-      <c r="B224" t="s">
-        <v>401</v>
-      </c>
       <c r="C224" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D224" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
+        <v>401</v>
+      </c>
+      <c r="B225" t="s">
         <v>402</v>
       </c>
-      <c r="B225" t="s">
+      <c r="C225" t="s">
+        <v>393</v>
+      </c>
+      <c r="D225" t="s">
         <v>403</v>
-      </c>
-      <c r="C225" t="s">
-        <v>394</v>
-      </c>
-      <c r="D225" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
+        <v>404</v>
+      </c>
+      <c r="B226" t="s">
         <v>405</v>
       </c>
-      <c r="B226" t="s">
+      <c r="C226" t="s">
+        <v>393</v>
+      </c>
+      <c r="D226" t="s">
         <v>406</v>
-      </c>
-      <c r="C226" t="s">
-        <v>394</v>
-      </c>
-      <c r="D226" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
+        <v>407</v>
+      </c>
+      <c r="B227" t="s">
         <v>408</v>
       </c>
-      <c r="B227" t="s">
+      <c r="C227" t="s">
+        <v>393</v>
+      </c>
+      <c r="D227" t="s">
         <v>409</v>
-      </c>
-      <c r="C227" t="s">
-        <v>394</v>
-      </c>
-      <c r="D227" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
+        <v>410</v>
+      </c>
+      <c r="B228" t="s">
+        <v>410</v>
+      </c>
+      <c r="C228" t="s">
         <v>411</v>
       </c>
-      <c r="B228" t="s">
-        <v>411</v>
-      </c>
-      <c r="C228" t="s">
+      <c r="D228" t="s">
         <v>412</v>
-      </c>
-      <c r="D228" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
+        <v>413</v>
+      </c>
+      <c r="B229" t="s">
+        <v>413</v>
+      </c>
+      <c r="C229" t="s">
+        <v>411</v>
+      </c>
+      <c r="D229" t="s">
         <v>414</v>
-      </c>
-      <c r="B229" t="s">
-        <v>414</v>
-      </c>
-      <c r="C229" t="s">
-        <v>412</v>
-      </c>
-      <c r="D229" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
+        <v>415</v>
+      </c>
+      <c r="B230" t="s">
+        <v>415</v>
+      </c>
+      <c r="C230" t="s">
+        <v>393</v>
+      </c>
+      <c r="D230" t="s">
         <v>416</v>
-      </c>
-      <c r="B230" t="s">
-        <v>416</v>
-      </c>
-      <c r="C230" t="s">
-        <v>394</v>
-      </c>
-      <c r="D230" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
+        <v>417</v>
+      </c>
+      <c r="B231" t="s">
+        <v>417</v>
+      </c>
+      <c r="C231" t="s">
+        <v>393</v>
+      </c>
+      <c r="D231" t="s">
         <v>418</v>
-      </c>
-      <c r="B231" t="s">
-        <v>418</v>
-      </c>
-      <c r="C231" t="s">
-        <v>394</v>
-      </c>
-      <c r="D231" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
+        <v>419</v>
+      </c>
+      <c r="B232" t="s">
+        <v>419</v>
+      </c>
+      <c r="C232" t="s">
+        <v>411</v>
+      </c>
+      <c r="D232" t="s">
         <v>420</v>
-      </c>
-      <c r="B232" t="s">
-        <v>420</v>
-      </c>
-      <c r="C232" t="s">
-        <v>412</v>
-      </c>
-      <c r="D232" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
+        <v>421</v>
+      </c>
+      <c r="B233" t="s">
+        <v>421</v>
+      </c>
+      <c r="C233" t="s">
         <v>422</v>
       </c>
-      <c r="B233" t="s">
-        <v>422</v>
-      </c>
-      <c r="C233" t="s">
+      <c r="D233" t="s">
         <v>423</v>
-      </c>
-      <c r="D233" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
+        <v>424</v>
+      </c>
+      <c r="B234" t="s">
+        <v>424</v>
+      </c>
+      <c r="C234" t="s">
         <v>425</v>
       </c>
-      <c r="B234" t="s">
-        <v>425</v>
-      </c>
-      <c r="C234" t="s">
+      <c r="D234" t="s">
         <v>426</v>
-      </c>
-      <c r="D234" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
+        <v>427</v>
+      </c>
+      <c r="B235" t="s">
+        <v>427</v>
+      </c>
+      <c r="C235" t="s">
+        <v>422</v>
+      </c>
+      <c r="D235" t="s">
         <v>428</v>
-      </c>
-      <c r="B235" t="s">
-        <v>428</v>
-      </c>
-      <c r="C235" t="s">
-        <v>423</v>
-      </c>
-      <c r="D235" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
+        <v>429</v>
+      </c>
+      <c r="B236" t="s">
         <v>430</v>
       </c>
-      <c r="B236" t="s">
+      <c r="C236" t="s">
         <v>431</v>
       </c>
-      <c r="C236" t="s">
+      <c r="D236" t="s">
         <v>432</v>
-      </c>
-      <c r="D236" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
+        <v>433</v>
+      </c>
+      <c r="B237" t="s">
+        <v>433</v>
+      </c>
+      <c r="C237" t="s">
+        <v>397</v>
+      </c>
+      <c r="D237" t="s">
         <v>434</v>
-      </c>
-      <c r="B237" t="s">
-        <v>434</v>
-      </c>
-      <c r="C237" t="s">
-        <v>398</v>
-      </c>
-      <c r="D237" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
+        <v>435</v>
+      </c>
+      <c r="B238" t="s">
         <v>436</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238" t="s">
+        <v>397</v>
+      </c>
+      <c r="D238" t="s">
         <v>437</v>
-      </c>
-      <c r="C238" t="s">
-        <v>398</v>
-      </c>
-      <c r="D238" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
+        <v>438</v>
+      </c>
+      <c r="B239" t="s">
         <v>439</v>
       </c>
-      <c r="B239" t="s">
+      <c r="C239" t="s">
+        <v>397</v>
+      </c>
+      <c r="D239" t="s">
         <v>440</v>
-      </c>
-      <c r="C239" t="s">
-        <v>398</v>
-      </c>
-      <c r="D239" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
+        <v>441</v>
+      </c>
+      <c r="B240" t="s">
+        <v>441</v>
+      </c>
+      <c r="C240" t="s">
         <v>442</v>
       </c>
-      <c r="B240" t="s">
-        <v>442</v>
-      </c>
-      <c r="C240" t="s">
+      <c r="D240" t="s">
         <v>443</v>
-      </c>
-      <c r="D240" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
+        <v>444</v>
+      </c>
+      <c r="B241" t="s">
         <v>445</v>
       </c>
-      <c r="B241" t="s">
+      <c r="C241" t="s">
         <v>446</v>
       </c>
-      <c r="C241" t="s">
+      <c r="D241" t="s">
         <v>447</v>
-      </c>
-      <c r="D241" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
+        <v>448</v>
+      </c>
+      <c r="B242" t="s">
         <v>449</v>
       </c>
-      <c r="B242" t="s">
+      <c r="C242" t="s">
+        <v>411</v>
+      </c>
+      <c r="D242" t="s">
         <v>450</v>
-      </c>
-      <c r="C242" t="s">
-        <v>412</v>
-      </c>
-      <c r="D242" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
+        <v>451</v>
+      </c>
+      <c r="B243" t="s">
         <v>452</v>
       </c>
-      <c r="B243" t="s">
-        <v>453</v>
-      </c>
       <c r="C243" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D243" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
+        <v>453</v>
+      </c>
+      <c r="B244" t="s">
         <v>454</v>
       </c>
-      <c r="B244" t="s">
+      <c r="C244" t="s">
+        <v>431</v>
+      </c>
+      <c r="D244" t="s">
         <v>455</v>
-      </c>
-      <c r="C244" t="s">
-        <v>432</v>
-      </c>
-      <c r="D244" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
+        <v>456</v>
+      </c>
+      <c r="B245" t="s">
         <v>457</v>
       </c>
-      <c r="B245" t="s">
+      <c r="C245" t="s">
+        <v>431</v>
+      </c>
+      <c r="D245" t="s">
         <v>458</v>
-      </c>
-      <c r="C245" t="s">
-        <v>432</v>
-      </c>
-      <c r="D245" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
+        <v>459</v>
+      </c>
+      <c r="B246" t="s">
         <v>460</v>
       </c>
-      <c r="B246" t="s">
+      <c r="C246" t="s">
         <v>461</v>
       </c>
-      <c r="C246" t="s">
+      <c r="D246" t="s">
         <v>462</v>
-      </c>
-      <c r="D246" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
+        <v>463</v>
+      </c>
+      <c r="B247" t="s">
         <v>464</v>
       </c>
-      <c r="B247" t="s">
+      <c r="C247" t="s">
+        <v>393</v>
+      </c>
+      <c r="D247" t="s">
         <v>465</v>
-      </c>
-      <c r="C247" t="s">
-        <v>394</v>
-      </c>
-      <c r="D247" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
+        <v>466</v>
+      </c>
+      <c r="B248" t="s">
         <v>467</v>
       </c>
-      <c r="B248" t="s">
+      <c r="C248" t="s">
+        <v>393</v>
+      </c>
+      <c r="D248" t="s">
         <v>468</v>
-      </c>
-      <c r="C248" t="s">
-        <v>394</v>
-      </c>
-      <c r="D248" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
+        <v>469</v>
+      </c>
+      <c r="B249" t="s">
+        <v>469</v>
+      </c>
+      <c r="C249" t="s">
+        <v>411</v>
+      </c>
+      <c r="D249" t="s">
         <v>470</v>
-      </c>
-      <c r="B249" t="s">
-        <v>470</v>
-      </c>
-      <c r="C249" t="s">
-        <v>412</v>
-      </c>
-      <c r="D249" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
+        <v>471</v>
+      </c>
+      <c r="B250" t="s">
+        <v>471</v>
+      </c>
+      <c r="C250" t="s">
+        <v>411</v>
+      </c>
+      <c r="D250" t="s">
         <v>472</v>
-      </c>
-      <c r="B250" t="s">
-        <v>472</v>
-      </c>
-      <c r="C250" t="s">
-        <v>412</v>
-      </c>
-      <c r="D250" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
+        <v>473</v>
+      </c>
+      <c r="B251" t="s">
+        <v>473</v>
+      </c>
+      <c r="C251" t="s">
+        <v>411</v>
+      </c>
+      <c r="D251" t="s">
         <v>474</v>
-      </c>
-      <c r="B251" t="s">
-        <v>474</v>
-      </c>
-      <c r="C251" t="s">
-        <v>412</v>
-      </c>
-      <c r="D251" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
+        <v>475</v>
+      </c>
+      <c r="B252" t="s">
+        <v>475</v>
+      </c>
+      <c r="C252" t="s">
+        <v>411</v>
+      </c>
+      <c r="D252" t="s">
         <v>476</v>
-      </c>
-      <c r="B252" t="s">
-        <v>476</v>
-      </c>
-      <c r="C252" t="s">
-        <v>412</v>
-      </c>
-      <c r="D252" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>477</v>
+      </c>
+      <c r="B253" t="s">
+        <v>477</v>
+      </c>
+      <c r="C253" t="s">
+        <v>393</v>
+      </c>
+      <c r="D253" t="s">
         <v>478</v>
-      </c>
-      <c r="B253" t="s">
-        <v>478</v>
-      </c>
-      <c r="C253" t="s">
-        <v>394</v>
-      </c>
-      <c r="D253" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
+        <v>479</v>
+      </c>
+      <c r="B254" t="s">
+        <v>479</v>
+      </c>
+      <c r="C254" t="s">
+        <v>393</v>
+      </c>
+      <c r="D254" t="s">
         <v>480</v>
-      </c>
-      <c r="B254" t="s">
-        <v>480</v>
-      </c>
-      <c r="C254" t="s">
-        <v>394</v>
-      </c>
-      <c r="D254" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
+        <v>481</v>
+      </c>
+      <c r="B255" t="s">
         <v>482</v>
       </c>
-      <c r="B255" t="s">
-        <v>483</v>
-      </c>
       <c r="C255" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D255" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
+        <v>483</v>
+      </c>
+      <c r="B256" t="s">
         <v>484</v>
       </c>
-      <c r="B256" t="s">
+      <c r="C256" t="s">
+        <v>393</v>
+      </c>
+      <c r="D256" t="s">
         <v>485</v>
-      </c>
-      <c r="C256" t="s">
-        <v>394</v>
-      </c>
-      <c r="D256" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
+        <v>486</v>
+      </c>
+      <c r="B257" t="s">
         <v>487</v>
       </c>
-      <c r="B257" t="s">
+      <c r="C257" t="s">
+        <v>411</v>
+      </c>
+      <c r="D257" t="s">
         <v>488</v>
-      </c>
-      <c r="C257" t="s">
-        <v>412</v>
-      </c>
-      <c r="D257" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
+        <v>489</v>
+      </c>
+      <c r="B258" t="s">
         <v>490</v>
       </c>
-      <c r="B258" t="s">
+      <c r="C258" t="s">
+        <v>442</v>
+      </c>
+      <c r="D258" t="s">
         <v>491</v>
-      </c>
-      <c r="C258" t="s">
-        <v>443</v>
-      </c>
-      <c r="D258" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
+        <v>492</v>
+      </c>
+      <c r="B259" t="s">
         <v>493</v>
       </c>
-      <c r="B259" t="s">
-        <v>494</v>
-      </c>
       <c r="C259" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D259" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
+        <v>494</v>
+      </c>
+      <c r="B260" t="s">
         <v>495</v>
       </c>
-      <c r="B260" t="s">
+      <c r="C260" t="s">
+        <v>393</v>
+      </c>
+      <c r="D260" t="s">
         <v>496</v>
-      </c>
-      <c r="C260" t="s">
-        <v>394</v>
-      </c>
-      <c r="D260" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
+        <v>497</v>
+      </c>
+      <c r="B261" t="s">
         <v>498</v>
       </c>
-      <c r="B261" t="s">
+      <c r="C261" t="s">
+        <v>393</v>
+      </c>
+      <c r="D261" t="s">
         <v>499</v>
-      </c>
-      <c r="C261" t="s">
-        <v>394</v>
-      </c>
-      <c r="D261" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
+        <v>500</v>
+      </c>
+      <c r="B262" t="s">
         <v>501</v>
       </c>
-      <c r="B262" t="s">
-        <v>502</v>
-      </c>
       <c r="C262" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D262" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
+        <v>502</v>
+      </c>
+      <c r="B263" t="s">
+        <v>502</v>
+      </c>
+      <c r="C263" t="s">
+        <v>446</v>
+      </c>
+      <c r="D263" t="s">
         <v>503</v>
-      </c>
-      <c r="B263" t="s">
-        <v>503</v>
-      </c>
-      <c r="C263" t="s">
-        <v>447</v>
-      </c>
-      <c r="D263" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
+        <v>504</v>
+      </c>
+      <c r="B264" t="s">
+        <v>504</v>
+      </c>
+      <c r="C264" t="s">
+        <v>431</v>
+      </c>
+      <c r="D264" t="s">
         <v>505</v>
-      </c>
-      <c r="B264" t="s">
-        <v>505</v>
-      </c>
-      <c r="C264" t="s">
-        <v>432</v>
-      </c>
-      <c r="D264" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
+        <v>506</v>
+      </c>
+      <c r="B265" t="s">
         <v>507</v>
       </c>
-      <c r="B265" t="s">
-        <v>508</v>
-      </c>
       <c r="C265" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D265" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
+        <v>508</v>
+      </c>
+      <c r="B266" t="s">
         <v>509</v>
       </c>
-      <c r="B266" t="s">
+      <c r="C266" t="s">
+        <v>393</v>
+      </c>
+      <c r="D266" t="s">
         <v>510</v>
-      </c>
-      <c r="C266" t="s">
-        <v>394</v>
-      </c>
-      <c r="D266" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
+        <v>511</v>
+      </c>
+      <c r="B267" t="s">
         <v>512</v>
       </c>
-      <c r="B267" t="s">
+      <c r="C267" t="s">
+        <v>393</v>
+      </c>
+      <c r="D267" t="s">
         <v>513</v>
-      </c>
-      <c r="C267" t="s">
-        <v>394</v>
-      </c>
-      <c r="D267" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
+        <v>514</v>
+      </c>
+      <c r="B268" t="s">
         <v>515</v>
       </c>
-      <c r="B268" t="s">
+      <c r="C268" t="s">
+        <v>431</v>
+      </c>
+      <c r="D268" t="s">
         <v>516</v>
-      </c>
-      <c r="C268" t="s">
-        <v>432</v>
-      </c>
-      <c r="D268" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
+        <v>517</v>
+      </c>
+      <c r="B269" t="s">
         <v>518</v>
       </c>
-      <c r="B269" t="s">
+      <c r="C269" t="s">
+        <v>446</v>
+      </c>
+      <c r="D269" t="s">
         <v>519</v>
-      </c>
-      <c r="C269" t="s">
-        <v>447</v>
-      </c>
-      <c r="D269" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
+        <v>520</v>
+      </c>
+      <c r="B270" t="s">
+        <v>520</v>
+      </c>
+      <c r="C270" t="s">
+        <v>411</v>
+      </c>
+      <c r="D270" t="s">
         <v>521</v>
-      </c>
-      <c r="B270" t="s">
-        <v>521</v>
-      </c>
-      <c r="C270" t="s">
-        <v>412</v>
-      </c>
-      <c r="D270" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
+        <v>522</v>
+      </c>
+      <c r="B271" t="s">
+        <v>522</v>
+      </c>
+      <c r="C271" t="s">
+        <v>411</v>
+      </c>
+      <c r="D271" t="s">
         <v>523</v>
-      </c>
-      <c r="B271" t="s">
-        <v>523</v>
-      </c>
-      <c r="C271" t="s">
-        <v>412</v>
-      </c>
-      <c r="D271" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
+        <v>524</v>
+      </c>
+      <c r="B272" t="s">
+        <v>524</v>
+      </c>
+      <c r="C272" t="s">
+        <v>411</v>
+      </c>
+      <c r="D272" t="s">
         <v>525</v>
-      </c>
-      <c r="B272" t="s">
-        <v>525</v>
-      </c>
-      <c r="C272" t="s">
-        <v>412</v>
-      </c>
-      <c r="D272" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>526</v>
+      </c>
+      <c r="B273" t="s">
+        <v>526</v>
+      </c>
+      <c r="C273" t="s">
+        <v>393</v>
+      </c>
+      <c r="D273" t="s">
         <v>527</v>
-      </c>
-      <c r="B273" t="s">
-        <v>527</v>
-      </c>
-      <c r="C273" t="s">
-        <v>394</v>
-      </c>
-      <c r="D273" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
+        <v>528</v>
+      </c>
+      <c r="B274" t="s">
+        <v>528</v>
+      </c>
+      <c r="C274" t="s">
+        <v>393</v>
+      </c>
+      <c r="D274" t="s">
         <v>529</v>
-      </c>
-      <c r="B274" t="s">
-        <v>529</v>
-      </c>
-      <c r="C274" t="s">
-        <v>394</v>
-      </c>
-      <c r="D274" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
+        <v>530</v>
+      </c>
+      <c r="B275" t="s">
+        <v>530</v>
+      </c>
+      <c r="C275" t="s">
+        <v>431</v>
+      </c>
+      <c r="D275" t="s">
         <v>531</v>
-      </c>
-      <c r="B275" t="s">
-        <v>531</v>
-      </c>
-      <c r="C275" t="s">
-        <v>432</v>
-      </c>
-      <c r="D275" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B276" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C276" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D276" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
+        <v>533</v>
+      </c>
+      <c r="B277" t="s">
+        <v>533</v>
+      </c>
+      <c r="C277" t="s">
         <v>534</v>
       </c>
-      <c r="B277" t="s">
-        <v>534</v>
-      </c>
-      <c r="C277" t="s">
+      <c r="D277" t="s">
         <v>535</v>
-      </c>
-      <c r="D277" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B278" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A279" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A280" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B280" s="3" t="s">
         <v>538</v>
-      </c>
-      <c r="B280" s="3" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A281" t="s">
+        <v>539</v>
+      </c>
+      <c r="B281" s="3" t="s">
         <v>540</v>
-      </c>
-      <c r="B281" s="3" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A282" t="s">
+        <v>541</v>
+      </c>
+      <c r="B282" s="3" t="s">
         <v>542</v>
-      </c>
-      <c r="B282" s="3" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A283" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="B283" s="3" t="s">
         <v>544</v>
-      </c>
-      <c r="B283" s="3" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
+        <v>545</v>
+      </c>
+      <c r="B284" t="s">
         <v>546</v>
       </c>
-      <c r="B284" t="s">
+      <c r="C284" t="s">
+        <v>411</v>
+      </c>
+      <c r="D284" t="s">
         <v>547</v>
-      </c>
-      <c r="C284" t="s">
-        <v>412</v>
-      </c>
-      <c r="D284" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
+        <v>548</v>
+      </c>
+      <c r="B285" t="s">
         <v>549</v>
       </c>
-      <c r="B285" t="s">
+      <c r="C285" t="s">
+        <v>393</v>
+      </c>
+      <c r="D285" t="s">
         <v>550</v>
-      </c>
-      <c r="C285" t="s">
-        <v>394</v>
-      </c>
-      <c r="D285" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
+        <v>551</v>
+      </c>
+      <c r="B286" t="s">
         <v>552</v>
       </c>
-      <c r="B286" t="s">
+      <c r="C286" t="s">
+        <v>411</v>
+      </c>
+      <c r="D286" t="s">
         <v>553</v>
-      </c>
-      <c r="C286" t="s">
-        <v>412</v>
-      </c>
-      <c r="D286" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
+        <v>554</v>
+      </c>
+      <c r="B287" t="s">
         <v>555</v>
       </c>
-      <c r="B287" t="s">
+      <c r="C287" t="s">
+        <v>393</v>
+      </c>
+      <c r="D287" t="s">
         <v>556</v>
-      </c>
-      <c r="C287" t="s">
-        <v>394</v>
-      </c>
-      <c r="D287" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
+        <v>557</v>
+      </c>
+      <c r="B288" t="s">
         <v>558</v>
       </c>
-      <c r="B288" t="s">
+      <c r="C288" t="s">
+        <v>397</v>
+      </c>
+      <c r="D288" t="s">
         <v>559</v>
-      </c>
-      <c r="C288" t="s">
-        <v>398</v>
-      </c>
-      <c r="D288" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
+        <v>560</v>
+      </c>
+      <c r="B289" t="s">
         <v>561</v>
       </c>
-      <c r="B289" t="s">
-        <v>562</v>
-      </c>
       <c r="C289" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D289" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
+        <v>562</v>
+      </c>
+      <c r="B290" t="s">
         <v>563</v>
       </c>
-      <c r="B290" t="s">
+      <c r="C290" t="s">
+        <v>393</v>
+      </c>
+      <c r="D290" t="s">
         <v>564</v>
-      </c>
-      <c r="C290" t="s">
-        <v>394</v>
-      </c>
-      <c r="D290" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
+        <v>565</v>
+      </c>
+      <c r="B291" t="s">
         <v>566</v>
       </c>
-      <c r="B291" t="s">
+      <c r="C291" t="s">
+        <v>393</v>
+      </c>
+      <c r="D291" t="s">
         <v>567</v>
-      </c>
-      <c r="C291" t="s">
-        <v>394</v>
-      </c>
-      <c r="D291" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
+        <v>568</v>
+      </c>
+      <c r="B292" t="s">
         <v>569</v>
       </c>
-      <c r="B292" t="s">
+      <c r="C292" t="s">
+        <v>431</v>
+      </c>
+      <c r="D292" t="s">
         <v>570</v>
-      </c>
-      <c r="C292" t="s">
-        <v>432</v>
-      </c>
-      <c r="D292" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
+        <v>571</v>
+      </c>
+      <c r="B293" t="s">
         <v>572</v>
       </c>
-      <c r="B293" t="s">
+      <c r="C293" t="s">
+        <v>397</v>
+      </c>
+      <c r="D293" t="s">
         <v>573</v>
-      </c>
-      <c r="C293" t="s">
-        <v>398</v>
-      </c>
-      <c r="D293" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
+        <v>574</v>
+      </c>
+      <c r="B294" t="s">
         <v>575</v>
       </c>
-      <c r="B294" t="s">
+      <c r="C294" t="s">
+        <v>393</v>
+      </c>
+      <c r="D294" t="s">
         <v>576</v>
-      </c>
-      <c r="C294" t="s">
-        <v>394</v>
-      </c>
-      <c r="D294" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
+        <v>577</v>
+      </c>
+      <c r="B295" t="s">
         <v>578</v>
       </c>
-      <c r="B295" t="s">
+      <c r="C295" t="s">
+        <v>411</v>
+      </c>
+      <c r="D295" t="s">
         <v>579</v>
-      </c>
-      <c r="C295" t="s">
-        <v>412</v>
-      </c>
-      <c r="D295" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
+        <v>580</v>
+      </c>
+      <c r="B296" t="s">
         <v>581</v>
       </c>
-      <c r="B296" t="s">
+      <c r="C296" t="s">
+        <v>393</v>
+      </c>
+      <c r="D296" t="s">
         <v>582</v>
-      </c>
-      <c r="C296" t="s">
-        <v>394</v>
-      </c>
-      <c r="D296" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
+        <v>583</v>
+      </c>
+      <c r="B297" t="s">
         <v>584</v>
       </c>
-      <c r="B297" t="s">
+      <c r="C297" t="s">
+        <v>393</v>
+      </c>
+      <c r="D297" t="s">
         <v>585</v>
-      </c>
-      <c r="C297" t="s">
-        <v>394</v>
-      </c>
-      <c r="D297" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
+        <v>586</v>
+      </c>
+      <c r="B298" t="s">
         <v>587</v>
       </c>
-      <c r="B298" t="s">
-        <v>588</v>
-      </c>
       <c r="C298" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D298" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
+        <v>588</v>
+      </c>
+      <c r="B299" t="s">
         <v>589</v>
       </c>
-      <c r="B299" t="s">
-        <v>590</v>
-      </c>
       <c r="C299" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D299" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
+        <v>590</v>
+      </c>
+      <c r="B300" t="s">
         <v>591</v>
       </c>
-      <c r="B300" t="s">
+      <c r="C300" t="s">
+        <v>411</v>
+      </c>
+      <c r="D300" t="s">
         <v>592</v>
-      </c>
-      <c r="C300" t="s">
-        <v>412</v>
-      </c>
-      <c r="D300" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
+        <v>593</v>
+      </c>
+      <c r="B301" t="s">
         <v>594</v>
       </c>
-      <c r="B301" t="s">
-        <v>595</v>
-      </c>
       <c r="C301" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D301" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
+        <v>595</v>
+      </c>
+      <c r="B302" t="s">
         <v>596</v>
       </c>
-      <c r="B302" t="s">
+      <c r="C302" t="s">
+        <v>411</v>
+      </c>
+      <c r="D302" t="s">
         <v>597</v>
-      </c>
-      <c r="C302" t="s">
-        <v>412</v>
-      </c>
-      <c r="D302" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
+        <v>598</v>
+      </c>
+      <c r="B303" t="s">
         <v>599</v>
       </c>
-      <c r="B303" t="s">
+      <c r="C303" t="s">
+        <v>431</v>
+      </c>
+      <c r="D303" t="s">
         <v>600</v>
-      </c>
-      <c r="C303" t="s">
-        <v>432</v>
-      </c>
-      <c r="D303" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
+        <v>601</v>
+      </c>
+      <c r="B304" t="s">
         <v>602</v>
       </c>
-      <c r="B304" t="s">
+      <c r="C304" t="s">
+        <v>411</v>
+      </c>
+      <c r="D304" t="s">
         <v>603</v>
-      </c>
-      <c r="C304" t="s">
-        <v>412</v>
-      </c>
-      <c r="D304" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
+        <v>604</v>
+      </c>
+      <c r="B305" t="s">
         <v>605</v>
       </c>
-      <c r="B305" t="s">
+      <c r="C305" t="s">
+        <v>431</v>
+      </c>
+      <c r="D305" t="s">
         <v>606</v>
-      </c>
-      <c r="C305" t="s">
-        <v>432</v>
-      </c>
-      <c r="D305" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
+        <v>607</v>
+      </c>
+      <c r="B306" t="s">
         <v>608</v>
       </c>
-      <c r="B306" t="s">
+      <c r="C306" t="s">
+        <v>397</v>
+      </c>
+      <c r="D306" t="s">
         <v>609</v>
-      </c>
-      <c r="C306" t="s">
-        <v>398</v>
-      </c>
-      <c r="D306" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
+        <v>610</v>
+      </c>
+      <c r="B307" t="s">
         <v>611</v>
       </c>
-      <c r="B307" t="s">
-        <v>612</v>
-      </c>
       <c r="C307" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D307" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
+        <v>612</v>
+      </c>
+      <c r="B308" t="s">
         <v>613</v>
       </c>
-      <c r="B308" t="s">
+      <c r="C308" t="s">
+        <v>393</v>
+      </c>
+      <c r="D308" t="s">
         <v>614</v>
-      </c>
-      <c r="C308" t="s">
-        <v>394</v>
-      </c>
-      <c r="D308" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
+        <v>615</v>
+      </c>
+      <c r="B309" t="s">
         <v>616</v>
       </c>
-      <c r="B309" t="s">
+      <c r="C309" t="s">
+        <v>411</v>
+      </c>
+      <c r="D309" t="s">
         <v>617</v>
-      </c>
-      <c r="C309" t="s">
-        <v>412</v>
-      </c>
-      <c r="D309" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
+        <v>618</v>
+      </c>
+      <c r="B310" t="s">
         <v>619</v>
       </c>
-      <c r="B310" t="s">
+      <c r="C310" t="s">
+        <v>393</v>
+      </c>
+      <c r="D310" t="s">
         <v>620</v>
-      </c>
-      <c r="C310" t="s">
-        <v>394</v>
-      </c>
-      <c r="D310" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
+        <v>621</v>
+      </c>
+      <c r="B311" t="s">
         <v>622</v>
       </c>
-      <c r="B311" t="s">
-        <v>623</v>
-      </c>
       <c r="C311" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D311" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
+        <v>623</v>
+      </c>
+      <c r="B312" t="s">
         <v>624</v>
       </c>
-      <c r="B312" t="s">
-        <v>625</v>
-      </c>
       <c r="C312" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D312" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
+        <v>625</v>
+      </c>
+      <c r="B313" t="s">
         <v>626</v>
       </c>
-      <c r="B313" t="s">
+      <c r="C313" t="s">
+        <v>397</v>
+      </c>
+      <c r="D313" t="s">
         <v>627</v>
-      </c>
-      <c r="C313" t="s">
-        <v>398</v>
-      </c>
-      <c r="D313" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
+        <v>628</v>
+      </c>
+      <c r="B314" t="s">
         <v>629</v>
       </c>
-      <c r="B314" t="s">
+      <c r="C314" t="s">
         <v>630</v>
       </c>
-      <c r="C314" t="s">
-        <v>631</v>
-      </c>
       <c r="D314" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
+        <v>631</v>
+      </c>
+      <c r="B315" t="s">
         <v>632</v>
       </c>
-      <c r="B315" t="s">
-        <v>633</v>
-      </c>
       <c r="C315" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D315" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
+        <v>633</v>
+      </c>
+      <c r="B316" t="s">
         <v>634</v>
       </c>
-      <c r="B316" t="s">
-        <v>635</v>
-      </c>
       <c r="C316" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D316" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
+        <v>635</v>
+      </c>
+      <c r="B317" t="s">
         <v>636</v>
       </c>
-      <c r="B317" t="s">
+      <c r="C317" t="s">
+        <v>393</v>
+      </c>
+      <c r="D317" t="s">
         <v>637</v>
-      </c>
-      <c r="C317" t="s">
-        <v>394</v>
-      </c>
-      <c r="D317" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
+        <v>638</v>
+      </c>
+      <c r="B318" t="s">
         <v>639</v>
       </c>
-      <c r="B318" t="s">
+      <c r="C318" t="s">
+        <v>393</v>
+      </c>
+      <c r="D318" t="s">
         <v>640</v>
-      </c>
-      <c r="C318" t="s">
-        <v>394</v>
-      </c>
-      <c r="D318" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
+        <v>641</v>
+      </c>
+      <c r="B319" t="s">
         <v>642</v>
       </c>
-      <c r="B319" t="s">
-        <v>643</v>
-      </c>
       <c r="C319" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D319" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
+        <v>643</v>
+      </c>
+      <c r="B320" t="s">
         <v>644</v>
       </c>
-      <c r="B320" t="s">
+      <c r="C320" t="s">
+        <v>393</v>
+      </c>
+      <c r="D320" t="s">
         <v>645</v>
-      </c>
-      <c r="C320" t="s">
-        <v>394</v>
-      </c>
-      <c r="D320" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
+        <v>646</v>
+      </c>
+      <c r="B321" t="s">
         <v>647</v>
       </c>
-      <c r="B321" t="s">
+      <c r="C321" t="s">
+        <v>431</v>
+      </c>
+      <c r="D321" t="s">
         <v>648</v>
-      </c>
-      <c r="C321" t="s">
-        <v>432</v>
-      </c>
-      <c r="D321" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
+        <v>649</v>
+      </c>
+      <c r="B322" t="s">
         <v>650</v>
       </c>
-      <c r="B322" t="s">
+      <c r="C322" t="s">
+        <v>393</v>
+      </c>
+      <c r="D322" t="s">
         <v>651</v>
-      </c>
-      <c r="C322" t="s">
-        <v>394</v>
-      </c>
-      <c r="D322" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
+        <v>652</v>
+      </c>
+      <c r="B323" t="s">
         <v>653</v>
       </c>
-      <c r="B323" t="s">
-        <v>654</v>
-      </c>
       <c r="C323" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D323" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
+        <v>654</v>
+      </c>
+      <c r="B324" t="s">
         <v>655</v>
       </c>
-      <c r="B324" t="s">
+      <c r="C324" t="s">
+        <v>431</v>
+      </c>
+      <c r="D324" t="s">
         <v>656</v>
-      </c>
-      <c r="C324" t="s">
-        <v>432</v>
-      </c>
-      <c r="D324" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
+        <v>657</v>
+      </c>
+      <c r="B325" t="s">
         <v>658</v>
       </c>
-      <c r="B325" t="s">
+      <c r="C325" t="s">
+        <v>431</v>
+      </c>
+      <c r="D325" t="s">
         <v>659</v>
-      </c>
-      <c r="C325" t="s">
-        <v>432</v>
-      </c>
-      <c r="D325" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
+        <v>660</v>
+      </c>
+      <c r="B326" t="s">
         <v>661</v>
       </c>
-      <c r="B326" t="s">
-        <v>662</v>
-      </c>
       <c r="C326" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D326" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
+        <v>662</v>
+      </c>
+      <c r="B327" t="s">
         <v>663</v>
       </c>
-      <c r="B327" t="s">
-        <v>664</v>
-      </c>
       <c r="C327" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D327" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
+        <v>664</v>
+      </c>
+      <c r="B328" t="s">
         <v>665</v>
       </c>
-      <c r="B328" t="s">
+      <c r="C328" t="s">
+        <v>431</v>
+      </c>
+      <c r="D328" t="s">
         <v>666</v>
-      </c>
-      <c r="C328" t="s">
-        <v>432</v>
-      </c>
-      <c r="D328" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
+        <v>667</v>
+      </c>
+      <c r="B329" t="s">
         <v>668</v>
       </c>
-      <c r="B329" t="s">
-        <v>669</v>
-      </c>
       <c r="C329" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D329" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
+        <v>669</v>
+      </c>
+      <c r="B330" t="s">
         <v>670</v>
       </c>
-      <c r="B330" t="s">
+      <c r="C330" t="s">
+        <v>393</v>
+      </c>
+      <c r="D330" t="s">
         <v>671</v>
-      </c>
-      <c r="C330" t="s">
-        <v>394</v>
-      </c>
-      <c r="D330" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
+        <v>672</v>
+      </c>
+      <c r="B331" t="s">
+        <v>672</v>
+      </c>
+      <c r="C331" t="s">
+        <v>411</v>
+      </c>
+      <c r="D331" t="s">
         <v>673</v>
-      </c>
-      <c r="B331" t="s">
-        <v>673</v>
-      </c>
-      <c r="C331" t="s">
-        <v>412</v>
-      </c>
-      <c r="D331" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
+        <v>674</v>
+      </c>
+      <c r="B332" t="s">
+        <v>674</v>
+      </c>
+      <c r="C332" t="s">
+        <v>411</v>
+      </c>
+      <c r="D332" t="s">
         <v>675</v>
-      </c>
-      <c r="B332" t="s">
-        <v>675</v>
-      </c>
-      <c r="C332" t="s">
-        <v>412</v>
-      </c>
-      <c r="D332" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
+        <v>676</v>
+      </c>
+      <c r="B333" t="s">
+        <v>676</v>
+      </c>
+      <c r="C333" t="s">
+        <v>393</v>
+      </c>
+      <c r="D333" t="s">
         <v>677</v>
-      </c>
-      <c r="B333" t="s">
-        <v>677</v>
-      </c>
-      <c r="C333" t="s">
-        <v>394</v>
-      </c>
-      <c r="D333" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
+        <v>678</v>
+      </c>
+      <c r="B334" t="s">
+        <v>678</v>
+      </c>
+      <c r="C334" t="s">
+        <v>393</v>
+      </c>
+      <c r="D334" t="s">
         <v>679</v>
-      </c>
-      <c r="B334" t="s">
-        <v>679</v>
-      </c>
-      <c r="C334" t="s">
-        <v>394</v>
-      </c>
-      <c r="D334" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
+        <v>680</v>
+      </c>
+      <c r="B335" t="s">
+        <v>680</v>
+      </c>
+      <c r="C335" t="s">
+        <v>446</v>
+      </c>
+      <c r="D335" t="s">
         <v>681</v>
-      </c>
-      <c r="B335" t="s">
-        <v>681</v>
-      </c>
-      <c r="C335" t="s">
-        <v>447</v>
-      </c>
-      <c r="D335" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
+        <v>682</v>
+      </c>
+      <c r="B336" t="s">
+        <v>682</v>
+      </c>
+      <c r="C336" t="s">
         <v>683</v>
       </c>
-      <c r="B336" t="s">
-        <v>683</v>
-      </c>
-      <c r="C336" t="s">
+      <c r="D336" t="s">
         <v>684</v>
-      </c>
-      <c r="D336" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
+        <v>685</v>
+      </c>
+      <c r="B337" t="s">
+        <v>685</v>
+      </c>
+      <c r="C337" t="s">
+        <v>534</v>
+      </c>
+      <c r="D337" t="s">
         <v>686</v>
-      </c>
-      <c r="B337" t="s">
-        <v>686</v>
-      </c>
-      <c r="C337" t="s">
-        <v>535</v>
-      </c>
-      <c r="D337" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
+        <v>687</v>
+      </c>
+      <c r="B338" t="s">
         <v>688</v>
       </c>
-      <c r="B338" t="s">
-        <v>689</v>
-      </c>
       <c r="C338" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D338" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
+        <v>689</v>
+      </c>
+      <c r="B339" t="s">
         <v>690</v>
       </c>
-      <c r="B339" t="s">
+      <c r="C339" t="s">
+        <v>393</v>
+      </c>
+      <c r="D339" t="s">
         <v>691</v>
-      </c>
-      <c r="C339" t="s">
-        <v>394</v>
-      </c>
-      <c r="D339" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
+        <v>692</v>
+      </c>
+      <c r="B340" t="s">
         <v>693</v>
       </c>
-      <c r="B340" t="s">
+      <c r="C340" t="s">
+        <v>393</v>
+      </c>
+      <c r="D340" t="s">
         <v>694</v>
-      </c>
-      <c r="C340" t="s">
-        <v>394</v>
-      </c>
-      <c r="D340" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
+        <v>695</v>
+      </c>
+      <c r="B341" t="s">
         <v>696</v>
       </c>
-      <c r="B341" t="s">
+      <c r="C341" t="s">
+        <v>393</v>
+      </c>
+      <c r="D341" t="s">
         <v>697</v>
-      </c>
-      <c r="C341" t="s">
-        <v>394</v>
-      </c>
-      <c r="D341" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
+        <v>698</v>
+      </c>
+      <c r="B342" t="s">
         <v>699</v>
       </c>
-      <c r="B342" t="s">
+      <c r="C342" t="s">
+        <v>411</v>
+      </c>
+      <c r="D342" t="s">
         <v>700</v>
-      </c>
-      <c r="C342" t="s">
-        <v>412</v>
-      </c>
-      <c r="D342" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B343" t="s">
         <v>319</v>
       </c>
       <c r="C343" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D343" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
+        <v>702</v>
+      </c>
+      <c r="B344" t="s">
+        <v>702</v>
+      </c>
+      <c r="C344" t="s">
+        <v>411</v>
+      </c>
+      <c r="D344" t="s">
         <v>703</v>
-      </c>
-      <c r="B344" t="s">
-        <v>703</v>
-      </c>
-      <c r="C344" t="s">
-        <v>412</v>
-      </c>
-      <c r="D344" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
+        <v>704</v>
+      </c>
+      <c r="B345" t="s">
+        <v>704</v>
+      </c>
+      <c r="C345" t="s">
+        <v>411</v>
+      </c>
+      <c r="D345" t="s">
         <v>705</v>
-      </c>
-      <c r="B345" t="s">
-        <v>705</v>
-      </c>
-      <c r="C345" t="s">
-        <v>412</v>
-      </c>
-      <c r="D345" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
+        <v>706</v>
+      </c>
+      <c r="B346" t="s">
+        <v>706</v>
+      </c>
+      <c r="C346" t="s">
+        <v>411</v>
+      </c>
+      <c r="D346" t="s">
         <v>707</v>
-      </c>
-      <c r="B346" t="s">
-        <v>707</v>
-      </c>
-      <c r="C346" t="s">
-        <v>412</v>
-      </c>
-      <c r="D346" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B347" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C347" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D347" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
+        <v>709</v>
+      </c>
+      <c r="B348" t="s">
+        <v>709</v>
+      </c>
+      <c r="C348" t="s">
+        <v>397</v>
+      </c>
+      <c r="D348" t="s">
         <v>710</v>
-      </c>
-      <c r="B348" t="s">
-        <v>710</v>
-      </c>
-      <c r="C348" t="s">
-        <v>398</v>
-      </c>
-      <c r="D348" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
+        <v>711</v>
+      </c>
+      <c r="B349" t="s">
+        <v>711</v>
+      </c>
+      <c r="C349" t="s">
+        <v>431</v>
+      </c>
+      <c r="D349" t="s">
         <v>712</v>
-      </c>
-      <c r="B349" t="s">
-        <v>712</v>
-      </c>
-      <c r="C349" t="s">
-        <v>432</v>
-      </c>
-      <c r="D349" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
+        <v>713</v>
+      </c>
+      <c r="B350" t="s">
+        <v>713</v>
+      </c>
+      <c r="C350" t="s">
+        <v>431</v>
+      </c>
+      <c r="D350" t="s">
         <v>714</v>
-      </c>
-      <c r="B350" t="s">
-        <v>714</v>
-      </c>
-      <c r="C350" t="s">
-        <v>432</v>
-      </c>
-      <c r="D350" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
+        <v>715</v>
+      </c>
+      <c r="B351" t="s">
+        <v>715</v>
+      </c>
+      <c r="C351" t="s">
+        <v>534</v>
+      </c>
+      <c r="D351" t="s">
         <v>716</v>
-      </c>
-      <c r="B351" t="s">
-        <v>716</v>
-      </c>
-      <c r="C351" t="s">
-        <v>535</v>
-      </c>
-      <c r="D351" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="352" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A352" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B352" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
+        <v>719</v>
+      </c>
+      <c r="B353" t="s">
         <v>720</v>
       </c>
-      <c r="B353" t="s">
+      <c r="C353" t="s">
+        <v>411</v>
+      </c>
+      <c r="D353" t="s">
         <v>721</v>
-      </c>
-      <c r="C353" t="s">
-        <v>412</v>
-      </c>
-      <c r="D353" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
+        <v>722</v>
+      </c>
+      <c r="B354" t="s">
         <v>723</v>
       </c>
-      <c r="B354" t="s">
+      <c r="C354" t="s">
+        <v>411</v>
+      </c>
+      <c r="D354" t="s">
         <v>724</v>
-      </c>
-      <c r="C354" t="s">
-        <v>412</v>
-      </c>
-      <c r="D354" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
+        <v>725</v>
+      </c>
+      <c r="B355" t="s">
         <v>726</v>
       </c>
-      <c r="B355" t="s">
+      <c r="C355" t="s">
+        <v>411</v>
+      </c>
+      <c r="D355" t="s">
         <v>727</v>
-      </c>
-      <c r="C355" t="s">
-        <v>412</v>
-      </c>
-      <c r="D355" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
+        <v>728</v>
+      </c>
+      <c r="B356" t="s">
         <v>729</v>
       </c>
-      <c r="B356" t="s">
+      <c r="C356" t="s">
+        <v>393</v>
+      </c>
+      <c r="D356" t="s">
         <v>730</v>
-      </c>
-      <c r="C356" t="s">
-        <v>394</v>
-      </c>
-      <c r="D356" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
+        <v>731</v>
+      </c>
+      <c r="B357" t="s">
         <v>732</v>
       </c>
-      <c r="B357" t="s">
+      <c r="C357" t="s">
+        <v>431</v>
+      </c>
+      <c r="D357" t="s">
         <v>733</v>
-      </c>
-      <c r="C357" t="s">
-        <v>432</v>
-      </c>
-      <c r="D357" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
+        <v>734</v>
+      </c>
+      <c r="B358" t="s">
         <v>735</v>
       </c>
-      <c r="B358" t="s">
+      <c r="C358" t="s">
+        <v>393</v>
+      </c>
+      <c r="D358" t="s">
         <v>736</v>
-      </c>
-      <c r="C358" t="s">
-        <v>394</v>
-      </c>
-      <c r="D358" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
+        <v>737</v>
+      </c>
+      <c r="B359" t="s">
         <v>738</v>
       </c>
-      <c r="B359" t="s">
+      <c r="C359" t="s">
+        <v>393</v>
+      </c>
+      <c r="D359" t="s">
         <v>739</v>
-      </c>
-      <c r="C359" t="s">
-        <v>394</v>
-      </c>
-      <c r="D359" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
+        <v>740</v>
+      </c>
+      <c r="B360" t="s">
         <v>741</v>
       </c>
-      <c r="B360" t="s">
+      <c r="C360" t="s">
+        <v>393</v>
+      </c>
+      <c r="D360" t="s">
         <v>742</v>
-      </c>
-      <c r="C360" t="s">
-        <v>394</v>
-      </c>
-      <c r="D360" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
+        <v>743</v>
+      </c>
+      <c r="B361" t="s">
         <v>744</v>
       </c>
-      <c r="B361" t="s">
+      <c r="C361" t="s">
+        <v>393</v>
+      </c>
+      <c r="D361" t="s">
         <v>745</v>
-      </c>
-      <c r="C361" t="s">
-        <v>394</v>
-      </c>
-      <c r="D361" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
+        <v>746</v>
+      </c>
+      <c r="B362" t="s">
         <v>747</v>
       </c>
-      <c r="B362" t="s">
-        <v>748</v>
-      </c>
       <c r="C362" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D362" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
+        <v>748</v>
+      </c>
+      <c r="B363" t="s">
         <v>749</v>
       </c>
-      <c r="B363" t="s">
-        <v>750</v>
-      </c>
       <c r="C363" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D363" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
+        <v>750</v>
+      </c>
+      <c r="B364" t="s">
         <v>751</v>
       </c>
-      <c r="B364" t="s">
-        <v>752</v>
-      </c>
       <c r="C364" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D364" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
+        <v>752</v>
+      </c>
+      <c r="B365" t="s">
         <v>753</v>
       </c>
-      <c r="B365" t="s">
+      <c r="C365" t="s">
+        <v>393</v>
+      </c>
+      <c r="D365" t="s">
         <v>754</v>
-      </c>
-      <c r="C365" t="s">
-        <v>394</v>
-      </c>
-      <c r="D365" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
+        <v>755</v>
+      </c>
+      <c r="B366" t="s">
         <v>756</v>
       </c>
-      <c r="B366" t="s">
+      <c r="C366" t="s">
+        <v>393</v>
+      </c>
+      <c r="D366" t="s">
         <v>757</v>
-      </c>
-      <c r="C366" t="s">
-        <v>394</v>
-      </c>
-      <c r="D366" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
+        <v>758</v>
+      </c>
+      <c r="B367" t="s">
         <v>759</v>
       </c>
-      <c r="B367" t="s">
+      <c r="C367" t="s">
+        <v>393</v>
+      </c>
+      <c r="D367" t="s">
         <v>760</v>
-      </c>
-      <c r="C367" t="s">
-        <v>394</v>
-      </c>
-      <c r="D367" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
+        <v>761</v>
+      </c>
+      <c r="B368" t="s">
         <v>762</v>
       </c>
-      <c r="B368" t="s">
+      <c r="C368" t="s">
+        <v>393</v>
+      </c>
+      <c r="D368" t="s">
         <v>763</v>
-      </c>
-      <c r="C368" t="s">
-        <v>394</v>
-      </c>
-      <c r="D368" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
+        <v>764</v>
+      </c>
+      <c r="B369" t="s">
         <v>765</v>
       </c>
-      <c r="B369" t="s">
+      <c r="C369" t="s">
+        <v>393</v>
+      </c>
+      <c r="D369" t="s">
         <v>766</v>
-      </c>
-      <c r="C369" t="s">
-        <v>394</v>
-      </c>
-      <c r="D369" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
+        <v>767</v>
+      </c>
+      <c r="B370" t="s">
         <v>768</v>
       </c>
-      <c r="B370" t="s">
+      <c r="C370" t="s">
+        <v>393</v>
+      </c>
+      <c r="D370" t="s">
         <v>769</v>
-      </c>
-      <c r="C370" t="s">
-        <v>394</v>
-      </c>
-      <c r="D370" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
+        <v>770</v>
+      </c>
+      <c r="B371" t="s">
         <v>771</v>
       </c>
-      <c r="B371" t="s">
+      <c r="C371" t="s">
+        <v>393</v>
+      </c>
+      <c r="D371" t="s">
         <v>772</v>
-      </c>
-      <c r="C371" t="s">
-        <v>394</v>
-      </c>
-      <c r="D371" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
+        <v>773</v>
+      </c>
+      <c r="B372" t="s">
+        <v>773</v>
+      </c>
+      <c r="C372" t="s">
+        <v>393</v>
+      </c>
+      <c r="D372" t="s">
         <v>774</v>
-      </c>
-      <c r="B372" t="s">
-        <v>774</v>
-      </c>
-      <c r="C372" t="s">
-        <v>394</v>
-      </c>
-      <c r="D372" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
+        <v>775</v>
+      </c>
+      <c r="B373" t="s">
+        <v>775</v>
+      </c>
+      <c r="C373" t="s">
+        <v>393</v>
+      </c>
+      <c r="D373" t="s">
         <v>776</v>
-      </c>
-      <c r="B373" t="s">
-        <v>776</v>
-      </c>
-      <c r="C373" t="s">
-        <v>394</v>
-      </c>
-      <c r="D373" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
+        <v>777</v>
+      </c>
+      <c r="B374" t="s">
+        <v>777</v>
+      </c>
+      <c r="C374" t="s">
+        <v>411</v>
+      </c>
+      <c r="D374" t="s">
         <v>778</v>
-      </c>
-      <c r="B374" t="s">
-        <v>778</v>
-      </c>
-      <c r="C374" t="s">
-        <v>412</v>
-      </c>
-      <c r="D374" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
+        <v>779</v>
+      </c>
+      <c r="B375" t="s">
+        <v>779</v>
+      </c>
+      <c r="C375" t="s">
+        <v>411</v>
+      </c>
+      <c r="D375" t="s">
         <v>780</v>
-      </c>
-      <c r="B375" t="s">
-        <v>780</v>
-      </c>
-      <c r="C375" t="s">
-        <v>412</v>
-      </c>
-      <c r="D375" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
+        <v>781</v>
+      </c>
+      <c r="B376" t="s">
+        <v>781</v>
+      </c>
+      <c r="C376" t="s">
+        <v>393</v>
+      </c>
+      <c r="D376" t="s">
         <v>782</v>
-      </c>
-      <c r="B376" t="s">
-        <v>782</v>
-      </c>
-      <c r="C376" t="s">
-        <v>394</v>
-      </c>
-      <c r="D376" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
+        <v>783</v>
+      </c>
+      <c r="B377" t="s">
+        <v>783</v>
+      </c>
+      <c r="C377" t="s">
+        <v>397</v>
+      </c>
+      <c r="D377" t="s">
         <v>784</v>
-      </c>
-      <c r="B377" t="s">
-        <v>784</v>
-      </c>
-      <c r="C377" t="s">
-        <v>398</v>
-      </c>
-      <c r="D377" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
+        <v>785</v>
+      </c>
+      <c r="B378" t="s">
+        <v>785</v>
+      </c>
+      <c r="C378" t="s">
+        <v>393</v>
+      </c>
+      <c r="D378" t="s">
         <v>786</v>
-      </c>
-      <c r="B378" t="s">
-        <v>786</v>
-      </c>
-      <c r="C378" t="s">
-        <v>394</v>
-      </c>
-      <c r="D378" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
+        <v>787</v>
+      </c>
+      <c r="B379" t="s">
+        <v>787</v>
+      </c>
+      <c r="C379" t="s">
+        <v>446</v>
+      </c>
+      <c r="D379" t="s">
         <v>788</v>
-      </c>
-      <c r="B379" t="s">
-        <v>788</v>
-      </c>
-      <c r="C379" t="s">
-        <v>447</v>
-      </c>
-      <c r="D379" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
+        <v>789</v>
+      </c>
+      <c r="B380" t="s">
         <v>790</v>
       </c>
-      <c r="B380" t="s">
+      <c r="C380" t="s">
+        <v>393</v>
+      </c>
+      <c r="D380" t="s">
         <v>791</v>
-      </c>
-      <c r="C380" t="s">
-        <v>394</v>
-      </c>
-      <c r="D380" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
+        <v>792</v>
+      </c>
+      <c r="B381" t="s">
         <v>793</v>
       </c>
-      <c r="B381" t="s">
+      <c r="C381" t="s">
+        <v>393</v>
+      </c>
+      <c r="D381" t="s">
         <v>794</v>
-      </c>
-      <c r="C381" t="s">
-        <v>394</v>
-      </c>
-      <c r="D381" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
+        <v>795</v>
+      </c>
+      <c r="B382" t="s">
         <v>796</v>
       </c>
-      <c r="B382" t="s">
+      <c r="C382" t="s">
+        <v>397</v>
+      </c>
+      <c r="D382" t="s">
         <v>797</v>
-      </c>
-      <c r="C382" t="s">
-        <v>398</v>
-      </c>
-      <c r="D382" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
+        <v>798</v>
+      </c>
+      <c r="B383" t="s">
         <v>799</v>
       </c>
-      <c r="B383" t="s">
+      <c r="C383" t="s">
+        <v>393</v>
+      </c>
+      <c r="D383" t="s">
         <v>800</v>
-      </c>
-      <c r="C383" t="s">
-        <v>394</v>
-      </c>
-      <c r="D383" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
+        <v>801</v>
+      </c>
+      <c r="B384" t="s">
         <v>802</v>
       </c>
-      <c r="B384" t="s">
+      <c r="C384" t="s">
+        <v>393</v>
+      </c>
+      <c r="D384" t="s">
         <v>803</v>
-      </c>
-      <c r="C384" t="s">
-        <v>394</v>
-      </c>
-      <c r="D384" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
+        <v>804</v>
+      </c>
+      <c r="B385" t="s">
         <v>805</v>
       </c>
-      <c r="B385" t="s">
-        <v>806</v>
-      </c>
       <c r="C385" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D385" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
+        <v>806</v>
+      </c>
+      <c r="B386" t="s">
         <v>807</v>
       </c>
-      <c r="B386" t="s">
+      <c r="C386" t="s">
+        <v>393</v>
+      </c>
+      <c r="D386" t="s">
         <v>808</v>
-      </c>
-      <c r="C386" t="s">
-        <v>394</v>
-      </c>
-      <c r="D386" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
+        <v>809</v>
+      </c>
+      <c r="B387" t="s">
         <v>810</v>
       </c>
-      <c r="B387" t="s">
+      <c r="C387" t="s">
+        <v>397</v>
+      </c>
+      <c r="D387" t="s">
         <v>811</v>
-      </c>
-      <c r="C387" t="s">
-        <v>398</v>
-      </c>
-      <c r="D387" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
+        <v>812</v>
+      </c>
+      <c r="B388" t="s">
         <v>813</v>
       </c>
-      <c r="B388" t="s">
+      <c r="C388" t="s">
+        <v>393</v>
+      </c>
+      <c r="D388" t="s">
         <v>814</v>
-      </c>
-      <c r="C388" t="s">
-        <v>394</v>
-      </c>
-      <c r="D388" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
+        <v>815</v>
+      </c>
+      <c r="B389" t="s">
         <v>816</v>
       </c>
-      <c r="B389" t="s">
+      <c r="C389" t="s">
+        <v>431</v>
+      </c>
+      <c r="D389" t="s">
         <v>817</v>
-      </c>
-      <c r="C389" t="s">
-        <v>432</v>
-      </c>
-      <c r="D389" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
+        <v>818</v>
+      </c>
+      <c r="B390" t="s">
         <v>819</v>
       </c>
-      <c r="B390" t="s">
+      <c r="C390" t="s">
+        <v>411</v>
+      </c>
+      <c r="D390" t="s">
         <v>820</v>
-      </c>
-      <c r="C390" t="s">
-        <v>412</v>
-      </c>
-      <c r="D390" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
+        <v>821</v>
+      </c>
+      <c r="B391" t="s">
         <v>822</v>
       </c>
-      <c r="B391" t="s">
+      <c r="C391" t="s">
+        <v>411</v>
+      </c>
+      <c r="D391" t="s">
         <v>823</v>
-      </c>
-      <c r="C391" t="s">
-        <v>412</v>
-      </c>
-      <c r="D391" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
+        <v>824</v>
+      </c>
+      <c r="B392" t="s">
         <v>825</v>
       </c>
-      <c r="B392" t="s">
+      <c r="C392" t="s">
+        <v>411</v>
+      </c>
+      <c r="D392" t="s">
         <v>826</v>
-      </c>
-      <c r="C392" t="s">
-        <v>412</v>
-      </c>
-      <c r="D392" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
+        <v>827</v>
+      </c>
+      <c r="B393" t="s">
         <v>828</v>
       </c>
-      <c r="B393" t="s">
-        <v>829</v>
-      </c>
       <c r="C393" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D393" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
+        <v>829</v>
+      </c>
+      <c r="B394" t="s">
         <v>830</v>
       </c>
-      <c r="B394" t="s">
+      <c r="C394" t="s">
+        <v>431</v>
+      </c>
+      <c r="D394" t="s">
         <v>831</v>
-      </c>
-      <c r="C394" t="s">
-        <v>432</v>
-      </c>
-      <c r="D394" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
+        <v>832</v>
+      </c>
+      <c r="B395" t="s">
         <v>833</v>
       </c>
-      <c r="B395" t="s">
+      <c r="C395" t="s">
+        <v>446</v>
+      </c>
+      <c r="D395" t="s">
         <v>834</v>
-      </c>
-      <c r="C395" t="s">
-        <v>447</v>
-      </c>
-      <c r="D395" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
+        <v>835</v>
+      </c>
+      <c r="B396" t="s">
+        <v>835</v>
+      </c>
+      <c r="C396" t="s">
+        <v>411</v>
+      </c>
+      <c r="D396" t="s">
         <v>836</v>
-      </c>
-      <c r="B396" t="s">
-        <v>836</v>
-      </c>
-      <c r="C396" t="s">
-        <v>412</v>
-      </c>
-      <c r="D396" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="397" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A397" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="B397" s="3" t="s">
         <v>839</v>
-      </c>
-      <c r="B397" s="3" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="398" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A398" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="B398" s="3" t="s">
         <v>841</v>
-      </c>
-      <c r="B398" s="3" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="399" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A399" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="B399" s="3" t="s">
         <v>843</v>
-      </c>
-      <c r="B399" s="3" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="400" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A400" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="B400" s="3" t="s">
         <v>845</v>
-      </c>
-      <c r="B400" s="3" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="401" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A401" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="B401" s="3" t="s">
         <v>847</v>
-      </c>
-      <c r="B401" s="3" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="402" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A402" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="B402" s="3" t="s">
         <v>849</v>
-      </c>
-      <c r="B402" s="3" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
+        <v>850</v>
+      </c>
+      <c r="B403" t="s">
+        <v>850</v>
+      </c>
+      <c r="C403" t="s">
+        <v>411</v>
+      </c>
+      <c r="D403" t="s">
         <v>851</v>
-      </c>
-      <c r="B403" t="s">
-        <v>851</v>
-      </c>
-      <c r="C403" t="s">
-        <v>412</v>
-      </c>
-      <c r="D403" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
+        <v>852</v>
+      </c>
+      <c r="B404" t="s">
+        <v>852</v>
+      </c>
+      <c r="C404" t="s">
+        <v>411</v>
+      </c>
+      <c r="D404" t="s">
         <v>853</v>
-      </c>
-      <c r="B404" t="s">
-        <v>853</v>
-      </c>
-      <c r="C404" t="s">
-        <v>412</v>
-      </c>
-      <c r="D404" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
+        <v>854</v>
+      </c>
+      <c r="B405" t="s">
         <v>855</v>
       </c>
-      <c r="B405" t="s">
+      <c r="C405" t="s">
+        <v>393</v>
+      </c>
+      <c r="D405" t="s">
         <v>856</v>
-      </c>
-      <c r="C405" t="s">
-        <v>394</v>
-      </c>
-      <c r="D405" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
+        <v>857</v>
+      </c>
+      <c r="B406" t="s">
         <v>858</v>
       </c>
-      <c r="B406" t="s">
+      <c r="C406" t="s">
+        <v>411</v>
+      </c>
+      <c r="D406" t="s">
         <v>859</v>
-      </c>
-      <c r="C406" t="s">
-        <v>412</v>
-      </c>
-      <c r="D406" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
+        <v>860</v>
+      </c>
+      <c r="B407" t="s">
         <v>861</v>
       </c>
-      <c r="B407" t="s">
-        <v>862</v>
-      </c>
       <c r="C407" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D407" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
+        <v>862</v>
+      </c>
+      <c r="B408" t="s">
         <v>863</v>
       </c>
-      <c r="B408" t="s">
+      <c r="C408" t="s">
+        <v>411</v>
+      </c>
+      <c r="D408" t="s">
         <v>864</v>
-      </c>
-      <c r="C408" t="s">
-        <v>412</v>
-      </c>
-      <c r="D408" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
+        <v>865</v>
+      </c>
+      <c r="B409" t="s">
         <v>866</v>
       </c>
-      <c r="B409" t="s">
+      <c r="C409" t="s">
+        <v>411</v>
+      </c>
+      <c r="D409" t="s">
         <v>867</v>
-      </c>
-      <c r="C409" t="s">
-        <v>412</v>
-      </c>
-      <c r="D409" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
+        <v>868</v>
+      </c>
+      <c r="B410" t="s">
         <v>869</v>
       </c>
-      <c r="B410" t="s">
+      <c r="C410" t="s">
+        <v>393</v>
+      </c>
+      <c r="D410" t="s">
         <v>870</v>
-      </c>
-      <c r="C410" t="s">
-        <v>394</v>
-      </c>
-      <c r="D410" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
+        <v>871</v>
+      </c>
+      <c r="B411" t="s">
         <v>872</v>
       </c>
-      <c r="B411" t="s">
+      <c r="C411" t="s">
+        <v>393</v>
+      </c>
+      <c r="D411" t="s">
         <v>873</v>
-      </c>
-      <c r="C411" t="s">
-        <v>394</v>
-      </c>
-      <c r="D411" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
+        <v>874</v>
+      </c>
+      <c r="B412" t="s">
         <v>875</v>
       </c>
-      <c r="B412" t="s">
+      <c r="C412" t="s">
+        <v>393</v>
+      </c>
+      <c r="D412" t="s">
         <v>876</v>
-      </c>
-      <c r="C412" t="s">
-        <v>394</v>
-      </c>
-      <c r="D412" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
+        <v>877</v>
+      </c>
+      <c r="B413" t="s">
         <v>878</v>
       </c>
-      <c r="B413" t="s">
-        <v>879</v>
-      </c>
       <c r="C413" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D413" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
+        <v>879</v>
+      </c>
+      <c r="B414" t="s">
         <v>880</v>
       </c>
-      <c r="B414" t="s">
-        <v>881</v>
-      </c>
       <c r="C414" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D414" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
+        <v>881</v>
+      </c>
+      <c r="B415" t="s">
         <v>882</v>
       </c>
-      <c r="B415" t="s">
+      <c r="C415" t="s">
+        <v>393</v>
+      </c>
+      <c r="D415" t="s">
         <v>883</v>
-      </c>
-      <c r="C415" t="s">
-        <v>394</v>
-      </c>
-      <c r="D415" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
+        <v>884</v>
+      </c>
+      <c r="B416" t="s">
         <v>885</v>
       </c>
-      <c r="B416" t="s">
+      <c r="C416" t="s">
+        <v>393</v>
+      </c>
+      <c r="D416" t="s">
         <v>886</v>
-      </c>
-      <c r="C416" t="s">
-        <v>394</v>
-      </c>
-      <c r="D416" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
+        <v>887</v>
+      </c>
+      <c r="B417" t="s">
         <v>888</v>
       </c>
-      <c r="B417" t="s">
+      <c r="C417" t="s">
         <v>889</v>
       </c>
-      <c r="C417" t="s">
+      <c r="D417" t="s">
         <v>890</v>
-      </c>
-      <c r="D417" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
+        <v>891</v>
+      </c>
+      <c r="B418" t="s">
         <v>892</v>
       </c>
-      <c r="B418" t="s">
+      <c r="C418" t="s">
+        <v>431</v>
+      </c>
+      <c r="D418" t="s">
         <v>893</v>
-      </c>
-      <c r="C418" t="s">
-        <v>432</v>
-      </c>
-      <c r="D418" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
+        <v>894</v>
+      </c>
+      <c r="B419" t="s">
         <v>895</v>
       </c>
-      <c r="B419" t="s">
+      <c r="C419" t="s">
+        <v>431</v>
+      </c>
+      <c r="D419" t="s">
         <v>896</v>
-      </c>
-      <c r="C419" t="s">
-        <v>432</v>
-      </c>
-      <c r="D419" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
+        <v>897</v>
+      </c>
+      <c r="B420" t="s">
         <v>898</v>
       </c>
-      <c r="B420" t="s">
+      <c r="C420" t="s">
+        <v>411</v>
+      </c>
+      <c r="D420" t="s">
         <v>899</v>
-      </c>
-      <c r="C420" t="s">
-        <v>412</v>
-      </c>
-      <c r="D420" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
+        <v>900</v>
+      </c>
+      <c r="B421" t="s">
         <v>901</v>
       </c>
-      <c r="B421" t="s">
+      <c r="C421" t="s">
+        <v>393</v>
+      </c>
+      <c r="D421" t="s">
         <v>902</v>
-      </c>
-      <c r="C421" t="s">
-        <v>394</v>
-      </c>
-      <c r="D421" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
+        <v>903</v>
+      </c>
+      <c r="B422" t="s">
         <v>904</v>
       </c>
-      <c r="B422" t="s">
-        <v>905</v>
-      </c>
       <c r="C422" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D422" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
+        <v>905</v>
+      </c>
+      <c r="B423" t="s">
         <v>906</v>
       </c>
-      <c r="B423" t="s">
+      <c r="C423" t="s">
+        <v>397</v>
+      </c>
+      <c r="D423" t="s">
         <v>907</v>
-      </c>
-      <c r="C423" t="s">
-        <v>398</v>
-      </c>
-      <c r="D423" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
+        <v>908</v>
+      </c>
+      <c r="B424" t="s">
         <v>909</v>
       </c>
-      <c r="B424" t="s">
+      <c r="C424" t="s">
+        <v>431</v>
+      </c>
+      <c r="D424" t="s">
         <v>910</v>
-      </c>
-      <c r="C424" t="s">
-        <v>432</v>
-      </c>
-      <c r="D424" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
+        <v>911</v>
+      </c>
+      <c r="B425" t="s">
+        <v>911</v>
+      </c>
+      <c r="C425" t="s">
+        <v>431</v>
+      </c>
+      <c r="D425" t="s">
         <v>912</v>
-      </c>
-      <c r="B425" t="s">
-        <v>912</v>
-      </c>
-      <c r="C425" t="s">
-        <v>432</v>
-      </c>
-      <c r="D425" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
+        <v>913</v>
+      </c>
+      <c r="B426" t="s">
         <v>914</v>
-      </c>
-      <c r="B426" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
+        <v>915</v>
+      </c>
+      <c r="B427" t="s">
         <v>916</v>
-      </c>
-      <c r="B427" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
+        <v>917</v>
+      </c>
+      <c r="B428" t="s">
         <v>918</v>
-      </c>
-      <c r="B428" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B429" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="430" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A430" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B430" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="431" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A431" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="B431" s="3" t="s">
         <v>922</v>
-      </c>
-      <c r="B431" s="3" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="432" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A432" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="B432" s="3" t="s">
         <v>924</v>
-      </c>
-      <c r="B432" s="3" t="s">
-        <v>925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update non_verbs.xlsx with changes
</commit_message>
<xml_diff>
--- a/non_verbs.xlsx
+++ b/non_verbs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE5F637-3AF8-4D31-95D8-1AFB8B47FD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D1274B-9F20-403C-AD63-175588B23AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="968">
   <si>
     <t>Kanji</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -446,22 +446,10 @@
     <t>いみ</t>
   </si>
   <si>
-    <t>日本語</t>
-  </si>
-  <si>
-    <t>にほんご</t>
-  </si>
-  <si>
     <t>英語</t>
   </si>
   <si>
     <t>えいご</t>
-  </si>
-  <si>
-    <t>中国語</t>
-  </si>
-  <si>
-    <t>ちゅうごくご</t>
   </si>
   <si>
     <t>台湾語</t>
@@ -2849,6 +2837,149 @@
   <si>
     <t>むり</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>いちど</t>
+  </si>
+  <si>
+    <t>一次</t>
+  </si>
+  <si>
+    <t>一回</t>
+  </si>
+  <si>
+    <t>いっかい</t>
+  </si>
+  <si>
+    <t>一杯</t>
+  </si>
+  <si>
+    <t>いっぱい</t>
+  </si>
+  <si>
+    <t>明日</t>
+  </si>
+  <si>
+    <t>あす</t>
+  </si>
+  <si>
+    <t>[2][0]</t>
+  </si>
+  <si>
+    <t>明天</t>
+  </si>
+  <si>
+    <t>今度</t>
+  </si>
+  <si>
+    <t>こんど</t>
+  </si>
+  <si>
+    <t>這次／下次</t>
+  </si>
+  <si>
+    <t>今回</t>
+  </si>
+  <si>
+    <t>こんかい</t>
+  </si>
+  <si>
+    <t>這次</t>
+  </si>
+  <si>
+    <t>今夜</t>
+  </si>
+  <si>
+    <t>こんや</t>
+  </si>
+  <si>
+    <t>今晚</t>
+  </si>
+  <si>
+    <t>最近</t>
+  </si>
+  <si>
+    <t>さいきん</t>
+  </si>
+  <si>
+    <t>最初</t>
+  </si>
+  <si>
+    <t>さいしょ</t>
+  </si>
+  <si>
+    <t>最初／首次</t>
+  </si>
+  <si>
+    <t>最後</t>
+  </si>
+  <si>
+    <t>さいご</t>
+  </si>
+  <si>
+    <t>正月</t>
+  </si>
+  <si>
+    <t>しょうがつ</t>
+  </si>
+  <si>
+    <t>[4][0]</t>
+  </si>
+  <si>
+    <t>時代</t>
+  </si>
+  <si>
+    <t>じだい</t>
+  </si>
+  <si>
+    <t>昼間</t>
+  </si>
+  <si>
+    <t>ひるま</t>
+  </si>
+  <si>
+    <t>白天</t>
+  </si>
+  <si>
+    <t>歴史</t>
+  </si>
+  <si>
+    <t>れきし</t>
+  </si>
+  <si>
+    <t>歷史</t>
+  </si>
+  <si>
+    <t>昔</t>
+  </si>
+  <si>
+    <t>むかし</t>
+  </si>
+  <si>
+    <t>從前、以前</t>
+  </si>
+  <si>
+    <t>久しぶり</t>
+  </si>
+  <si>
+    <t>ひさしぶり</t>
+  </si>
+  <si>
+    <t>[0][5]</t>
+  </si>
+  <si>
+    <t>久、久違</t>
+  </si>
+  <si>
+    <t>一度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>夜中</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>よなか</t>
   </si>
 </sst>
 </file>
@@ -3257,10 +3388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F432"/>
+  <dimension ref="A1:F447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="D198" sqref="D198"/>
+    <sheetView tabSelected="1" topLeftCell="A428" workbookViewId="0">
+      <selection activeCell="B447" sqref="B447"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4083,17 +4214,13 @@
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" t="s">
         <v>138</v>
       </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
     </row>
     <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
@@ -4123,23 +4250,23 @@
       <c r="A82" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B82" t="s">
-        <v>146</v>
+      <c r="B82" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B83" t="s">
         <v>147</v>
-      </c>
-      <c r="B83" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B84" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" t="s">
         <v>149</v>
       </c>
     </row>
@@ -4275,47 +4402,47 @@
       <c r="A101" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B101" t="s">
-        <v>183</v>
+      <c r="B101" s="5" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B102" t="s">
-        <v>185</v>
+        <v>183</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
+      </c>
+      <c r="B105" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B106" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B106" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4403,87 +4530,87 @@
       <c r="A117" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B117" t="s">
-        <v>211</v>
+      <c r="B117" s="5" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B118" t="s">
-        <v>213</v>
+        <v>211</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
+      </c>
+      <c r="B126" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B127" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B127" t="s">
         <v>223</v>
       </c>
     </row>
@@ -4611,101 +4738,101 @@
       <c r="A143" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="B143" t="s">
-        <v>255</v>
+      <c r="B143" s="5" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B144" t="s">
-        <v>257</v>
+        <v>255</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="B151" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
+      </c>
+      <c r="B151" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="B152" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B152" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="B153" t="s">
         <v>266</v>
-      </c>
-      <c r="B153" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B154" t="s">
         <v>268</v>
-      </c>
-      <c r="B154" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>718</v>
+        <v>269</v>
       </c>
       <c r="B155" t="s">
         <v>270</v>
@@ -4767,16 +4894,16 @@
         <v>284</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="5" t="s">
+    <row r="163" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A163" s="3" t="s">
         <v>285</v>
       </c>
       <c r="B163" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
+    <row r="164" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A164" s="7" t="s">
         <v>287</v>
       </c>
       <c r="B164" t="s">
@@ -4784,7 +4911,7 @@
       </c>
     </row>
     <row r="165" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A165" s="3" t="s">
+      <c r="A165" s="7" t="s">
         <v>289</v>
       </c>
       <c r="B165" t="s">
@@ -4807,16 +4934,16 @@
         <v>294</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A168" s="7" t="s">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>295</v>
       </c>
       <c r="B168" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A169" s="7" t="s">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>297</v>
       </c>
       <c r="B169" t="s">
@@ -4865,23 +4992,23 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>215</v>
+      </c>
+      <c r="B175" t="s">
         <v>309</v>
-      </c>
-      <c r="B175" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>310</v>
+      </c>
+      <c r="B176" t="s">
         <v>311</v>
-      </c>
-      <c r="B176" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>219</v>
+        <v>312</v>
       </c>
       <c r="B177" t="s">
         <v>313</v>
@@ -4924,54 +5051,54 @@
         <v>322</v>
       </c>
       <c r="B182" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B183" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B184" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B185" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
+        <v>326</v>
+      </c>
+      <c r="B186" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A187" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B187" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="B186" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+    </row>
+    <row r="188" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A188" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="B187" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>330</v>
-      </c>
-      <c r="B188" t="s">
+      <c r="B188" s="3" t="s">
         <v>330</v>
       </c>
     </row>
@@ -4983,19 +5110,19 @@
         <v>332</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A190" s="3" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>333</v>
       </c>
-      <c r="B190" s="3" t="s">
+      <c r="B190" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A191" s="3" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>335</v>
       </c>
-      <c r="B191" s="3" t="s">
+      <c r="B191" t="s">
         <v>336</v>
       </c>
     </row>
@@ -5044,28 +5171,28 @@
         <v>347</v>
       </c>
       <c r="B197" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B198" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B199" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B200" t="s">
         <v>352</v>
@@ -5140,20 +5267,20 @@
         <v>369</v>
       </c>
       <c r="B209" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
+        <v>370</v>
+      </c>
+      <c r="B210" t="s">
         <v>371</v>
-      </c>
-      <c r="B210" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B211" t="s">
         <v>373</v>
@@ -5204,134 +5331,146 @@
         <v>384</v>
       </c>
       <c r="B217" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B218" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B219" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
+        <v>387</v>
+      </c>
+      <c r="B220" t="s">
+        <v>388</v>
+      </c>
+      <c r="C220" t="s">
         <v>389</v>
       </c>
-      <c r="B220" t="s">
-        <v>389</v>
+      <c r="D220" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B221" t="s">
-        <v>390</v>
+        <v>392</v>
+      </c>
+      <c r="C221" t="s">
+        <v>393</v>
+      </c>
+      <c r="D221" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B222" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="C222" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D222" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B223" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C223" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D223" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B224" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C224" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D224" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B225" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C225" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D225" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B226" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C226" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D226" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
+        <v>409</v>
+      </c>
+      <c r="B227" t="s">
+        <v>409</v>
+      </c>
+      <c r="C227" t="s">
         <v>407</v>
       </c>
-      <c r="B227" t="s">
-        <v>408</v>
-      </c>
-      <c r="C227" t="s">
-        <v>393</v>
-      </c>
       <c r="D227" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B228" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C228" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D228" t="s">
         <v>412</v>
@@ -5345,7 +5484,7 @@
         <v>413</v>
       </c>
       <c r="C229" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D229" t="s">
         <v>414</v>
@@ -5359,7 +5498,7 @@
         <v>415</v>
       </c>
       <c r="C230" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D230" t="s">
         <v>416</v>
@@ -5373,147 +5512,147 @@
         <v>417</v>
       </c>
       <c r="C231" t="s">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="D231" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B232" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C232" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="D232" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B233" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C233" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D233" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B234" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C234" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D234" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B235" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C235" t="s">
-        <v>422</v>
+        <v>393</v>
       </c>
       <c r="D235" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B236" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C236" t="s">
-        <v>431</v>
+        <v>393</v>
       </c>
       <c r="D236" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B237" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C237" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D237" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B238" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C238" t="s">
-        <v>397</v>
+        <v>438</v>
       </c>
       <c r="D238" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B239" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C239" t="s">
-        <v>397</v>
+        <v>442</v>
       </c>
       <c r="D239" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B240" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C240" t="s">
-        <v>442</v>
+        <v>407</v>
       </c>
       <c r="D240" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="B241" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C241" t="s">
-        <v>446</v>
+        <v>389</v>
       </c>
       <c r="D241" t="s">
         <v>447</v>
@@ -5521,97 +5660,97 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B242" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C242" t="s">
-        <v>411</v>
+        <v>427</v>
       </c>
       <c r="D242" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B243" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C243" t="s">
-        <v>393</v>
+        <v>427</v>
       </c>
       <c r="D243" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B244" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C244" t="s">
-        <v>431</v>
+        <v>457</v>
       </c>
       <c r="D244" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B245" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="C245" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="D245" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="B246" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C246" t="s">
-        <v>461</v>
+        <v>389</v>
       </c>
       <c r="D246" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B247" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C247" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D247" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B248" t="s">
         <v>467</v>
       </c>
       <c r="C248" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D248" t="s">
         <v>468</v>
@@ -5625,7 +5764,7 @@
         <v>469</v>
       </c>
       <c r="C249" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D249" t="s">
         <v>470</v>
@@ -5639,7 +5778,7 @@
         <v>471</v>
       </c>
       <c r="C250" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D250" t="s">
         <v>472</v>
@@ -5653,7 +5792,7 @@
         <v>473</v>
       </c>
       <c r="C251" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D251" t="s">
         <v>474</v>
@@ -5667,7 +5806,7 @@
         <v>475</v>
       </c>
       <c r="C252" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D252" t="s">
         <v>476</v>
@@ -5678,13 +5817,13 @@
         <v>477</v>
       </c>
       <c r="B253" t="s">
+        <v>478</v>
+      </c>
+      <c r="C253" t="s">
+        <v>407</v>
+      </c>
+      <c r="D253" t="s">
         <v>477</v>
-      </c>
-      <c r="C253" t="s">
-        <v>393</v>
-      </c>
-      <c r="D253" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -5692,52 +5831,52 @@
         <v>479</v>
       </c>
       <c r="B254" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C254" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D254" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B255" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C255" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D255" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B256" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C256" t="s">
-        <v>393</v>
+        <v>438</v>
       </c>
       <c r="D256" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B257" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C257" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="D257" t="s">
         <v>488</v>
@@ -5745,41 +5884,41 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B258" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C258" t="s">
-        <v>442</v>
+        <v>389</v>
       </c>
       <c r="D258" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B259" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C259" t="s">
-        <v>425</v>
+        <v>389</v>
       </c>
       <c r="D259" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B260" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C260" t="s">
-        <v>393</v>
+        <v>427</v>
       </c>
       <c r="D260" t="s">
         <v>496</v>
@@ -5787,13 +5926,13 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B261" t="s">
         <v>498</v>
       </c>
       <c r="C261" t="s">
-        <v>393</v>
+        <v>442</v>
       </c>
       <c r="D261" t="s">
         <v>499</v>
@@ -5804,13 +5943,13 @@
         <v>500</v>
       </c>
       <c r="B262" t="s">
+        <v>500</v>
+      </c>
+      <c r="C262" t="s">
+        <v>427</v>
+      </c>
+      <c r="D262" t="s">
         <v>501</v>
-      </c>
-      <c r="C262" t="s">
-        <v>431</v>
-      </c>
-      <c r="D262" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
@@ -5818,13 +5957,13 @@
         <v>502</v>
       </c>
       <c r="B263" t="s">
+        <v>503</v>
+      </c>
+      <c r="C263" t="s">
+        <v>418</v>
+      </c>
+      <c r="D263" t="s">
         <v>502</v>
-      </c>
-      <c r="C263" t="s">
-        <v>446</v>
-      </c>
-      <c r="D263" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
@@ -5832,80 +5971,80 @@
         <v>504</v>
       </c>
       <c r="B264" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C264" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="D264" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B265" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C265" t="s">
-        <v>422</v>
+        <v>389</v>
       </c>
       <c r="D265" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B266" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C266" t="s">
-        <v>393</v>
+        <v>427</v>
       </c>
       <c r="D266" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B267" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="C267" t="s">
-        <v>393</v>
+        <v>442</v>
       </c>
       <c r="D267" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B268" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C268" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="D268" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B269" t="s">
         <v>518</v>
       </c>
       <c r="C269" t="s">
-        <v>446</v>
+        <v>407</v>
       </c>
       <c r="D269" t="s">
         <v>519</v>
@@ -5919,7 +6058,7 @@
         <v>520</v>
       </c>
       <c r="C270" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D270" t="s">
         <v>521</v>
@@ -5933,7 +6072,7 @@
         <v>522</v>
       </c>
       <c r="C271" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D271" t="s">
         <v>523</v>
@@ -5947,7 +6086,7 @@
         <v>524</v>
       </c>
       <c r="C272" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D272" t="s">
         <v>525</v>
@@ -5961,7 +6100,7 @@
         <v>526</v>
       </c>
       <c r="C273" t="s">
-        <v>393</v>
+        <v>427</v>
       </c>
       <c r="D273" t="s">
         <v>527</v>
@@ -5975,21 +6114,21 @@
         <v>528</v>
       </c>
       <c r="C274" t="s">
-        <v>393</v>
+        <v>427</v>
       </c>
       <c r="D274" t="s">
-        <v>529</v>
+        <v>474</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
+        <v>529</v>
+      </c>
+      <c r="B275" t="s">
+        <v>529</v>
+      </c>
+      <c r="C275" t="s">
         <v>530</v>
-      </c>
-      <c r="B275" t="s">
-        <v>530</v>
-      </c>
-      <c r="C275" t="s">
-        <v>431</v>
       </c>
       <c r="D275" t="s">
         <v>531</v>
@@ -6002,45 +6141,33 @@
       <c r="B276" t="s">
         <v>532</v>
       </c>
-      <c r="C276" t="s">
-        <v>431</v>
-      </c>
-      <c r="D276" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
+    </row>
+    <row r="277" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A277" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A278" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="B277" t="s">
-        <v>533</v>
-      </c>
-      <c r="C277" t="s">
+      <c r="B278" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="D277" t="s">
+    </row>
+    <row r="279" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A279" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
+      <c r="B279" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="B278" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="279" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A279" s="3" t="s">
-        <v>837</v>
-      </c>
-      <c r="B279" s="3" t="s">
-        <v>837</v>
-      </c>
     </row>
     <row r="280" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A280" s="3" t="s">
+      <c r="A280" t="s">
         <v>537</v>
       </c>
       <c r="B280" s="3" t="s">
@@ -6048,80 +6175,92 @@
       </c>
     </row>
     <row r="281" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A281" t="s">
+      <c r="A281" s="3" t="s">
         <v>539</v>
       </c>
       <c r="B281" s="3" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>541</v>
       </c>
-      <c r="B282" s="3" t="s">
+      <c r="B282" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="283" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A283" s="3" t="s">
+      <c r="C282" t="s">
+        <v>407</v>
+      </c>
+      <c r="D282" t="s">
         <v>543</v>
       </c>
-      <c r="B283" s="3" t="s">
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
         <v>544</v>
+      </c>
+      <c r="B283" t="s">
+        <v>545</v>
+      </c>
+      <c r="C283" t="s">
+        <v>389</v>
+      </c>
+      <c r="D283" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B284" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C284" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D284" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B285" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C285" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D285" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B286" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="C286" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="D286" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B287" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="C287" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D287" t="s">
         <v>556</v>
@@ -6129,125 +6268,125 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B288" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C288" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D288" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B289" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C289" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D289" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B290" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="C290" t="s">
-        <v>393</v>
+        <v>427</v>
       </c>
       <c r="D290" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B291" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="C291" t="s">
         <v>393</v>
       </c>
       <c r="D291" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B292" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C292" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="D292" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B293" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C293" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="D293" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="B294" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="C294" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D294" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B295" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C295" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D295" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B296" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="C296" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D296" t="s">
         <v>582</v>
@@ -6255,16 +6394,16 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B297" t="s">
+        <v>585</v>
+      </c>
+      <c r="C297" t="s">
+        <v>407</v>
+      </c>
+      <c r="D297" t="s">
         <v>584</v>
-      </c>
-      <c r="C297" t="s">
-        <v>393</v>
-      </c>
-      <c r="D297" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -6275,105 +6414,105 @@
         <v>587</v>
       </c>
       <c r="C298" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D298" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B299" t="s">
+        <v>590</v>
+      </c>
+      <c r="C299" t="s">
+        <v>407</v>
+      </c>
+      <c r="D299" t="s">
         <v>589</v>
-      </c>
-      <c r="C299" t="s">
-        <v>411</v>
-      </c>
-      <c r="D299" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B300" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C300" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D300" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B301" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C301" t="s">
-        <v>411</v>
+        <v>427</v>
       </c>
       <c r="D301" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="B302" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C302" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D302" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B303" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="C303" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D303" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B304" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="C304" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="D304" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="B305" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="C305" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="D305" t="s">
         <v>606</v>
@@ -6381,55 +6520,55 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B306" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C306" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D306" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B307" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C307" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D307" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B308" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="C308" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D308" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B309" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C309" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D309" t="s">
         <v>617</v>
@@ -6437,16 +6576,16 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B310" t="s">
+        <v>620</v>
+      </c>
+      <c r="C310" t="s">
+        <v>407</v>
+      </c>
+      <c r="D310" t="s">
         <v>619</v>
-      </c>
-      <c r="C310" t="s">
-        <v>393</v>
-      </c>
-      <c r="D310" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -6457,35 +6596,35 @@
         <v>622</v>
       </c>
       <c r="C311" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="D311" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B312" t="s">
+        <v>625</v>
+      </c>
+      <c r="C312" t="s">
+        <v>626</v>
+      </c>
+      <c r="D312" t="s">
         <v>624</v>
-      </c>
-      <c r="C312" t="s">
-        <v>411</v>
-      </c>
-      <c r="D312" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B313" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="C313" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D313" t="s">
         <v>627</v>
@@ -6493,16 +6632,16 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B314" t="s">
+        <v>630</v>
+      </c>
+      <c r="C314" t="s">
+        <v>389</v>
+      </c>
+      <c r="D314" t="s">
         <v>629</v>
-      </c>
-      <c r="C314" t="s">
-        <v>630</v>
-      </c>
-      <c r="D314" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
@@ -6513,32 +6652,32 @@
         <v>632</v>
       </c>
       <c r="C315" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D315" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B316" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C316" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D316" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="B317" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="C317" t="s">
         <v>393</v>
@@ -6549,55 +6688,55 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B318" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C318" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D318" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B319" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C319" t="s">
-        <v>397</v>
+        <v>427</v>
       </c>
       <c r="D319" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="B320" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="C320" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D320" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B321" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C321" t="s">
-        <v>431</v>
+        <v>393</v>
       </c>
       <c r="D321" t="s">
         <v>648</v>
@@ -6605,41 +6744,41 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B322" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C322" t="s">
-        <v>393</v>
+        <v>427</v>
       </c>
       <c r="D322" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B323" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C323" t="s">
-        <v>397</v>
+        <v>427</v>
       </c>
       <c r="D323" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B324" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C324" t="s">
-        <v>431</v>
+        <v>442</v>
       </c>
       <c r="D324" t="s">
         <v>656</v>
@@ -6647,16 +6786,16 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B325" t="s">
+        <v>659</v>
+      </c>
+      <c r="C325" t="s">
+        <v>626</v>
+      </c>
+      <c r="D325" t="s">
         <v>658</v>
-      </c>
-      <c r="C325" t="s">
-        <v>431</v>
-      </c>
-      <c r="D325" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -6667,63 +6806,63 @@
         <v>661</v>
       </c>
       <c r="C326" t="s">
-        <v>446</v>
+        <v>427</v>
       </c>
       <c r="D326" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B327" t="s">
+        <v>664</v>
+      </c>
+      <c r="C327" t="s">
+        <v>427</v>
+      </c>
+      <c r="D327" t="s">
         <v>663</v>
-      </c>
-      <c r="C327" t="s">
-        <v>630</v>
-      </c>
-      <c r="D327" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B328" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C328" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="D328" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B329" t="s">
         <v>668</v>
       </c>
       <c r="C329" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="D329" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B330" t="s">
         <v>670</v>
       </c>
       <c r="C330" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D330" t="s">
         <v>671</v>
@@ -6737,7 +6876,7 @@
         <v>672</v>
       </c>
       <c r="C331" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D331" t="s">
         <v>673</v>
@@ -6751,7 +6890,7 @@
         <v>674</v>
       </c>
       <c r="C332" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D332" t="s">
         <v>675</v>
@@ -6765,7 +6904,7 @@
         <v>676</v>
       </c>
       <c r="C333" t="s">
-        <v>393</v>
+        <v>442</v>
       </c>
       <c r="D333" t="s">
         <v>677</v>
@@ -6779,38 +6918,38 @@
         <v>678</v>
       </c>
       <c r="C334" t="s">
-        <v>393</v>
+        <v>679</v>
       </c>
       <c r="D334" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B335" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C335" t="s">
-        <v>446</v>
+        <v>530</v>
       </c>
       <c r="D335" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B336" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="C336" t="s">
+        <v>393</v>
+      </c>
+      <c r="D336" t="s">
         <v>683</v>
-      </c>
-      <c r="D336" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -6818,66 +6957,66 @@
         <v>685</v>
       </c>
       <c r="B337" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="C337" t="s">
-        <v>534</v>
+        <v>389</v>
       </c>
       <c r="D337" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B338" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C338" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D338" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B339" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="C339" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D339" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B340" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C340" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D340" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B341" t="s">
-        <v>696</v>
+        <v>315</v>
       </c>
       <c r="C341" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D341" t="s">
         <v>697</v>
@@ -6888,24 +7027,24 @@
         <v>698</v>
       </c>
       <c r="B342" t="s">
+        <v>698</v>
+      </c>
+      <c r="C342" t="s">
+        <v>407</v>
+      </c>
+      <c r="D342" t="s">
         <v>699</v>
-      </c>
-      <c r="C342" t="s">
-        <v>411</v>
-      </c>
-      <c r="D342" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B343" t="s">
-        <v>319</v>
+        <v>700</v>
       </c>
       <c r="C343" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D343" t="s">
         <v>701</v>
@@ -6919,7 +7058,7 @@
         <v>702</v>
       </c>
       <c r="C344" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D344" t="s">
         <v>703</v>
@@ -6933,38 +7072,38 @@
         <v>704</v>
       </c>
       <c r="C345" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D345" t="s">
-        <v>705</v>
+        <v>355</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
+        <v>705</v>
+      </c>
+      <c r="B346" t="s">
+        <v>705</v>
+      </c>
+      <c r="C346" t="s">
+        <v>393</v>
+      </c>
+      <c r="D346" t="s">
         <v>706</v>
-      </c>
-      <c r="B346" t="s">
-        <v>706</v>
-      </c>
-      <c r="C346" t="s">
-        <v>411</v>
-      </c>
-      <c r="D346" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
+        <v>707</v>
+      </c>
+      <c r="B347" t="s">
+        <v>707</v>
+      </c>
+      <c r="C347" t="s">
+        <v>427</v>
+      </c>
+      <c r="D347" t="s">
         <v>708</v>
-      </c>
-      <c r="B347" t="s">
-        <v>708</v>
-      </c>
-      <c r="C347" t="s">
-        <v>411</v>
-      </c>
-      <c r="D347" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
@@ -6975,7 +7114,7 @@
         <v>709</v>
       </c>
       <c r="C348" t="s">
-        <v>397</v>
+        <v>427</v>
       </c>
       <c r="D348" t="s">
         <v>710</v>
@@ -6989,24 +7128,18 @@
         <v>711</v>
       </c>
       <c r="C349" t="s">
-        <v>431</v>
+        <v>530</v>
       </c>
       <c r="D349" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
+    <row r="350" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A350" s="3" t="s">
         <v>713</v>
       </c>
-      <c r="B350" t="s">
+      <c r="B350" s="3" t="s">
         <v>713</v>
-      </c>
-      <c r="C350" t="s">
-        <v>431</v>
-      </c>
-      <c r="D350" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
@@ -7014,130 +7147,136 @@
         <v>715</v>
       </c>
       <c r="B351" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C351" t="s">
-        <v>534</v>
+        <v>407</v>
       </c>
       <c r="D351" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="352" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A352" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="B352" s="3" t="s">
-        <v>717</v>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>718</v>
+      </c>
+      <c r="B352" t="s">
+        <v>719</v>
+      </c>
+      <c r="C352" t="s">
+        <v>407</v>
+      </c>
+      <c r="D352" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B353" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C353" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D353" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B354" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C354" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D354" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B355" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C355" t="s">
-        <v>411</v>
+        <v>427</v>
       </c>
       <c r="D355" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="B356" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="C356" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D356" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B357" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="C357" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="D357" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B358" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="C358" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D358" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B359" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="C359" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D359" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B360" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="C360" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D360" t="s">
         <v>742</v>
@@ -7145,16 +7284,16 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B361" t="s">
+        <v>745</v>
+      </c>
+      <c r="C361" t="s">
+        <v>427</v>
+      </c>
+      <c r="D361" t="s">
         <v>744</v>
-      </c>
-      <c r="C361" t="s">
-        <v>393</v>
-      </c>
-      <c r="D361" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -7179,119 +7318,119 @@
         <v>749</v>
       </c>
       <c r="C363" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="D363" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B364" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C364" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D364" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="B365" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C365" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D365" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="B366" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C366" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D366" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="B367" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="C367" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D367" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B368" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="C368" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D368" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B369" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C369" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D369" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B370" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C370" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D370" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="B371" t="s">
         <v>771</v>
       </c>
       <c r="C371" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D371" t="s">
         <v>772</v>
@@ -7305,7 +7444,7 @@
         <v>773</v>
       </c>
       <c r="C372" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D372" t="s">
         <v>774</v>
@@ -7319,7 +7458,7 @@
         <v>775</v>
       </c>
       <c r="C373" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D373" t="s">
         <v>776</v>
@@ -7333,7 +7472,7 @@
         <v>777</v>
       </c>
       <c r="C374" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D374" t="s">
         <v>778</v>
@@ -7347,7 +7486,7 @@
         <v>779</v>
       </c>
       <c r="C375" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="D375" t="s">
         <v>780</v>
@@ -7361,7 +7500,7 @@
         <v>781</v>
       </c>
       <c r="C376" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D376" t="s">
         <v>782</v>
@@ -7375,7 +7514,7 @@
         <v>783</v>
       </c>
       <c r="C377" t="s">
-        <v>397</v>
+        <v>442</v>
       </c>
       <c r="D377" t="s">
         <v>784</v>
@@ -7386,80 +7525,80 @@
         <v>785</v>
       </c>
       <c r="B378" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C378" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D378" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B379" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="C379" t="s">
-        <v>446</v>
+        <v>389</v>
       </c>
       <c r="D379" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B380" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="C380" t="s">
         <v>393</v>
       </c>
       <c r="D380" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="B381" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="C381" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D381" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B382" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C382" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D382" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="B383" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="C383" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D383" t="s">
         <v>800</v>
@@ -7467,111 +7606,111 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B384" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C384" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D384" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B385" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="C385" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="D385" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="B386" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C386" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D386" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B387" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C387" t="s">
-        <v>397</v>
+        <v>427</v>
       </c>
       <c r="D387" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B388" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="C388" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D388" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="B389" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="C389" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="D389" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="B390" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="C390" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D390" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="B391" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C391" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D391" t="s">
         <v>823</v>
@@ -7579,72 +7718,60 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B392" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C392" t="s">
-        <v>411</v>
+        <v>427</v>
       </c>
       <c r="D392" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B393" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C393" t="s">
-        <v>393</v>
+        <v>442</v>
       </c>
       <c r="D393" t="s">
-        <v>827</v>
+        <v>830</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="B394" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C394" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="D394" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A395" t="s">
         <v>832</v>
       </c>
-      <c r="B395" t="s">
-        <v>833</v>
-      </c>
-      <c r="C395" t="s">
-        <v>446</v>
-      </c>
-      <c r="D395" t="s">
+    </row>
+    <row r="395" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A395" s="3" t="s">
         <v>834</v>
       </c>
-    </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A396" t="s">
+      <c r="B395" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="B396" t="s">
-        <v>835</v>
-      </c>
-      <c r="C396" t="s">
-        <v>411</v>
-      </c>
-      <c r="D396" t="s">
+    </row>
+    <row r="396" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A396" s="3" t="s">
         <v>836</v>
+      </c>
+      <c r="B396" s="3" t="s">
+        <v>837</v>
       </c>
     </row>
     <row r="397" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
@@ -7679,19 +7806,31 @@
         <v>845</v>
       </c>
     </row>
-    <row r="401" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A401" s="3" t="s">
+    <row r="401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
         <v>846</v>
       </c>
-      <c r="B401" s="3" t="s">
+      <c r="B401" t="s">
+        <v>846</v>
+      </c>
+      <c r="C401" t="s">
+        <v>407</v>
+      </c>
+      <c r="D401" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="402" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A402" s="3" t="s">
+    <row r="402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
         <v>848</v>
       </c>
-      <c r="B402" s="3" t="s">
+      <c r="B402" t="s">
+        <v>848</v>
+      </c>
+      <c r="C402" t="s">
+        <v>407</v>
+      </c>
+      <c r="D402" t="s">
         <v>849</v>
       </c>
     </row>
@@ -7700,38 +7839,38 @@
         <v>850</v>
       </c>
       <c r="B403" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C403" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D403" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B404" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C404" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D404" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="B405" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C405" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D405" t="s">
         <v>856</v>
@@ -7739,83 +7878,83 @@
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B406" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C406" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D406" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B407" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C407" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D407" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="B408" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="C408" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D408" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="B409" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="C409" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D409" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="B410" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="C410" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D410" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="B411" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="C411" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D411" t="s">
         <v>873</v>
@@ -7823,16 +7962,16 @@
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B412" t="s">
+        <v>876</v>
+      </c>
+      <c r="C412" t="s">
+        <v>389</v>
+      </c>
+      <c r="D412" t="s">
         <v>875</v>
-      </c>
-      <c r="C412" t="s">
-        <v>393</v>
-      </c>
-      <c r="D412" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
@@ -7843,163 +7982,157 @@
         <v>878</v>
       </c>
       <c r="C413" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D413" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B414" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C414" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D414" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B415" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C415" t="s">
-        <v>393</v>
+        <v>885</v>
       </c>
       <c r="D415" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c r="B416" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="C416" t="s">
-        <v>393</v>
+        <v>427</v>
       </c>
       <c r="D416" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="B417" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="C417" t="s">
-        <v>889</v>
+        <v>427</v>
       </c>
       <c r="D417" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="B418" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="C418" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="D418" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="B419" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="C419" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
       <c r="D419" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="B420" t="s">
+        <v>900</v>
+      </c>
+      <c r="C420" t="s">
+        <v>407</v>
+      </c>
+      <c r="D420" t="s">
         <v>898</v>
-      </c>
-      <c r="C420" t="s">
-        <v>411</v>
-      </c>
-      <c r="D420" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B421" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C421" t="s">
         <v>393</v>
       </c>
       <c r="D421" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B422" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C422" t="s">
-        <v>411</v>
+        <v>427</v>
       </c>
       <c r="D422" t="s">
-        <v>902</v>
+        <v>906</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="B423" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C423" t="s">
-        <v>397</v>
+        <v>427</v>
       </c>
       <c r="D423" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B424" t="s">
-        <v>909</v>
-      </c>
-      <c r="C424" t="s">
-        <v>431</v>
-      </c>
-      <c r="D424" t="s">
         <v>910</v>
       </c>
     </row>
@@ -8008,12 +8141,6 @@
         <v>911</v>
       </c>
       <c r="B425" t="s">
-        <v>911</v>
-      </c>
-      <c r="C425" t="s">
-        <v>431</v>
-      </c>
-      <c r="D425" t="s">
         <v>912</v>
       </c>
     </row>
@@ -8030,47 +8157,263 @@
         <v>915</v>
       </c>
       <c r="B427" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A428" s="3" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A428" t="s">
+      <c r="B428" s="3" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A429" s="3" t="s">
         <v>917</v>
       </c>
-      <c r="B428" t="s">
+      <c r="B429" s="3" t="s">
         <v>918</v>
-      </c>
-    </row>
-    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A429" t="s">
-        <v>919</v>
-      </c>
-      <c r="B429" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="430" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A430" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B430" s="3" t="s">
         <v>920</v>
       </c>
     </row>
-    <row r="431" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A431" s="3" t="s">
+    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>965</v>
+      </c>
+      <c r="B431" t="s">
         <v>921</v>
       </c>
-      <c r="B431" s="3" t="s">
+      <c r="C431" t="s">
+        <v>885</v>
+      </c>
+      <c r="D431" t="s">
         <v>922</v>
       </c>
     </row>
-    <row r="432" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A432" s="3" t="s">
+    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
         <v>923</v>
       </c>
-      <c r="B432" s="3" t="s">
+      <c r="B432" t="s">
         <v>924</v>
+      </c>
+      <c r="C432" t="s">
+        <v>427</v>
+      </c>
+      <c r="D432" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>925</v>
+      </c>
+      <c r="B433" t="s">
+        <v>926</v>
+      </c>
+      <c r="C433" t="s">
+        <v>407</v>
+      </c>
+      <c r="D433" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>927</v>
+      </c>
+      <c r="B434" t="s">
+        <v>928</v>
+      </c>
+      <c r="C434" t="s">
+        <v>929</v>
+      </c>
+      <c r="D434" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>931</v>
+      </c>
+      <c r="B435" t="s">
+        <v>932</v>
+      </c>
+      <c r="C435" t="s">
+        <v>407</v>
+      </c>
+      <c r="D435" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>934</v>
+      </c>
+      <c r="B436" t="s">
+        <v>935</v>
+      </c>
+      <c r="C436" t="s">
+        <v>407</v>
+      </c>
+      <c r="D436" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>937</v>
+      </c>
+      <c r="B437" t="s">
+        <v>938</v>
+      </c>
+      <c r="C437" t="s">
+        <v>407</v>
+      </c>
+      <c r="D437" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>940</v>
+      </c>
+      <c r="B438" t="s">
+        <v>941</v>
+      </c>
+      <c r="C438" t="s">
+        <v>389</v>
+      </c>
+      <c r="D438" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>942</v>
+      </c>
+      <c r="B439" t="s">
+        <v>943</v>
+      </c>
+      <c r="C439" t="s">
+        <v>389</v>
+      </c>
+      <c r="D439" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>945</v>
+      </c>
+      <c r="B440" t="s">
+        <v>946</v>
+      </c>
+      <c r="C440" t="s">
+        <v>407</v>
+      </c>
+      <c r="D440" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>947</v>
+      </c>
+      <c r="B441" t="s">
+        <v>948</v>
+      </c>
+      <c r="C441" t="s">
+        <v>949</v>
+      </c>
+      <c r="D441" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>950</v>
+      </c>
+      <c r="B442" t="s">
+        <v>951</v>
+      </c>
+      <c r="C442" t="s">
+        <v>389</v>
+      </c>
+      <c r="D442" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>952</v>
+      </c>
+      <c r="B443" t="s">
+        <v>953</v>
+      </c>
+      <c r="C443" t="s">
+        <v>427</v>
+      </c>
+      <c r="D443" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>955</v>
+      </c>
+      <c r="B444" t="s">
+        <v>956</v>
+      </c>
+      <c r="C444" t="s">
+        <v>389</v>
+      </c>
+      <c r="D444" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>958</v>
+      </c>
+      <c r="B445" t="s">
+        <v>959</v>
+      </c>
+      <c r="C445" t="s">
+        <v>389</v>
+      </c>
+      <c r="D445" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>961</v>
+      </c>
+      <c r="B446" t="s">
+        <v>962</v>
+      </c>
+      <c r="C446" t="s">
+        <v>963</v>
+      </c>
+      <c r="D446" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>966</v>
+      </c>
+      <c r="B447" t="s">
+        <v>967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update non_verbs.xlsx and verbs.xlsx with recent changes
</commit_message>
<xml_diff>
--- a/non_verbs.xlsx
+++ b/non_verbs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\local testing\online web app deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DF2458-C12F-4191-94E0-54D6E5411F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6552EE8E-1DA1-4E00-841B-36F97943980B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A357A7E5-BAA5-4C24-A2E6-28D531E07DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="993">
   <si>
     <t>Kanji</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3011,6 +3011,74 @@
   </si>
   <si>
     <t>ポスター</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>錠剤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>液剤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>散剤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>カプセル</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>習慣</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>じょうざい</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>えきざい</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>さんざい</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>しゅうかん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>従業</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>じゅうぎょう</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>貯金</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ちょきん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>しょうひん</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>大統領</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>だいとうりょう</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3420,10 +3488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C76790-D60C-4D2A-B9EE-DB30025A8785}">
-  <dimension ref="A1:F452"/>
+  <dimension ref="A1:F461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
-      <selection activeCell="A452" sqref="A452"/>
+    <sheetView tabSelected="1" topLeftCell="A442" workbookViewId="0">
+      <selection activeCell="B461" sqref="B461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8488,6 +8556,78 @@
         <v>975</v>
       </c>
     </row>
+    <row r="453" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A453" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="B453" s="3" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A454" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="B454" s="3" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A455" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="B455" s="3" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A456" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="B456" s="3" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A457" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="B457" s="3" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A458" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="B458" s="3" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A459" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="B459" s="3" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A460" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="B460" s="3" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="A461" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="B461" s="3" t="s">
+        <v>992</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>